<commit_message>
Update all files to distribute with two demo
</commit_message>
<xml_diff>
--- a/canada_articles.xlsx
+++ b/canada_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,3740 +453,3315 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLOG: Canada’s economic stagnation—a big problem for Canadians</t>
+          <t>Match day roster taking on Scotland in Ottawa named for Canada’s Men’s Rugby Team</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.552015</t>
+          <t>2024-07-03 15:27:02.930379</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZyYXNlcmluc3RpdHV0ZS5vcmcvYmxvZ3MvY2FuYWRhcy1lY29ub21pYy1zdGFnbmF0aW9uLWEtYmlnLXByb2JsZW0tZm9yLWNhbmFkaWFuc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L21hdGNoLWRheS1yb3N0ZXItdGFraW5nLW9uLXNjb3RsYW5kLWluLW90dGF3YS1uYW1lZC1mb3ItY2FuYWRhLXMtbWVuLXMtcnVnYnktdGVhbdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Canada Soccer and Canadian Olympic Committee unveil Women’s National Team roster for the Paris Olympic Games</t>
+          <t>Skate Canada Names 25 Athletes &amp; Three Synchronized Skating Teams to 2024-2025 National Team</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.552015</t>
+          <t>2024-07-03 15:27:02.930379</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiigFodHRwczovL2NhbmFkYXNvY2Nlci5jb20vbmV3cy9jYW5hZGEtc29jY2VyLWFuZC1jYW5hZGlhbi1vbHltcGljLWNvbW1pdHRlZS11bnZlaWwtd29tZW5zLW5hdGlvbmFsLXRlYW0tcm9zdGVyLWZvci10aGUtcGFyaXMtb2x5bXBpYy1nYW1lcy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vc2thdGVjYW5hZGEuY2EvMjAyNC8wNy9za2F0ZS1jYW5hZGEtbmFtZXMtMjUtYXRobGV0ZXMtdGhyZWUtc3luY2hyb25pemVkLXNrYXRpbmctdGVhbXMtdG8tMjAyNC0yMDI1LW5hdGlvbmFsLXRlYW0v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>People across Canada who responded to my message of joy</t>
+          <t>Canadian Dream? High housing costs has two-in-five recent immigrants saying they may leave their province (or Canada)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.552015</t>
+          <t>2024-07-03 15:27:02.945959</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiqQFodHRwczovL3d3dy50aGVzdGFyLmNvbS9vcGluaW9uL2NvbnRyaWJ1dG9ycy9pdmUtbWV0LXBlb3BsZS1hY3Jvc3MtY2FuYWRhLXdoby1yZXNwb25kZWQtdG8tbXktbWVzc2FnZS1vZi1qb3ktYnV0LXdlLWNhbi9hcnRpY2xlX2RiMmRhZDNhLTM2ODMtMTFlZi05ZTIyLTFiMTEwNTQ0NDQ1YS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vYW5ndXNyZWlkLm9yZy9jYW5hZGEtaW50ZXJwcm92aW5jaWFsLW1pZ3JhdGlvbi1ob3VzaW5nLWNyaXNpcy1pbW1pZ3JhdGlvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Canada Day in Ottawa: Everything you need to know about the 2024 celebrations</t>
+          <t>Measuring Progressivity in Canada’s Tax System, 2024</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.552015</t>
+          <t>2024-07-03 15:27:02.945959</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vb3R0YXdhY2l0aXplbi5jb20vbmV3cy9sb2NhbC1uZXdzL2NhbmFkYS1kYXktaW4tb3R0YXdhLTIwMjQtZmFx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmZyYXNlcmluc3RpdHV0ZS5vcmcvc3R1ZGllcy9tZWFzdXJpbmctcHJvZ3Jlc3Npdml0eS1pbi1jYW5hZGFzLXRheC1zeXN0ZW0tMjAyNNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>In his own words: Prime Minister Justin Trudeau's message on Canada Day</t>
+          <t>IGNITE the Lights Across Canada</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.562260</t>
+          <t>2024-07-03 15:27:02.945959</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvaW4taGlzLW93bi13b3Jkcy1wcmltZS1taW5pc3Rlci1qdXN0aW4tdHJ1ZGVhdS1zLW1lc3NhZ2Utb24tY2FuYWRhLWRheS0xLjY5NDczMzTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiI2h0dHBzOi8vcGFyYWx5bXBpYy5jYS9pZ25pdGVjYW5hZGEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>‘Canada’ Day reflections: Our complicity in genocide</t>
+          <t>Vestas secures 347 MW EnVentus order in Canada</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.565381</t>
+          <t>2024-07-03 15:27:02.945959</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vcmFiYmxlLmNhL2NvbHVtbmlzdHMvY2FuYWRhLWRheS1yZWZsZWN0aW9ucy1vdXItY29tcGxpY2l0eS1pbi1nZW5vY2lkZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnZlc3Rhcy5jb20vZW4vbWVkaWEvY29tcGFueS1uZXdzLzIwMjQvdmVzdGFzLXNlY3VyZXMtMzQ3LW13LWVudmVudHVzLW9yZGVyLWluLWNhbmFkYS1jNDAxMDY4MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Canada Day festivities attract hundreds at ceremonies, parties across the country</t>
+          <t>Canada officially joins Horizon Europe</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.565381</t>
+          <t>2024-07-03 15:27:02.945959</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1kYXktZmVzdGl2aXRpZXMtYXR0cmFjdC1odW5kcmVkcy1hdC1jZXJlbW9uaWVzLXBhcnRpZXMtYWNyb3NzLXRoZS1jb3VudHJ5LTEuNjk0NzQyONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vc2NpZW5jZWJ1c2luZXNzLm5ldC9uZXdzL2hvcml6b24tZXVyb3BlL2NhbmFkYS1vZmZpY2lhbGx5LWpvaW5zLWhvcml6b24tZXVyb3Bl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>If you qualify for this tax credit, you can expect a payment in your bank account this week</t>
+          <t>CDS Message: Appointment of the new Chief of the Defence Staff</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-07-01 13:14:39.572000</t>
+          <t>2024-07-03 15:27:02.945959</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiggFodHRwczovL3d3dy5jdHZuZXdzLmNhL2NhbmFkYS9pZi15b3UtcXVhbGlmeS1mb3ItdGhpcy10YXgtY3JlZGl0LXlvdS1jYW4tZXhwZWN0LWEtcGF5bWVudC1pbi15b3VyLWJhbmstYWNjb3VudC10aGlzLXdlZWstMS42OTQ3NDU40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikgFodHRwczovL3d3dy5jYW5hZGEuY2EvZW4vZGVwYXJ0bWVudC1uYXRpb25hbC1kZWZlbmNlL21hcGxlLWxlYWYvZGVmZW5jZS8yMDI0LzA3L2Nkcy1tZXNzYWdlLWFwcG9pbnRtZW50LW9mLXRoZS1uZXctY2hpZWYtb2YtdGhlLWRlZmVuY2Utc3RhZmYuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLOG: Canada's economic stagnation—a big problem for Canadians</t>
+          <t>Breaking standout Phil Wizard set to rep Team Canada at Paris 2024</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.394367</t>
+          <t>2024-07-03 15:27:02.977255</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZyYXNlcmluc3RpdHV0ZS5vcmcvYmxvZ3MvY2FuYWRhcy1lY29ub21pYy1zdGFnbmF0aW9uLWEtYmlnLXByb2JsZW0tZm9yLWNhbmFkaWFuc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzAzL3RlYW0tY2FuYWRhLWFubm91Y21lbnQtcGhpbC13aXphcmQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Statement by Minister Miller on Canada Day</t>
+          <t>Joint statement by Prime Minister Trudeau and President von der Leyen on the association of Canada to Horizon Europe</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.394367</t>
+          <t>2024-07-03 15:27:02.984815</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9pbW1pZ3JhdGlvbi1yZWZ1Z2Vlcy1jaXRpemVuc2hpcC9uZXdzLzIwMjQvMDYvc3RhdGVtZW50LWJ5LW1pbmlzdGVyLW1pbGxlci1vbi1jYW5hZGEtZGF5Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3Mvc3RhdGVtZW50cy8yMDI0LzA3LzAzL2pvaW50LXN0YXRlbWVudC1wcmltZS1taW5pc3Rlci10cnVkZWF1LWFuZC1wcmVzaWRlbnQtdm9uLWRlci1sZXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Statement by the Prime Minister on Canada Day</t>
+          <t>Cost of living has immigrants considering leaving Canada: poll</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.394367</t>
+          <t>2024-07-03 15:27:02.984815</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3Mvc3RhdGVtZW50cy8yMDI0LzA3LzAxL3N0YXRlbWVudC1wcmltZS1taW5pc3Rlci1jYW5hZGEtZGF50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDMvY29zdC1vZi1saXZpbmctY2FuYWRpYW4taW1taWdyYW50cy1sZWF2aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Canada Soccer and Canadian Olympic Committee unveil Women's National Team roster for the Paris Olympic Games</t>
+          <t>Lt.-Gen. Jennie Carignan will be Canada’s 1st female defence chief</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.404287</t>
+          <t>2024-07-03 15:27:02.984815</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiigFodHRwczovL2NhbmFkYXNvY2Nlci5jb20vbmV3cy9jYW5hZGEtc29jY2VyLWFuZC1jYW5hZGlhbi1vbHltcGljLWNvbW1pdHRlZS11bnZlaWwtd29tZW5zLW5hdGlvbmFsLXRlYW0tcm9zdGVyLWZvci10aGUtcGFyaXMtb2x5bXBpYy1nYW1lcy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjAxNjUyL2plbm5pZS1jYXJpZ25hbi1uZXctY2hpZWYtb2YtZGVmZW5jZS1jYW5hZGEv0gFUaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDE2NTIvamVubmllLWNhcmlnbmFuLW5ldy1jaGllZi1vZi1kZWZlbmNlLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Trudeau hails Canadian values as celebrations kick off marking Canada Day</t>
+          <t>Lt.-Gen. Jennie Carignan named Canada's newest chief of the defence staff</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.404287</t>
+          <t>2024-07-03 15:27:02.984815</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiOGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9jYW5hZGEtZGF5LTIwMjQtMS43MjUwODMw0gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTA4MzA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2plbm5pZS1jYXJpZ25hbi1uYW1lZC1jaGllZi1vZi10aGUtZGVmZW5jZS1zdGFmZi0xLjcyNTMyNTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1MzI1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>I've met people across Canada who responded to my message of joy. But we can all do more to build bridges in these ...</t>
+          <t>Here's how many medals Canada might win at the Olympics</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.404287</t>
+          <t>2024-07-03 15:27:02.984815</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiqQFodHRwczovL3d3dy50aGVzdGFyLmNvbS9vcGluaW9uL2NvbnRyaWJ1dG9ycy9pdmUtbWV0LXBlb3BsZS1hY3Jvc3MtY2FuYWRhLXdoby1yZXNwb25kZWQtdG8tbXktbWVzc2FnZS1vZi1qb3ktYnV0LXdlLWNhbi9hcnRpY2xlX2RiMmRhZDNhLTM2ODMtMTFlZi05ZTIyLTFiMTEwNTQ0NDQ1YS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvdGhlLWJ1enplci1uZXdzbGV0dGVyLWNhbmFkYS1tZWRhbC1wcmVkaWN0aW9uLW9seW1waWNzLTEuNzI1MzU2MdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzNTYx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Is Canada broken? Not to the diverse crowd at Canada Place's big celebration</t>
+          <t>“We don’t want it to catch on like wildfire,” says Health Canada on clinics charging patients</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.404287</t>
+          <t>2024-07-03 15:27:02.993374</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vdmFuY291dmVyc3VuLmNvbS9uZXdzL2xvY2FsLW5ld3MvY2FuYWRhLWRheS1jZWxlYnJhdGlvbnMtZGl2ZXJzZS1jcm93ZC12YW5jb3V2ZXItY2FuYWRhLXBsYWNlLWJyb2tlbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LmhlYWx0aGNvYWxpdGlvbi5jYS93ZS1kb250LXdhbnQtaXQtdG8tY2F0Y2gtb24tbGlrZS13aWxkZmlyZS1zYXlzLWhlYWx0aC1jYW5hZGEtb24tY2xpbmljcy1jaGFyZ2luZy1wYXRpZW50cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Premier Ford Shares Canada Day Greetings</t>
+          <t>Nearly 40% of new Canadians say they're considering leaving their province — or Canada — over high housing costs</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.404287</t>
+          <t>2024-07-03 15:27:02.993374</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vbmV3cy5vbnRhcmlvLmNhL2VuL3N0YXRlbWVudC8xMDA0Nzg2L3ByZW1pZXItZm9yZC1zaGFyZXMtY2FuYWRhLWRheS1ncmVldGluZ3PSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy50aGVzdGFyLmNvbS9uZXdzL2NhbmFkYS9uZWFybHktNDAtb2YtbmV3LWNhbmFkaWFucy1zYXktdGhleXJlLWNvbnNpZGVyaW5nLWxlYXZpbmctdGhlaXItcHJvdmluY2Utb3ItY2FuYWRhLW92ZXItaGlnaC9hcnRpY2xlXzAwMjZmNTQ2LTM5MzctMTFlZi05N2I5LWE3Mzk3ZTA1OGYxYS5odG1s0gG2AWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL25ld3MvY2FuYWRhL25lYXJseS00MC1vZi1uZXctY2FuYWRpYW5zLXNheS10aGV5cmUtY29uc2lkZXJpbmctbGVhdmluZy10aGVpci1wcm92aW5jZS1vci1jYW5hZGEtb3Zlci1oaWdoL2FydGljbGVfMDAyNmY1NDYtMzkzNy0xMWVmLTk3YjktYTczOTdlMDU4ZjFhLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Canada Day in Ottawa 2024: Where to go, what to see?</t>
+          <t>Proof point: Rental housing construction picks up in Canada but will it be enough?</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.404287</t>
+          <t>2024-07-03 15:27:03.009077</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vb3R0YXdhY2l0aXplbi5jb20vbmV3cy9sb2NhbC1uZXdzL2NhbmFkYS1kYXktaW4tb3R0YXdhLTIwMjQtZmFx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3Rob3VnaHRsZWFkZXJzaGlwLnJiYy5jb20vcHJvb2YtcG9pbnQtcmVudGFsLWhvdXNpbmctY29uc3RydWN0aW9uLWlzLWZpbmFsbHktcGlja2luZy11cC1pbi1jYW5hZGEtYnV0LXdpbGwtaXQtYmUtZW5vdWdoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Islanders can expect road closures due to Canada Day celebrations</t>
+          <t>MP Housefather denounces antisemitic poster telling him to 'get out of Canada'</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.414181</t>
+          <t>2024-07-03 15:27:03.009077</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9wcmluY2UtZWR3YXJkLWlzbGFuZC9wZWktY2FuYWRhLWRheS0yMDI0LXJvYWQtY2xvc3VyZXMtMS43MjUwMDg50gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTAwODk?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2hvdXNlZmF0aGVyLW1wLWFudGlzZW10aWMtcG9zdGVyLTEuNzI1MzAwNtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzMDA2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>56 new Canadian citizens honoured at Heritage Park on Canada Day</t>
+          <t>First-ever breaking athlete named to Canadian Olympic Team</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.419254</t>
+          <t>2024-07-03 15:27:03.009077</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vY2FsZ2FyeWhlcmFsZC5jb20vbmV3cy9sb2NhbC1uZXdzLzU2LW5ldy1jYW5hZGlhbi1jaXRpemVucy1ob25vdXJlZC1hdC1oZXJpdGFnZS1wYXJrLW9uLWNhbmFkYS1kYXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy9maXJzdC1ldmVyLWJyZWFraW5nLWF0aGxldGUtbmFtZWQtdG8tY2FuYWRpYW4tb2x5bXBpYy10ZWFtL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Citizenship ceremony, other Canada Day festivities go ahead despite rainy Winnipeg skies</t>
+          <t>Prince Albert National Park</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.419254</t>
+          <t>2024-07-04 15:27:02.930379</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9tYW5pdG9iYS9jYW5hZGEtZGF5LXdpbm5pcGVnLTIwMjQtMS43MjUxNTk10gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTE1OTU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLWh0dHBzOi8vcGFya3MuY2FuYWRhLmNhL3BuLW5wL3NrL3ByaW5jZWFsYmVydNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16 interesting facts about Canada to celebrate Canada Day</t>
+          <t>Workers at Canada Border Services Agency ratify tentative agreement for more than 9,000 workers</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.424007</t>
+          <t>2024-07-04 15:27:02.945959</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmNpY25ld3MuY29tLzIwMjQvMDcvMTYtaW50ZXJlc3RpbmctZmFjdHMtYWJvdXQtY2FuYWRhLXRvLWNlbGVicmF0ZS1jYW5hZGEtZGF5LTA3NDUwNzguaHRtbNIBamh0dHBzOi8vd3d3LmNpY25ld3MuY29tLzIwMjQvMDcvMTYtaW50ZXJlc3RpbmctZmFjdHMtYWJvdXQtY2FuYWRhLXRvLWNlbGVicmF0ZS1jYW5hZGEtZGF5LTA3NDUwNzguaHRtbC9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcHNhY3VuaW9uLmNhL3dvcmtlcnMtY2FuYWRhLWJvcmRlci1zZXJ2aWNlcy1hZ2VuY3ktcmF0aWZ50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Justin Trudeau's 2024 Canada Day message</t>
+          <t>Alice Munro Was Bigger than Canada</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.428066</t>
+          <t>2024-07-04 15:27:02.945959</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0MzY5ODLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiOGh0dHBzOi8vdGhld2FscnVzLmNhL2FsaWNlLW11bnJvLXdhcy1iaWdnZXItdGhhbi1jYW5hZGEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Canada Day: Celebrations held nationwide, Trudeau hails ‘inclusive’ values</t>
+          <t>Canada’s digital services tax is here. How could it affect you?</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.428066</t>
+          <t>2024-07-04 15:27:02.945959</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNTk3OTk4L2NhbmFkYS1kYXktY2VsZWJyYXRpb25zLXBsYW5uZWQtbmF0aW9ud2lkZS10cnVkZWF1LWhhaWxzLWluY2x1c2l2ZS12YWx1ZXMv0gFyaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA1OTc5OTgvY2FuYWRhLWRheS1jZWxlYnJhdGlvbnMtcGxhbm5lZC1uYXRpb253aWRlLXRydWRlYXUtaGFpbHMtaW5jbHVzaXZlLXZhbHVlcy9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiOWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L9IBPWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Canada Day 2024: Justin Trudeau's message</t>
+          <t>Canada to deport one of Iran's Larijani brothers after granting him PR status</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.428066</t>
+          <t>2024-07-04 15:27:02.977255</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvaW4taGlzLW93bi13b3Jkcy1wcmltZS1taW5pc3Rlci1qdXN0aW4tdHJ1ZGVhdS1zLW1lc3NhZ2Utb24tY2FuYWRhLWRheS0xLjY5NDczMzTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiKGh0dHBzOi8vd3d3LmlyYW5pbnRsLmNvbS9lbi8yMDI0MDcwNDcyMjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Maple leaf rising: Windsor celebrates Canada Day with downtown parade</t>
+          <t>Canada to host the 70th annual NATO session in Montreal</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.428066</t>
+          <t>2024-07-04 15:27:02.977255</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd2luZHNvcnN0YXIuY29tL25ld3MvbG9jYWwtbmV3cy93aW5kc29yLWNlbGVicmF0ZXMtY2FuYWRhLWRheS13aXRoLWFubnVhbC1wYXJhZGXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY2FuYWRhLXRvLWhvc3QtdGhlLTcwdGgtYW5udWFsLW5hdG8tc2Vzc2lvbi1pbi1tb250cmVhbC0xLjY5NTIxMDXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Canada's women's soccer team stacked with Olympic champions as Paris roster revealed</t>
+          <t>U of T community members recognized with Order of Canada</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.438876</t>
+          <t>2024-07-04 15:27:02.977255</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL29seW1waWNzLWNhbmFkYS13b21lbi1zb2NjZXItYW5ub3VuY2VtZW50LWp1bHkxLTEuNzI1MTQwOdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUxNDA5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LnV0b3JvbnRvLmNhL25ld3MvdS10LWNvbW11bml0eS1tZW1iZXJzLXJlY29nbml6ZWQtb3JkZXItY2FuYWRhLTHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Skyhawks team member seriously injured in Canada Day performance on Parliament Hill</t>
+          <t>Why Canada must act urgently to give undocumented migrants legal status</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.444729</t>
+          <t>2024-07-04 15:27:02.984815</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy5jYmMuY2EvbmV3cy9jYW5hZGEvb3R0YXdhL3NreWhhd2tzLXRlYW0tbWVtYmVyLXNlcmlvdXNseS1pbmp1cmVkLWluLWNhbmFkYS1kYXktcGVyZm9ybWFuY2Utb24tcGFybGlhbWVudC1oaWxsLTEuNzI1MTc4NdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUxNzg1?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vdGhlY29udmVyc2F0aW9uLmNvbS93aHktY2FuYWRhLW11c3QtYWN0LXVyZ2VudGx5LXRvLWdpdmUtdW5kb2N1bWVudGVkLW1pZ3JhbnRzLWxlZ2FsLXN0YXR1cy0yMzI2ODbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>I'm fluent in English, but my accent still feels like a barrier to acceptance</t>
+          <t>Permanent Residence in Canada is not guaranteed for international students</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.446344</t>
+          <t>2024-07-04 15:27:02.984815</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9zYXNrYXRjaGV3YW4vZW5nbGlzaC1hY2NlbnQtc3BlYWtpbmctMS43MjM3NjQ40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyMzc2NDg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmNpY25ld3MuY29tLzIwMjQvMDcvcGVybWFuZW50LXJlc2lkZW5jZS1pbi1jYW5hZGEtaXMtbm90LWd1YXJhbnRlZWQtZm9yLWludGVybmF0aW9uYWwtc3R1ZGVudHMtMDc0NDg1Ni5odG1s0gF7aHR0cHM6Ly93d3cuY2ljbmV3cy5jb20vMjAyNC8wNy9wZXJtYW5lbnQtcmVzaWRlbmNlLWluLWNhbmFkYS1pcy1ub3QtZ3VhcmFudGVlZC1mb3ItaW50ZXJuYXRpb25hbC1zdHVkZW50cy0wNzQ0ODU2Lmh0bWwvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Canada to face unbeaten Venezuela in Copa America quarterfinal</t>
+          <t>Team Canada’s women’s water polo team seeks to make a splash at Paris 2024</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.454036</t>
+          <t>2024-07-04 15:27:02.993374</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NvcGEtYW1lcmljYS1yZWNhcC1qdW5lLTMwLTEuNzI1MTA4OdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUxMDg5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA0L3RlYW0tY2FuYWRhcy13b21lbnMtd2F0ZXItcG9sby10ZWFtLXNlZWtzLXRvLW1ha2UtYS1zcGxhc2gtYXQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Canada Day celebrations today in Maple Ridge and Pitt Meadows</t>
+          <t>Creating Online harms regulators expected to cost Canada $200 million: PBO</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.459094</t>
+          <t>2024-07-04 15:27:02.993374</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3Lm1hcGxlcmlkZ2VuZXdzLmNvbS9sb2NhbC1lbnRlcnRhaW5tZW50L2NhbmFkYS1kYXktY2VsZWJyYXRpb25zLXRvZGF5LWluLW1hcGxlLXJpZGdlLWFuZC1waXR0LW1lYWRvd3MtNzQxNjU3M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY3JlYXRpbmctb25saW5lLWhhcm1zLXJlZ3VsYXRvcnMtZXhwZWN0ZWQtdG8tY29zdC1jYW5hZGEtMjAwLW1pbGxpb24tcGJvLTEuNjk1MTIyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Canada Day celebrations marked across the country</t>
+          <t>Canada’s digital services tax enters into force</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.459094</t>
+          <t>2024-07-04 15:27:02.993374</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1kYXktZmVzdGl2aXRpZXMtYXR0cmFjdC1odW5kcmVkcy1hdC1jZXJlbW9uaWVzLXBhcnRpZXMtYWNyb3NzLXRoZS1jb3VudHJ5LTEuNjk0NzQyONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vd3d3Lm9zbGVyLmNvbS9lbi9pbnNpZ2h0cy91cGRhdGVzL2NhbmFkYXMtZGlnaXRhbC1zZXJ2aWNlcy10YXgtZW50ZXJzLWludG8tZm9yY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Canada's GST tax credit coming July 5</t>
+          <t>Liberal government enacts controversial digital services tax, raising trade concerns</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.463994</t>
+          <t>2024-07-04 15:27:02.993374</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiggFodHRwczovL3d3dy5jdHZuZXdzLmNhL2NhbmFkYS9pZi15b3UtcXVhbGlmeS1mb3ItdGhpcy10YXgtY3JlZGl0LXlvdS1jYW4tZXhwZWN0LWEtcGF5bWVudC1pbi15b3VyLWJhbmstYWNjb3VudC10aGlzLXdlZWstMS42OTQ3NDU40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2RpZ2l0YWwtc2VydmljZXMtdGF4LWltcGxlbWVudGVkLTEuNzI1NDM1NtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU0MzU2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>'Canada' Day reflections: Our complicity in genocide</t>
+          <t>Canada's world junior team coming to Windsor for four days this month</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.463994</t>
+          <t>2024-07-04 15:27:02.993374</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vcmFiYmxlLmNhL2NvbHVtbmlzdHMvY2FuYWRhLWRheS1yZWZsZWN0aW9ucy1vdXItY29tcGxpY2l0eS1pbi1nZW5vY2lkZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd2luZHNvcnN0YXIuY29tL3Nwb3J0cy9jYW5hZGFzLXdvcmxkLWp1bmlvci10ZWFtLWNvbWluZy10by13aW5kc29yLWZvci1mb3VyLWRheXMtdGhpcy1tb250aNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Driver dead after two-vehicle Canada Day crash in Brampton</t>
+          <t>Pro-Palestine protesters make pitch at disrupting Team Israel at Canada Cup women's softball tournament</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-07-01 13:18:31.469050</t>
+          <t>2024-07-04 15:27:02.993374</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNTk4MDc3L2JyYW1wdG9uLWNhbmFkYS1kYXktZmF0YWwtY3Jhc2gv0gFIaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA1OTgwNzcvYnJhbXB0b24tY2FuYWRhLWRheS1mYXRhbC1jcmFzaC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibWh0dHBzOi8vdGhlcHJvdmluY2UuY29tL3Nwb3J0cy9wcm8tcGFsZXN0aW5lLXByb3Rlc3RlcnMtZGlzcnVwdC10ZWFtLWlzcmFlbC1hdC1jYW5hZGEtY3VwLXNvZnRiYWxsLXRvdXJuYW1lbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Team Canada announces women’s basketball roster heading to Paris 2024</t>
+          <t>Head of Canada's spy agency announces he's stepping down from the job</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-07-02 13:14:39.552015</t>
+          <t>2024-07-04 15:27:03.009077</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzAyL3RlYW0tY2FuYWRhLWFubm91bmNlcy13b21lbnMtYmFza2V0YmFsbC1yb3N0ZXItaGVhZGluZy10by1wYXJpcy0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2RhdmlkLXZpZ25lYXVsdC1zdGVwcGluZy1kb3duLWNzaXMtZGlyZWN0b3ItMS43MjU0OTA50gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTQ5MDk?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Team Canada’s Paris 2024 athletics team unveiled</t>
+          <t>Nutrition labelling: List of ingredients</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-07-02 13:14:39.552015</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vYXRobGV0aWNzLmNhL2Jsb2cvMjAyNC8wNy8wMi90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1hdGhsZXRpY3MtdGVhbS11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9oZWFsdGgtY2FuYWRhL3NlcnZpY2VzL2Zvb2QtbnV0cml0aW9uL251dHJpdGlvbi1sYWJlbGxpbmcvaW5ncmVkaWVudC1saXN0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Harjit Sajjan failed Canada, and Canadians</t>
+          <t>Dressage and eventing athletes and horses named to Team Canada for Paris 2024</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-07-02 13:14:39.562260</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vb3Bpbmlvbi9lZGl0b3JpYWxzL2FydGljbGUtaGFyaml0LXNhamphbi1mYWlsZWQtY2FuYWRhLWFuZC1jYW5hZGlhbnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA1L2RyZXNzYWdlLWFuZC1ldmVudGluZy1hdGhsZXRlcy1hbmQtaG9yc2VzLW5hbWVkLXRvLXRlYW0tY2FuYWRhLWZvci1wYXJpcy0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Canada Day fireworks and drone display – y’eh or n’eh?</t>
+          <t>Air Canada has new policy on sacred items in the cabin after incident with national chief's headdress</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-07-02 13:14:39.565381</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmJ1cmxpbmd0b24uY2EvZW4vbmV3cy9jYW5hZGEtZGF5LWZpcmV3b3Jrcy1hbmQtZHJvbmUtZGlzcGxheS15LWVoLW9yLW4tZWguYXNweNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2luZGlnZW5vdXMvYWlyLWNhbmFkYS1uZXctcG9saWN5LXNhY3JlZC1pdGVtcy0xLjcyNTYwNzHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjA3MQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Team Canada's Paris 2024 athletics team unveiled</t>
+          <t>Team Canada’s Athletics Squad Grows Ahead of Paris 2024</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.404287</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vYXRobGV0aWNzLmNhL2Jsb2cvMjAyNC8wNy8wMi90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1hdGhsZXRpY3MtdGVhbS11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vYXRobGV0aWNzLmNhL2Jsb2cvMjAyNC8wNy8wNS90ZWFtLWNhbmFkYXMtYXRobGV0aWNzLXNxdWFkLWdyb3dzLWFoZWFkLW9mLXBhcmlzLTIwMjQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Canada announces women's basketball roster heading to Paris</t>
+          <t>Canada semi-final bound after heart-stopping penalty shootout win over Venezuela in Copa América QF</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.414181</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzAyL3RlYW0tY2FuYWRhLWFubm91bmNlcy13b21lbnMtYmFza2V0YmFsbC1yb3N0ZXItaGVhZGluZy10by1wYXJpcy0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtYm91bmQtZm9yLXNlbWktZmluYWxzLWFmdGVyLXRocmlsbGluZy1wZW5hbHR5LXNob290b3V0LXdpbi1vdmVyLXZlbmV6dWVsYS1pbi1jb3BhLWFtZXJpY2EtcWbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Embassy takes down AI-generated Canada Day social media post</t>
+          <t>Canada beats Venezuela in penalty kicks, reaches semis in 1st Copa America</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.414181</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL3dhc2hpbmd0b24tc29jaWFsLW1lZGlhLXBvc3QtYWktZ2VuZXJhdGVkLTEuNzI1MjA0ONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS12ZW5lenVlbGEtY29wYS1hbWVyaWNhLXJlY2FwLWp1bHktNS0xLjcyNTYyNTjSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjI1OA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>United States looking at all options to respond to Canada's digital services tax</t>
+          <t>Team Canada’s Paris 2024 equestrian dressage and eventing teams unveiled</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.414181</t>
+          <t>2024-07-05 15:27:02.930379</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiU2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL3VzLWxvb2tpbmctdG8tcmVzcG9uZC1jYW5hZGEtZGlnaXRhbC10YXgtMS43MjUyMTg10gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTIxODU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1lcXVlc3RyaWFuLWRyZXNzYWdlLWFuZC1ldmVudGluZy10ZWFtcy11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>A big Team Canada athletics team seeks a big medal haul at Paris 2024</t>
+          <t>Canadian unemployment rate rose to 6.4% in June as jobs market stalls</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.423819</t>
+          <t>2024-07-05 15:27:02.945959</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzAyL2EtYmlnLXRlYW0tY2FuYWRhLWF0aGxldGljcy10ZWFtLXNlZWtzLWEtYmlnLW1lZGFsLWhhdWwtYXQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRpYW4tdW5lbXBsb3ltZW50LXJhdGUtcm9zZS10by02LTQtaW4tanVuZS1hcy1qb2JzLW1hcmtldC1zdGFsbHMtMS42OTUyNDkx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Globe editorial: Harjit Sajjan failed Canada, and Canadians</t>
+          <t>Canada beat Venezuela on penalties to reach Copa America semifinals</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.428066</t>
+          <t>2024-07-05 15:27:02.945959</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vb3Bpbmlvbi9lZGl0b3JpYWxzL2FydGljbGUtaGFyaml0LXNhamphbi1mYWlsZWQtY2FuYWRhLWFuZC1jYW5hZGlhbnMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL2NhbmFkYS1iZWF0LXZlbmV6dWVsYS1vbi1wZW5hbHRpZXMtdG8tcmVhY2gtY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMtMS42OTUzMTk10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Canada winger Tajon Buchanan to undergo surgery after breaking tibia in training</t>
+          <t>A new U.K. government renews hopes for a free trade deal with Canada</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.428066</t>
+          <t>2024-07-05 15:27:02.945959</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL3Rham9uLWJ1Y2hhbmFuLWxvd2VyLWxlZy1pbmp1cnktY2FuYWRhLWNvcGEtYW1lcmljYS0xLjcyNTIxNTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1MjE1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2xhYm91ci11ay1lbGVjdGlvbi1mcmVlLXRyYWRlLWNhbmFkYS0xLjcyNTU3NzPSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTc3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Prime Minister to travel to Washington, D.C., for NATO Summit</t>
+          <t>Canada Soccer delivers new level of competition with PDP Championship</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.434310</t>
+          <t>2024-07-05 15:27:02.945959</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3MvbmV3cy1yZWxlYXNlcy8yMDI0LzA3LzAyL3ByaW1lLW1pbmlzdGVyLXRyYXZlbC13YXNoaW5ndG9uLWRjLW5hdG8tc3VtbWl00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItZGVsaXZlcnMtbmV3LWxldmVsLW9mLWNvbXBldGl0aW9uLXdpdGgtcGRwLWNoYW1waW9uc2hpcC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5 more alleged senior members of Iranian regime face deportation from Canada</t>
+          <t>Canada leads Venezuela after first half of Copa America quarters showdown</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.434310</t>
+          <t>2024-07-05 15:27:02.977255</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNTk3MDkxL2ZpdmUtaXJhbi1yZWdpbWUtbWVtYmVycy1kZXBvcnRlZC1mcm9tLWNhbmFkYS_SAVZodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDU5NzA5MS9maXZlLWlyYW4tcmVnaW1lLW1lbWJlcnMtZGVwb3J0ZWQtZnJvbS1jYW5hZGEvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY2FuYWRhLWxlYWRzLXZlbmV6dWVsYS1hZnRlci1maXJzdC1oYWxmLW9mLWNvcGEtYW1lcmljYS1xdWFydGVyLWZpbmFsLXNob3dkb3duLTEuMjE0NTA2ONIBc2h0dHBzOi8vd3d3LnRzbi5jYS9jYW5hZGEtbGVhZHMtdmVuZXp1ZWxhLWFmdGVyLWZpcnN0LWhhbGYtb2YtY29wYS1hbWVyaWNhLXF1YXJ0ZXItZmluYWwtc2hvd2Rvd24tMS4yMTQ1MDY4P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Drones take over Sudbury, Ont. skies on Canada Day</t>
+          <t>Is Canada still on fire in 2024?</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.438876</t>
+          <t>2024-07-05 15:27:02.977255</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0Mzc4MTnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiO2h0dHBzOi8vZWNvanVzdGljZS5jYS9uZXdzL2lzLWNhbmFkYS1zdGlsbC1vbi1maXJlLWluLTIwMjQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Man dead after falling from equipment during Canada Day parade in northern Alberta: RCMP</t>
+          <t>Motivated Canada ready to face Venezuela in Copa America quarter-final on TSN</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.446344</t>
+          <t>2024-07-05 15:27:02.984815</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNTk5MzMxL2NhbmFkYS1kYXktcGFyYWRlLWRlYXRoLW5vcnRoZXJuLWFsYmVydGEv0gFRaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA1OTkzMzEvY2FuYWRhLWRheS1wYXJhZGUtZGVhdGgtbm9ydGhlcm4tYWxiZXJ0YS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvbW90aXZhdGVkLWNhbmFkYS1yZWFkeS10by1mYWNlLXZlbmV6dWVsYS1pbi1jb3BhLWFtZXJpY2EtcXVhcnRlci1maW5hbC1vbi10c24tMS4yMTQ0Njc20gFyaHR0cHM6Ly93d3cudHNuLmNhL21vdGl2YXRlZC1jYW5hZGEtcmVhZHktdG8tZmFjZS12ZW5lenVlbGEtaW4tY29wYS1hbWVyaWNhLXF1YXJ0ZXItZmluYWwtb24tdHNuLTEuMjE0NDY3Nj90c24tYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Man throwing candy in northern Alberta Canada Day parade dies after fall</t>
+          <t>Canada edges Venezuela in shootout thriller; advances to Copa America semis</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.454036</t>
+          <t>2024-07-05 15:27:02.984815</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vZWRtb250b25qb3VybmFsLmNvbS9uZXdzL2xvY2FsLW5ld3MvbWFuLWRlYWQtY2FuYWRhLWRheS1wYXJhZGUtZmFsbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY2FuYWRhLWRlZmVhdHMtdmVuZXp1ZWxhLWluLXBlbmFsdGllcy10by1hZHZhbmNlLWF0LWNvcGEtYW1lcmljYS0xLjIxNDUwOTHSAWVodHRwczovL3d3dy50c24uY2EvY2FuYWRhLWRlZmVhdHMtdmVuZXp1ZWxhLWluLXBlbmFsdGllcy10by1hZHZhbmNlLWF0LWNvcGEtYW1lcmljYS0xLjIxNDUwOTE_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Canada Day fireworks and drone display – y'eh or n'eh?</t>
+          <t>What will the Canada-U.K. relationship look like under a Labour government?</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.459094</t>
+          <t>2024-07-05 15:27:02.993374</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmJ1cmxpbmd0b24uY2EvZW4vbmV3cy9jYW5hZGEtZGF5LWZpcmV3b3Jrcy1hbmQtZHJvbmUtZGlzcGxheS15LWVoLW9yLW4tZWguYXNweNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiPmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjAyNjAwL3VrLWVsZWN0aW9uLWxhYm91ci1jYW5hZGEv0gFCaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDI2MDAvdWstZWxlY3Rpb24tbGFib3VyLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Monday Digest: Canadians Arrive In Form at Wimbledon</t>
+          <t>'Canada's standing in the world has slipped' under Trudeau, Marc Garneau says in autobiography</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.462767</t>
+          <t>2024-07-05 15:27:02.993374</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LnRlbm5pc2NhbmFkYS5jb20vbmV3cy9tb25kYXktZGlnZXN0LWNhbmFkaWFucy1hcnJpdmUtaW4tZm9ybS1hdC13aW1ibGVkb24v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL21hcmMtZ2FybmVhdS10cnVkZWF1LWNhbmFkYS1yZXB1dGF0aW9uLXN1ZmZlcmluZy0xLjcyNTUxMjDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTEyMA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Watch Edmonton's Canada Day fireworks</t>
+          <t>Ontario judge authorizes sales process for The Body Shop Canada</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.463994</t>
+          <t>2024-07-05 15:27:02.993374</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0MzcyOTPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3LmNwMjQuY29tL25ld3Mvb250YXJpby1qdWRnZS1hdXRob3JpemVzLXNhbGVzLXByb2Nlc3MtZm9yLXRoZS1ib2R5LXNob3AtY2FuYWRhLTEuNjk1MzAyNdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Giant of geriatric medicine Dr. Kenneth Rockwood named to Order of Canada</t>
+          <t>Canadian unemployment rate rises to 6.4%, with student summer jobs especially hard to come by</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2024-07-02 13:18:31.463994</t>
+          <t>2024-07-05 15:27:02.993374</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LmRhbC5jYS9uZXdzLzIwMjQvMDcvMDMvY2xpbmljYWwtZnJhaWx0eS1zY2FsZS1rZW5uZXRoLXJvY2t3b29kLW9yZGVyLW9mLWNhbmFkYS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2J1c2luZXNzL2p1bmUtbGFib3VyLWZvcmNlLXN1cnZleS0xLjcyNTUxNDDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTE0MA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Match day roster taking on Scotland in Ottawa named for Canada’s Men’s Rugby Team</t>
+          <t>Canada's unemployment rate rises to 6.4% as job market stalls</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>2024-07-03 13:14:39.552015</t>
+          <t>2024-07-05 15:27:02.993374</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L21hdGNoLWRheS1yb3N0ZXItdGFraW5nLW9uLXNjb3RsYW5kLWluLW90dGF3YS1uYW1lZC1mb3ItY2FuYWRhLXMtbWVuLXMtcnVnYnktdGVhbdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9jYW5hZGEtdW5lbXBsb3ltZW50LXJhdGUtcmlzZXMtYXMtam9iLW1hcmtldC1zdGFsbHPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Canadian Dream? High housing costs has two-in-five recent immigrants saying they may leave their province (or Canada)</t>
+          <t>Unemployment rose to 6.4% in June: Statistics Canada</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2024-07-03 13:14:39.552015</t>
+          <t>2024-07-05 15:27:02.993374</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vYW5ndXNyZWlkLm9yZy9jYW5hZGEtaW50ZXJwcm92aW5jaWFsLW1pZ3JhdGlvbi1ob3VzaW5nLWNyaXNpcy1pbW1pZ3JhdGlvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmJubmJsb29tYmVyZy5jYS9zdGF0aXN0aWNzLWNhbmFkYS10by1yZWxlYXNlLWpvYnMtcmVwb3J0LWZvci1qdW5lLXRvZGF5LTEuMjA5MzI5OdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>“We don’t want it to catch on like wildfire,” says Health Canada on clinics charging patients</t>
+          <t>Zero-emission public transit for York Region</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>2024-07-03 13:14:39.565381</t>
+          <t>2024-07-05 15:27:03.009077</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LmhlYWx0aGNvYWxpdGlvbi5jYS93ZS1kb250LXdhbnQtaXQtdG8tY2F0Y2gtb24tbGlrZS13aWxkZmlyZS1zYXlzLWhlYWx0aC1jYW5hZGEtb24tY2xpbmljcy1jaGFyZ2luZy1wYXRpZW50cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3MvbmV3cy1yZWxlYXNlcy8yMDI0LzA3LzA1L3plcm8tZW1pc3Npb24tcHVibGljLXRyYW5zaXQteW9yay1yZWdpb27SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Breaking standout Phil Wizard set to rep Team Canada at Paris 2024</t>
+          <t>‘We just did that’: Canada celebrates after advancing to Copa America semifinals</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>2024-07-03 13:14:39.565381</t>
+          <t>2024-07-05 15:27:03.009077</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzAzL3RlYW0tY2FuYWRhLWFubm91Y21lbnQtcGhpbC13aXphcmQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS90aGlzLXRlYW0taXMtc3BlY2lhbC1jYW5hZGEtY2VsZWJyYXRlcy1hZnRlci1hZHZhbmNpbmctdG8tY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMv0gF5aHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL3NvY2Nlci90aGlzLXRlYW0taXMtc3BlY2lhbC1jYW5hZGEtY2VsZWJyYXRlcy1hZnRlci1hZHZhbmNpbmctdG8tY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMvc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Joint statement by Prime Minister Trudeau and President von der Leyen on the association of Canada to Horizon Europe</t>
+          <t>Trae Bell-Haynes released from Canadian Olympic men's basketball training camp</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>2024-07-03 13:14:39.565381</t>
+          <t>2024-07-06 15:27:02.930379</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3Mvc3RhdGVtZW50cy8yMDI0LzA3LzAzL2pvaW50LXN0YXRlbWVudC1wcmltZS1taW5pc3Rlci10cnVkZWF1LWFuZC1wcmVzaWRlbnQtdm9uLWRlci1sZXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvb2x5bXBpY3Mvc3VtbWVyL2Jhc2tldGJhbGwvdHJhZS1iZWlsbC1jYW5hZGEtb2x5bXBpYy1iYXNrZXRiYWxsLWNhbXAtMS43MjU2NDU30gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTY0NTc?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Canada issues travel warning as Hurricane Beryl tears through southeast Caribbean</t>
+          <t>Scotland wins Douglas Horn Trophy in Canada’s Men’s Rugby Team’s return to home soil</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>2024-07-03 13:14:39.572000</t>
+          <t>2024-07-06 15:27:02.930379</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1pc3N1ZXMtdHJhdmVsLXdhcm5pbmctYXMtaHVycmljYW5lLWJlcnlsLXRlYXJzLXRocm91Z2gtc291dGhlYXN0LWNhcmliYmVhbi0xLjY5NDk1NTLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L3Njb3RsYW5kLXdpbnMtZG91Z2xhcy1ob3JuLXRyb3BoeS1pbi1jYW5hZGEtcy1tZW4tcy1ydWdieS10ZWFtLXMtcmV0dXJuLXRvLWhvbWUtc29pbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Match day roster taking on Scotland in Ottawa named for Canada's Men's Rugby Team</t>
+          <t>In Canada for 7 years, family fights deportation to Nigeria</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.404287</t>
+          <t>2024-07-06 15:27:02.945959</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L21hdGNoLWRheS1yb3N0ZXItdGFraW5nLW9uLXNjb3RsYW5kLWluLW90dGF3YS1uYW1lZC1mb3ItY2FuYWRhLXMtbWVuLXMtcnVnYnktdGVhbdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvZmFtaWx5LWZpZ2h0cy1kZXBvcnRhdGlvbi1uaWdlcmlhLTEuNzI1NTUzMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU1NTMy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Skate Canada Names 25 Athletes &amp; Three Synchronized Skating Teams to 2024-2025 National Team</t>
+          <t>Young Scottish side shows its class in rugby win over Canadian men</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.412096</t>
+          <t>2024-07-06 15:27:02.945959</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vc2thdGVjYW5hZGEuY2EvMjAyNC8wNy9za2F0ZS1jYW5hZGEtbmFtZXMtMjUtYXRobGV0ZXMtdGhyZWUtc3luY2hyb25pemVkLXNrYXRpbmctdGVhbXMtdG8tMjAyNC0yMDI1LW5hdGlvbmFsLXRlYW0v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvcnVnYnkvc2NvdGxhbmQtY2FuYWRhLXJ1Z2J5LTEuNzI1NjUxMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU2NTEx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Prime Minister announces the upcoming appointment of the new Chief of the Defence Staff</t>
+          <t>Copa America Takeaways: Canada continues sensational run in its debut</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.414181</t>
+          <t>2024-07-06 15:27:02.945959</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3MvbmV3cy1yZWxlYXNlcy8yMDI0LzA3LzAzL3ByaW1lLW1pbmlzdGVyLWFubm91bmNlcy11cGNvbWluZy1hcHBvaW50bWVudC1uZXctY2hpZWYtZGVmZW5jZS1zdGFmZtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1jb250aW51ZXMtc2Vuc2F0aW9uYWwtcnVuLWluLWRlYnV0L9IBaGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtY29udGludWVzLXNlbnNhdGlvbmFsLXJ1bi1pbi1kZWJ1dC9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Canadian Dream? High housing costs has two-in-five recent immigrants saying they may leave their province (or ...</t>
+          <t>Canada captures four medals at World Cup Super Final in Hungary</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.419254</t>
+          <t>2024-07-06 15:27:02.945959</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vYW5ndXNyZWlkLm9yZy9jYW5hZGEtaW50ZXJwcm92aW5jaWFsLW1pZ3JhdGlvbi1ob3VzaW5nLWNyaXNpcy1pbW1pZ3JhdGlvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA2L3RlYW0tY2FuYWRhLXdvcmxkLWN1cC1zdXBlcmZpbmFsLXBhcmlzLTIwMi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Canada officially joins Horizon Europe</t>
+          <t>Canada’s 1st female defence chief, a U.K. vote and top stories this week</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.428066</t>
+          <t>2024-07-06 15:27:02.993374</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vc2NpZW5jZWJ1c2luZXNzLm5ldC9uZXdzL2hvcml6b24tZXVyb3BlL2NhbmFkYS1vZmZpY2lhbGx5LWpvaW5zLWhvcml6b24tZXVyb3Bl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA2OTE3L2NhbmFkYXMtMXN0LWZlbWFsZS1kZWZlbmNlLXRvcC1zdG9yaWVzLXRoaXMtd2Vlay_SAVlodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYwNjkxNy9jYW5hZGFzLTFzdC1mZW1hbGUtZGVmZW5jZS10b3Atc3Rvcmllcy10aGlzLXdlZWsvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CDS Message: Appointment of the new Chief of the Defence Staff</t>
+          <t>Trudeau should expect criticism at NATO summit over defence spending: analysis</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.434310</t>
+          <t>2024-07-06 15:27:03.009077</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikgFodHRwczovL3d3dy5jYW5hZGEuY2EvZW4vZGVwYXJ0bWVudC1uYXRpb25hbC1kZWZlbmNlL21hcGxlLWxlYWYvZGVmZW5jZS8yMDI0LzA3L2Nkcy1tZXNzYWdlLWFwcG9pbnRtZW50LW9mLXRoZS1uZXctY2hpZWYtb2YtdGhlLWRlZmVuY2Utc3RhZmYuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigwFodHRwczovL290dGF3YWNpdGl6ZW4uY29tL25ld3MvbmF0aW9uYWwvZGVmZW5jZS13YXRjaC90cnVkZWF1LXNob3VsZC1leHBlY3QtY3JpdGljaXNtLWF0LW5hdG8tc3VtbWl0LW92ZXItZGVmZW5jZS1zcGVuZGluZy1hbmFseXNpc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Cost of living has immigrants considering leaving Canada: poll</t>
+          <t>Canada projected roster for 2025 NHL 4 Nations Face-Off</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.438876</t>
+          <t>2024-07-07 15:27:24.449599</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDMvY29zdC1vZi1saXZpbmctY2FuYWRpYW4taW1taWdyYW50cy1sZWF2aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3d3Lm5obC5jb20vbmV3cy80LW5hdGlvbnMtZmFjZS1vZmYtcHJvamVjdGVkLXJvc3Rlci1jYW5hZGHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Lt.-Gen. Jennie Carignan will be Canada’s 1st female defence chief</t>
+          <t>Extreme heat grips much of Western Canada</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.443936</t>
+          <t>2024-07-07 15:27:24.461367</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjAxNjUyL2plbm5pZS1jYXJpZ25hbi1uZXctY2hpZWYtb2YtZGVmZW5jZS1jYW5hZGEv0gFUaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDE2NTIvamVubmllLWNhcmlnbmFuLW5ldy1jaGllZi1vZi1kZWZlbmNlLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9iYy1oZWF0LWRvbWUtMS43MjU2NTk30gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTY1OTc?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Phil Wizard set to rep Team Canada in breaking at Paris 2024</t>
+          <t>U of T ranks 17th globally, first in Canada in U.S. News &amp; World Report university rankings</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.444729</t>
+          <t>2024-07-08 15:27:24.426857</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzAzL3RlYW0tY2FuYWRhLWFubm91Y21lbnQtcGhpbC13aXphcmQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LnV0b3JvbnRvLmNhL25ld3MvdS10LXJhbmtzLTE3dGgtZ2xvYmFsbHktZmlyc3QtY2FuYWRhLXVzLW5ld3Mtd29ybGQtcmVwb3J0LXVuaXZlcnNpdHktcmFua2luZ3PSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Here's how many medals Canada might win at the Olympics</t>
+          <t>Inventories rebuilding fast in Canada’s largest housing markets</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.445837</t>
+          <t>2024-07-08 15:27:24.426857</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvdGhlLWJ1enplci1uZXdzbGV0dGVyLWNhbmFkYS1tZWRhbC1wcmVkaWN0aW9uLW9seW1waWNzLTEuNzI1MzU2MdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzNTYx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vdGhvdWdodGxlYWRlcnNoaXAucmJjLmNvbS9pbnZlbnRvcmllcy1yZWJ1aWxkaW5nLWZhc3QtaW4tY2FuYWRhcy1sYXJnZXN0LWhvdXNpbmctbWFya2V0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Lt.-Gen. Jennie Carignan named Canada's newest chief of the defence staff</t>
+          <t>Heat wave across Western Canada forecast to last through midweek</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.446344</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2plbm5pZS1jYXJpZ25hbi1uYW1lZC1jaGllZi1vZi10aGUtZGVmZW5jZS1zdGFmZi0xLjcyNTMyNTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1MzI1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2Vudmlyb25tZW50LWNhbmFkYS1oZWF0LXdhdmUtMS43MjU2OTYw0gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTY5NjA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Joint statement by Prime Minister Trudeau and President von der Leyen on the association of Canada to Horizon ...</t>
+          <t>Canada can’t catch a break from the heat. Will it last all summer?</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.446344</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3Mvc3RhdGVtZW50cy8yMDI0LzA3LzAzL2pvaW50LXN0YXRlbWVudC1wcmltZS1taW5pc3Rlci10cnVkZWF1LWFuZC1wcmVzaWRlbnQtdm9uLWRlci1sZXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwNjI3L2hlYXQtd2F2ZS1jYW5hZGEtaG90dGVzdC1qdW5lL9IBRmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwNjI3L2hlYXQtd2F2ZS1jYW5hZGEtaG90dGVzdC1qdW5lL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Ukrainian best friends separated by war reunite over Canada Day long weekend</t>
+          <t>Team Canada men’s volleyball team ready to smash it in Paris</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.454036</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9zYXNrYXRjaGV3YW4vdWtyYWluaWFuLWJlc3QtZnJpZW5kcy1zZXBhcmF0ZWQtd2FyLXJldW5pdGUtY2FuYWRhLWRheS1sb25nLXdlZWtlbmQtMS43MjUyMzgw0gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTIzODA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA4L3RlYW0tY2FuYWRhLW1lbnMtdm9sbGV5YmFsbC10ZWFtLXJlYWR5LXRvLXNtYXNoLWl0LWluLXBhcmlzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Nearly 40% of new Canadians say they're considering leaving their province — or Canada — over high housing costs</t>
+          <t>5 things to know as Canada meets Argentina in 'David vs. Goliath' Copa semifinal</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.454036</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy50aGVzdGFyLmNvbS9uZXdzL2NhbmFkYS9uZWFybHktNDAtb2YtbmV3LWNhbmFkaWFucy1zYXktdGhleXJlLWNvbnNpZGVyaW5nLWxlYXZpbmctdGhlaXItcHJvdmluY2Utb3ItY2FuYWRhLW92ZXItaGlnaC9hcnRpY2xlXzAwMjZmNTQ2LTM5MzctMTFlZi05N2I5LWE3Mzk3ZTA1OGYxYS5odG1s0gG2AWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL25ld3MvY2FuYWRhL25lYXJseS00MC1vZi1uZXctY2FuYWRpYW5zLXNheS10aGV5cmUtY29uc2lkZXJpbmctbGVhdmluZy10aGVpci1wcm92aW5jZS1vci1jYW5hZGEtb3Zlci1oaWdoL2FydGljbGVfMDAyNmY1NDYtMzkzNy0xMWVmLTk3YjktYTczOTdlMDU4ZjFhLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzLzUtdGhpbmdzLXRvLWtub3ctYXMtY2FuYWRhLW1lZXRzLWFyZ2VudGluYS1pbi1kYXZpZC12cy1nb2xpYXRoLWNvcGEtc2VtaWZpbmFsLTEuNjk1NTY4NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>“We don't want it to catch on like wildfire,” says Health Canada on clinics charging patients</t>
+          <t>Liberal government hopes changes to dental care program will increase uptake</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.459094</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LmhlYWx0aGNvYWxpdGlvbi5jYS93ZS1kb250LXdhbnQtaXQtdG8tY2F0Y2gtb24tbGlrZS13aWxkZmlyZS1zYXlzLWhlYWx0aC1jYW5hZGEtb24tY2xpbmljcy1jaGFyZ2luZy1wYXRpZW50cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvbGliZXJhbC1nb3Zlcm5tZW50LWhvcGVzLWNoYW5nZXMtdG8tZGVudGFsLWNhcmUtcHJvZ3JhbS13aWxsLWluY3JlYXNlLXVwdGFrZS0xLjY5NTU0NznSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MP Housefather denounces antisemitic poster telling him to 'get out of Canada'</t>
+          <t>Team Canada’s Paris 2024 men’s volleyball team unveiled</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.463994</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2hvdXNlZmF0aGVyLW1wLWFudGlzZW10aWMtcG9zdGVyLTEuNzI1MzAwNtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzMDA2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1tZW5zLXZvbGxleWJhbGwtdGVhbS11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Hurricane Beryl tracker: Canada issues warning</t>
+          <t>PREVIEW: Canada look to continue dream run at Copa América in semifinal rematch with Argentina</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.469050</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1pc3N1ZXMtdHJhdmVsLXdhcm5pbmctYXMtaHVycmljYW5lLWJlcnlsLXRlYXJzLXRocm91Z2gtc291dGhlYXN0LWNhcmliYmVhbi0xLjY5NDk1NTLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijAFodHRwczovL2NhbnBsLmNhL2FydGljbGUvcHJldmlldy1jYW5hZGEtbG9va2luZy10by1jb250aW51ZS1kcmVhbS1ydW4tYXQtMjAyNC1jb3BhLWFtZXJpY2EtaW4tc2VtaWZpbmFsLXJlbWF0Y2gtd2l0aC1saW9uZWwtbWVzc2lzLWFyZ2VudGluYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Proof point: Rental housing construction picks up in Canada but will it be enough?</t>
+          <t>Silk, Great Value plant-based beverages recalled across Canada</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2024-07-03 13:18:31.469050</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3Rob3VnaHRsZWFkZXJzaGlwLnJiYy5jb20vcHJvb2YtcG9pbnQtcmVudGFsLWhvdXNpbmctY29uc3RydWN0aW9uLWlzLWZpbmFsbHktcGlja2luZy11cC1pbi1jYW5hZGEtYnV0LXdpbGwtaXQtYmUtZW5vdWdoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtYmV2ZXJhZ2UtcmVjYWxsLTEuNzI1NzgyMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3ODIx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Canada's world junior team coming to Windsor for four days this month</t>
+          <t>Messi fit for Argentina's Copa America semifinal showdown with Canada</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2024-07-04 13:14:39.552015</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd2luZHNvcnN0YXIuY29tL3Nwb3J0cy9jYW5hZGFzLXdvcmxkLWp1bmlvci10ZWFtLWNvbWluZy10by13aW5kc29yLWZvci1mb3VyLWRheXMtdGhpcy1tb250aNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2xpb25lbC1tZXNzaS1maXQtYXJnZW50aW5hLWNhbmFkYS1jb3BhLWFtZXJpY2EtanVseS04LTEuNzI1Nzc0MtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3NzQy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Workers at Canada Border Services Agency ratify tentative agreement for more than 9,000 workers</t>
+          <t>Canada’s longest river seeing historically low levels</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2024-07-04 13:14:39.552015</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcHNhY3VuaW9uLmNhL3dvcmtlcnMtY2FuYWRhLWJvcmRlci1zZXJ2aWNlcy1hZ2VuY3ktcmF0aWZ50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwMzc0L21hY2tlbnppZS1yaXZlci1jYW5hZGEtbG93LWxldmVscy1oaXN0b3J5L9IBUmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwMzc0L21hY2tlbnppZS1yaXZlci1jYW5hZGEtbG93LWxldmVscy1oaXN0b3J5L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Team Canada’s women’s water polo team seeks to make a splash at Paris 2024</t>
+          <t>Opinion: Once the envy of the world, Canada’s immigration system now lies dismantled</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-07-04 13:14:39.565381</t>
+          <t>2024-07-08 15:27:24.460215</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA0L3RlYW0tY2FuYWRhcy13b21lbnMtd2F0ZXItcG9sby10ZWFtLXNlZWtzLXRvLW1ha2UtYS1zcGxhc2gtYXQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vYnVzaW5lc3MvY29tbWVudGFyeS9hcnRpY2xlLW9uY2UtdGhlLWVudnktb2YtdGhlLXdvcmxkLWNhbmFkYXMtaW1taWdyYXRpb24tc3lzdGVtLW5vdy1sYXlzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Pro-Palestine protesters make pitch at disrupting Team Israel at Canada Cup women's softball tournament</t>
+          <t>Letters July 8: Canada is best country on Earth; lack of courteous driving; desperate housing strategy</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2024-07-04 13:14:39.565381</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibWh0dHBzOi8vdGhlcHJvdmluY2UuY29tL3Nwb3J0cy9wcm8tcGFsZXN0aW5lLXByb3Rlc3RlcnMtZGlzcnVwdC10ZWFtLWlzcmFlbC1hdC1jYW5hZGEtY3VwLXNvZnRiYWxsLXRvdXJuYW1lbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy50aW1lc2NvbG9uaXN0LmNvbS9vcGluaW9uL2xldHRlcnMtanVseS04LWNhbmFkYS1pcy1iZXN0LWNvdW50cnktb24tZWFydGgtbGFjay1vZi1jb3VydGVvdXMtZHJpdmluZy1kZXNwZXJhdGUtaG91c2luZy1zdHJhdGVneS05MTg4MDQ00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Creating Online harms regulators expected to cost Canada $200 million: PBO</t>
+          <t>Marsch says he 'feels home' with Canada after being overlooked by U.S. Soccer Federation</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2024-07-04 13:14:39.565381</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY3JlYXRpbmctb25saW5lLWhhcm1zLXJlZ3VsYXRvcnMtZXhwZWN0ZWQtdG8tY29zdC1jYW5hZGEtMjAwLW1pbGxpb24tcGJvLTEuNjk1MTIyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS1jb3BhLWFtZXJpY2EtamVzc2UtbWFyc2NoLWp1bHktOC0xLjcyNTc4NjbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1Nzg2Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Alice Munro Was Bigger than Canada</t>
+          <t>B.C. municipalities struggle with what to do with RV dwellers</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.419254</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiOGh0dHBzOi8vdGhld2FscnVzLmNhL2FsaWNlLW11bnJvLXdhcy1iaWdnZXItdGhhbi1jYW5hZGEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2xvbmctdGVybS1ydi1mdXR1cmUtMS43MjU2MTQ00gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTYxNDQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Workers at Canada Border Services Agency ratify tentative agreement for more than 9000 workers</t>
+          <t>Canada Averts New Threat of Strikes at British Columbia Ports</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.419254</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcHNhY3VuaW9uLmNhL3dvcmtlcnMtY2FuYWRhLWJvcmRlci1zZXJ2aWNlcy1hZ2VuY3ktcmF0aWZ50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lndzai5jb20vYXJ0aWNsZXMvY2FuYWRhLWF2ZXJ0cy1uZXctdGhyZWF0LW9mLXN0cmlrZXMtYXQtYnJpdGlzaC1jb2x1bWJpYS1wb3J0cy00NGI4MTJmZtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Many Canadians in their 20s and 30s are delaying having kids — and some say high rent is a factor</t>
+          <t>Canada-Argentina headlines Copa, Euro semifinal action starting Tuesday on TSN</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.424007</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9yZW50LWNhbmFkYS1kZWxheWluZy1raWRzLTEuNzI1MjkyNtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUyOTI2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy50c24uY2Evc29jY2VyL2NhbmFkYS1hcmdlbnRpbmEtaGVhZGxpbmVzLWNvcGEtYW1lcmljYS11ZWZhLWV1cm8tMjAyNC1zZW1pZmluYWwtYWN0aW9uLXN0YXJ0aW5nLXR1ZXNkYXktb24tdHNuLTEuMjE0NTkyOdIBhAFodHRwczovL3d3dy50c24uY2EvY2FuYWRhLWFyZ2VudGluYS1oZWFkbGluZXMtY29wYS1hbWVyaWNhLXVlZmEtZXVyby0yMDI0LXNlbWlmaW5hbC1hY3Rpb24tc3RhcnRpbmctdHVlc2RheS1vbi10c24tMS4yMTQ1OTI5P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Canada’s national junior team is headed to Windsor.</t>
+          <t>Monday Digest: Dabrowski Carries Canadian Hopes at Wimbledon</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.424007</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd2luZHNvcnN0YXIuY29tL3Nwb3J0cy9jYW5hZGFzLXdvcmxkLWp1bmlvci10ZWFtLWNvbWluZy10by13aW5kc29yLWZvci1mb3VyLWRheXMtdGhpcy1tb250aNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnRlbm5pc2NhbmFkYS5jb20vbmV3cy9tb25kYXktZGlnZXN0LWRhYnJvd3NraS1jYXJyaWVzLWNhbmFkaWFuLWhvcGVzLWF0LXdpbWJsZWRvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Canada’s digital services tax is here. How could it affect you?</t>
+          <t>Trudeau heads for the hot seat at NATO summit as allies question Canada's defence commitments</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.428066</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiOWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L9IBPWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL3RydWRlYXUtbmF0by1kZWZlbmNlLXNwZW5kaW5nLXN1bW1pdC0xLjcyNTYwMjfSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjAyNw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Head of Canada's spy agency announces he's stepping down from the job</t>
+          <t>Rival Watch: Is Canada earning respect ahead of Copa America semifinal vs. Argentina?</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.434310</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2RhdmlkLXZpZ25lYXVsdC1zdGVwcGluZy1kb3duLWNzaXMtZGlyZWN0b3ItMS43MjU0OTA50gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTQ5MDk?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9yaXZhbC13YXRjaC1pcy1jYW5hZGEtZWFybmluZy1yZXNwZWN0LWFoZWFkLW9mLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtdnMtYXJnZW50aW5hL9IBemh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvcml2YWwtd2F0Y2gtaXMtY2FuYWRhLWVhcm5pbmctcmVzcGVjdC1haGVhZC1vZi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLXZzLWFyZ2VudGluYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Canada to host the 70th annual NATO session in Montreal</t>
+          <t>Theo Argitis: Carney speculation summer mirage for disgruntled corporate Canada</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.434310</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY2FuYWRhLXRvLWhvc3QtdGhlLTcwdGgtYW5udWFsLW5hdG8tc2Vzc2lvbi1pbi1tb250cmVhbC0xLjY5NTIxMDXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9lY29ub215L21hcmstY2FybmV5LXNwZWN1bGF0aW9uLXN1bW1lci1taXJhZ2UtZm9yLWNvcnBvcmF0ZS1jYW5hZGHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Permanent Residence in Canada is not guaranteed for international students</t>
+          <t>Minister Joly to travel to the United Kingdom</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.438876</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmNpY25ld3MuY29tLzIwMjQvMDcvcGVybWFuZW50LXJlc2lkZW5jZS1pbi1jYW5hZGEtaXMtbm90LWd1YXJhbnRlZWQtZm9yLWludGVybmF0aW9uYWwtc3R1ZGVudHMtMDc0NDg1Ni5odG1s0gF7aHR0cHM6Ly93d3cuY2ljbmV3cy5jb20vMjAyNC8wNy9wZXJtYW5lbnQtcmVzaWRlbmNlLWluLWNhbmFkYS1pcy1ub3QtZ3VhcmFudGVlZC1mb3ItaW50ZXJuYXRpb25hbC1zdHVkZW50cy0wNzQ0ODU2Lmh0bWwvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9nbG9iYWwtYWZmYWlycy9uZXdzLzIwMjQvMDcvbWluaXN0ZXItam9seS10by10cmF2ZWwtdG8tdGhlLXVuaXRlZC1raW5nZG9tLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Canada to deport one of Iran's Larijani brothers after granting him PR status</t>
+          <t>Remnants of Hurricane Beryl could bring downpours to Ottawa-Gatineau</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.438876</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiKGh0dHBzOi8vd3d3LmlyYW5pbnRsLmNvbS9lbi8yMDI0MDcwNDcyMjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvcmVtbmFudHMtb2YtaHVycmljYW5lLWJlcnlsLWNvdWxkLWJyaW5nLWRvd25wb3Vycy10by1vdHRhd2EtZ2F0aW5lYXUtMS43MjU3NjE10gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTc2MTU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>U of T community members recognized with Order of Canada</t>
+          <t>VIDA Launches $300M Fund to Combat Canada's Affordable Housing Crisis</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.438876</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LnV0b3JvbnRvLmNhL25ld3MvdS10LWNvbW11bml0eS1tZW1iZXJzLXJlY29nbml6ZWQtb3JkZXItY2FuYWRhLTHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm5ld3N3aXJlLmNhL25ld3MtcmVsZWFzZXMvdmlkYS1sYXVuY2hlcy0zMDBtLWZ1bmQtdG8tY29tYmF0LWNhbmFkYS1zLWFmZm9yZGFibGUtaG91c2luZy1jcmlzaXMtODgzNDk1ODQ2Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Liberal government enacts controversial digital services tax, raising trade concerns</t>
+          <t>Canada to Share Plan for Reaching NATO’s Spending Target, Defense Minister Says</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.446344</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2RpZ2l0YWwtc2VydmljZXMtdGF4LWltcGxlbWVudGVkLTEuNzI1NDM1NtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU0MzU2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigQFodHRwczovL3d3dy5ibG9vbWJlcmcuY29tL25ld3MvYXJ0aWNsZXMvMjAyNC0wNy0wOC9jYW5hZGEtdG8tc2hhcmUtcGxhbi1mb3ItcmVhY2hpbmctbmF0by1zLXNwZW5kaW5nLXRhcmdldC1kZWZlbnNlLW1pbmlzdGVyLXNheXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Why Canada must act urgently to give undocumented migrants legal status</t>
+          <t>Unable to work in their official language of choice, some public servants are quitting — to Canada’s detriment</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.446344</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vdGhlY29udmVyc2F0aW9uLmNvbS93aHktY2FuYWRhLW11c3QtYWN0LXVyZ2VudGx5LXRvLWdpdmUtdW5kb2N1bWVudGVkLW1pZ3JhbnRzLWxlZ2FsLXN0YXR1cy0yMzI2ODbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vdW5hYmxlLXRvLXdvcmstaW4tdGhlaXItb2ZmaWNpYWwtbGFuZ3VhZ2Utb2YtY2hvaWNlLXNvbWUtcHVibGljLXNlcnZhbnRzLWFyZS1xdWl0dGluZy10by1jYW5hZGFzLWRldHJpbWVudC0yMzMxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Parks Canada considers visitor restrictions for Lake Louise area</t>
+          <t>Canada's gold exports to China rise, shining through the trade tensions</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.446344</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA1MDQxL3BhcmtzLWNhbmFkYS12aXNpdG9yLXJlc3RyaWN0aW9ucy1sYWtlLWxvdWlzZS1hbGJlcnRhL9IBXmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA1MDQxL3BhcmtzLWNhbmFkYS12aXNpdG9yLXJlc3RyaWN0aW9ucy1sYWtlLWxvdWlzZS1hbGJlcnRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vY29tbW9kaXRpZXMvbWluaW5nL2NhbmFkYS1nb2xkLWV4cG9ydHMtY2hpbmEtcmlzZS10cmFkZS10ZW5zaW9uc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>What is Canada's online harms bill, and what will it cost?</t>
+          <t>Standing Senate Committee on Agriculture and Forestry (44th Parliament, 1st Session)</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.454036</t>
+          <t>2024-07-09 15:26:45.075148</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY3JlYXRpbmctb25saW5lLWhhcm1zLXJlZ3VsYXRvcnMtZXhwZWN0ZWQtdG8tY29zdC1jYW5hZGEtMjAwLW1pbGxpb24tcGJvLTEuNjk1MTIyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLGh0dHBzOi8vc2VuY2FuYWRhLmNhL2VuL2NvbW1pdHRlZXMvYWdmby80NC0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Team Canada's women's water polo team seeks to make a splash at Paris 2024</t>
+          <t>Copa America Preview: Messi, Argentina rematch stand between Canada and glory</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.454036</t>
+          <t>2024-07-09 15:26:45.106418</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA0L3RlYW0tY2FuYWRhcy13b21lbnMtd2F0ZXItcG9sby10ZWFtLXNlZWtzLXRvLW1ha2UtYS1zcGxhc2gtYXQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdG9yb250by5jaXR5bmV3cy5jYS8yMDI0LzA3LzA5L2NhbmFkYS1jb3BhLWFtZXJpY2Etc2VtaS1maW5hbHMtYXJnZW50aW5hLW1hdGNoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Copa America Preview: Canada faces tough test in young Venezuela squad</t>
+          <t>Niagara Health is hiring!</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.462767</t>
+          <t>2024-07-09 15:26:45.106418</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtcHJldmlldy1jYW5hZGEtZmFjZXMtdG91Z2gtdGVzdC1pbi15b3VuZy12ZW5lenVlbGEtc3F1YWQv0gFtaHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL3NvY2Nlci9jb3BhLWFtZXJpY2EtcHJldmlldy1jYW5hZGEtZmFjZXMtdG91Z2gtdGVzdC1pbi15b3VuZy12ZW5lenVlbGEtc3F1YWQvc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiKWh0dHBzOi8vd3d3Lm5pYWdhcmFoZWFsdGgub24uY2Evc2l0ZS9ob21l0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Pro-Palestine group protests Israel game at Canada Cup softball</t>
+          <t>Canada vs. Messi, Argentina - Transcript</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2024-07-04 13:18:31.463994</t>
+          <t>2024-07-09 15:26:45.106418</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibWh0dHBzOi8vdGhlcHJvdmluY2UuY29tL3Nwb3J0cy9wcm8tcGFsZXN0aW5lLXByb3Rlc3RlcnMtZGlzcnVwdC10ZWFtLWlzcmFlbC1hdC1jYW5hZGEtY3VwLXNvZnRiYWxsLXRvdXJuYW1lbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vd3d3LmNiYy5jYS9yYWRpby9mcm9udGJ1cm5lci9jYW5hZGEtdnMtbWVzc2ktYXJnZW50aW5hLXRyYW5zY3JpcHQtMS43MjU4NTI40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTg1Mjg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Canada beat Venezuela on penalties to reach Copa America semifinals</t>
+          <t>Canada’s average rents just saw their biggest drop in 3 years</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2024-07-05 13:14:39.552015</t>
+          <t>2024-07-09 15:27:24.426857</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL2NhbmFkYS1iZWF0LXZlbmV6dWVsYS1vbi1wZW5hbHRpZXMtdG8tcmVhY2gtY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMtMS42OTUzMTk10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyODAwL3JlbnRhbC1tYXJrZXQtY2FuYWRhLXJlbnRzLWp1bmUtMjAyNC_SAU1odHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYxMjgwMC9yZW50YWwtbWFya2V0LWNhbmFkYS1yZW50cy1qdW5lLTIwMjQvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Canadian unemployment rate rose to 6.4% in June as jobs market stalls</t>
+          <t>How Canada became a car theft capital of the world</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2024-07-05 13:14:39.565381</t>
+          <t>2024-07-09 15:27:24.426857</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRpYW4tdW5lbXBsb3ltZW50LXJhdGUtcm9zZS10by02LTQtaW4tanVuZS1hcy1qb2JzLW1hcmtldC1zdGFsbHMtMS42OTUyNDkx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy9hcnRpY2xlcy9jeTc5ZHEybjA5M2_SATJodHRwczovL3d3dy5iYmMuY29tL25ld3MvYXJ0aWNsZXMvY3k3OWRxMm4wOTNvLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Canada semi-final bound after heart-stopping penalty shootout win over Venezuela in Copa América QF</t>
+          <t>Canada’s Men’s Rugby Team’s match day roster named ahead of match against Romania in Ottawa</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.412948</t>
+          <t>2024-07-09 15:27:24.426857</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtYm91bmQtZm9yLXNlbWktZmluYWxzLWFmdGVyLXRocmlsbGluZy1wZW5hbHR5LXNob290b3V0LXdpbi1vdmVyLXZlbmV6dWVsYS1pbi1jb3BhLWFtZXJpY2EtcWbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L2NhbmFkYS1zLW1lbi1zLXJ1Z2J5LXRlYW0tcy1tYXRjaC1kYXktcm9zdGVyLW5hbWVkLWFoZWFkLW9mLW1hdGNoLWFnYWluc3Qtcm9tYW5pYS1pbi1vdHRhd2HSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Nutrition labelling: List of ingredients</t>
+          <t>Canada ready for rematch with Messi, Argentina in Copa America semifinal on TSN</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.414005</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9oZWFsdGgtY2FuYWRhL3NlcnZpY2VzL2Zvb2QtbnV0cml0aW9uL251dHJpdGlvbi1sYWJlbGxpbmcvaW5ncmVkaWVudC1saXN0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY2FuYWRhLXJlYWR5LWZvci1yZW1hdGNoLXdpdGgtbGlvbmVsLW1lc3NpLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLW9uLXRzbi0xLjIxNDYxNzHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Canada beats Venezuela in penalty kicks, reaches semis in 1st Copa America</t>
+          <t>Nato allies pressure Canada to step up spending at Washington summit</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.414181</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS12ZW5lenVlbGEtY29wYS1hbWVyaWNhLXJlY2FwLWp1bHktNS0xLjcyNTYyNTjSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjI1OA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy9hcnRpY2xlcy9jbDR5Z3psejRtem_SATJodHRwczovL3d3dy5iYmMuY29tL25ld3MvYXJ0aWNsZXMvY2w0eWd6bHo0bXpvLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Dressage and eventing athletes and horses named to Team Canada for Paris 2024</t>
+          <t>TIFF announces five more World Premieres from Canada, France, India, UK, and USA</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.419254</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA1L2RyZXNzYWdlLWFuZC1ldmVudGluZy1hdGhsZXRlcy1hbmQtaG9yc2VzLW5hbWVkLXRvLXRlYW0tY2FuYWRhLWZvci1wYXJpcy0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vdGlmZi5uZXQvcHJlc3MvbmV3cy90aWZmLWFubm91bmNlcy1maXZlLW1vcmUtd29ybGQtcHJlbWllcmVzLWZyb20tY2FuYWRhLWZyYW5jZS1pbmRpYS11ay1hbmQtdXNh0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>A new U.K. government renews hopes for a free trade deal with Canada</t>
+          <t>Silk, Great Value plant-based milks recalled in Canada</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.424007</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2xhYm91ci11ay1lbGVjdGlvbi1mcmVlLXRyYWRlLWNhbmFkYS0xLjcyNTU3NzPSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTc3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMjUwL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtbWlsay1yZWNhbGwtY2FuYWRhL9IBWGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMjUwL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtbWlsay1yZWNhbGwtY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Canada job report: Country lost 1,400 jobs in June as unemployment rate</t>
+          <t>The remnants of hurricane Beryl are heading to Canada. Here's where it's expected to land</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.446344</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRpYW4tdW5lbXBsb3ltZW50LXJhdGUtcm9zZS10by02LTQtaW4tanVuZS1hcy1qb2JzLW1hcmtldC1zdGFsbHMtMS42OTUyNDkx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy5jdHZuZXdzLmNhL2NsaW1hdGUtYW5kLWVudmlyb25tZW50L3RoZS1yZW1uYW50cy1vZi1odXJyaWNhbmUtYmVyeWwtYXJlLWhlYWRpbmctdG8tY2FuYWRhLWhlcmUtcy13aGVyZS1pdC1zLWV4cGVjdGVkLXRvLWxhbmQtMS42OTU2OTE40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Canada edges Venezuela in shootout thriller; advances to Copa America semis</t>
+          <t>Canada’s priorities at NATO summit take backseat to spending concerns</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.446344</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY2FuYWRhLWRlZmVhdHMtdmVuZXp1ZWxhLWluLXBlbmFsdGllcy10by1hZHZhbmNlLWF0LWNvcGEtYW1lcmljYS0xLjIxNDUwOTHSAWVodHRwczovL3d3dy50c24uY2EvY2FuYWRhLWRlZmVhdHMtdmVuZXp1ZWxhLWluLXBlbmFsdGllcy10by1hZHZhbmNlLWF0LWNvcGEtYW1lcmljYS0xLjIxNDUwOTE_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwMzIzL2NhbmFkYS1uYXRvLXN1bW1pdC13YXNoaW5ndG9uLWRlZmVuY2Utc3BlbmRpbmcv0gFXaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTAzMjMvY2FuYWRhLW5hdG8tc3VtbWl0LXdhc2hpbmd0b24tZGVmZW5jZS1zcGVuZGluZy9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Canadian unemployment rate rises to 6.4%, with student summer jobs especially hard to come by</t>
+          <t>Canada vs. Argentina: Your guide to historic Copa America semifinal showdown</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.454036</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2J1c2luZXNzL2p1bmUtbGFib3VyLWZvcmNlLXN1cnZleS0xLjcyNTUxNDDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTE0MA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjExMDA1L2NhbmFkYS1hcmdlbnRpbmEtY29wYS1hbWVyaWNhL9IBRmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjExMDA1L2NhbmFkYS1hcmdlbnRpbmEtY29wYS1hbWVyaWNhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>What will the Canada-U.K. relationship look like under a Labour government?</t>
+          <t>BLOG: Canada unlikely to meet NATO commitments without significant debt accumulation</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.454036</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiPmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjAyNjAwL3VrLWVsZWN0aW9uLWxhYm91ci1jYW5hZGEv0gFCaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDI2MDAvdWstZWxlY3Rpb24tbGFib3VyLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmZyYXNlcmluc3RpdHV0ZS5vcmcvYmxvZ3MvY2FuYWRhLXVubGlrZWx5LXRvLW1lZXQtbmF0by1jb21taXRtZW50cy13aXRob3V0LXNpZ25pZmljYW50LWRlYnQtYWNjdW11bGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Unemployment rose to 6.4% in June: Statistics Canada</t>
+          <t>Tory leader widens gap over Trudeau on economy in Canada poll</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.459094</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmJubmJsb29tYmVyZy5jYS9zdGF0aXN0aWNzLWNhbmFkYS10by1yZWxlYXNlLWpvYnMtcmVwb3J0LWZvci1qdW5lLXRvZGF5LTEuMjA5MzI5OdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmJubmJsb29tYmVyZy5jYS9idXNpbmVzcy9wb2xpdGljcy8yMDI0LzA3LzA5L3RvcnktbGVhZGVyLXdpZGVucy1nYXAtb3Zlci10cnVkZWF1LW9uLWVjb25vbXktaW4tY2FuYWRhLXBvbGwv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Canada Soccer delivers new level of competition with PDP Championship</t>
+          <t>East Coast RV trip features family, food and a few bumps</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2024-07-05 13:18:31.463994</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItZGVsaXZlcnMtbmV3LWxldmVsLW9mLWNvbXBldGl0aW9uLXdpdGgtcGRwLWNoYW1waW9uc2hpcC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vby5jYW5hZGEuY29tL3RyYXZlbC9lYXN0LWNvYXN0LXJ2LXRyaXAtZmVhdHVyZXMtZmFtaWx5LWZvb2QtYW5kLWEtZmV3LWJ1bXBz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Scotland wins Douglas Horn Trophy in Canada’s Men’s Rugby Team’s return to home soil</t>
+          <t>Posthaste: Sellers are swarming Canada's housing market — especially in these cities</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2024-07-06 13:14:39.552015</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidWh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L3Njb3RsYW5kLXdpbnMtZG91Z2xhcy1ob3JuLXRyb3BoeS1pbi1jYW5hZGEtcy1tZW4tcy1ydWdieS10ZWFtLXMtcmV0dXJuLXRvLWhvbWUtc29pbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9zZWxsZXJzLXJ1c2gtYmFjay1jYW5hZGEtaG91c2luZy1tYXJrZXTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Scotland wins Douglas Horn Trophy in Canada's Men's Rugby Team's return to home soil</t>
+          <t>Alberta firefighters facing challenging conditions as heat wave sweeps Western Canada</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.419254</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidWh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L3Njb3RsYW5kLXdpbnMtZG91Z2xhcy1ob3JuLXRyb3BoeS1pbi1jYW5hZGEtcy1tZW4tcy1ydWdieS10ZWFtLXMtcmV0dXJuLXRvLWhvbWUtc29pbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9lZG1vbnRvbi9hbGJlcnRhLXdpbGRmaXJlcy1oZWF0LTEuNzI1Nzk0MtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3OTQy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Copa America Takeaways: Canada continues sensational run in its debut</t>
+          <t>Nova Scotia soccer star Shaffelburg at Copa America an 'achievement for whole family'</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.434310</t>
+          <t>2024-07-09 15:27:24.462518</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1jb250aW51ZXMtc2Vuc2F0aW9uYWwtcnVuLWluLWRlYnV0L9IBaGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtY29udGludWVzLXNlbnNhdGlvbmFsLXJ1bi1pbi1kZWJ1dC9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2phY29iLXNoYWZmZWxidXJnLWNhbmFkYS1jb3BhLWFtZXJpY2EtZmFtaWx5LWFjaGlldmVtZW50LTEuNzI1ODE4N9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4MTg3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Trae Bell-Haynes released from Canadian Olympic men's basketball training camp</t>
+          <t>Suspect in Carling Avenue homicide wanted on Canada-wide warrant</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.434310</t>
+          <t>2024-07-09 15:27:24.463530</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvb2x5bXBpY3Mvc3VtbWVyL2Jhc2tldGJhbGwvdHJhZS1iZWlsbC1jYW5hZGEtb2x5bXBpYy1iYXNrZXRiYWxsLWNhbXAtMS43MjU2NDU30gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTY0NTc?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb3R0YXdhY2l0aXplbi5jb20vbmV3cy9sb2NhbC1uZXdzL3N1c3BlY3QtaW4tY2FybGluZy1hdmUtaG9taWNpZGUtd2FudGVkLW9uLWNhbmFkYS13aWRlLXdhcnJhbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>In Canada for 7 years, family fights deportation to Nigeria</t>
+          <t>Canada draws link between June heat wave and climate change with new attribution analysis</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.438876</t>
+          <t>2024-07-09 15:27:24.463530</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvZmFtaWx5LWZpZ2h0cy1kZXBvcnRhdGlvbi1uaWdlcmlhLTEuNzI1NTUzMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU1NTMy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NsaW1hdGUvY2FuYWRhLWVjY2MtcmFwaWQtYXR0cmlidXRpb24taGVhdC0xLjcyNTc0NTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzQ1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Canada's Davies scores shootout penalty to bury World Cup demons</t>
+          <t>Meet Canada’s Best Employers For Diversity 2024</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.446344</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL3NvY2Nlci1jYW5hZGEtcy1kYXZpZXMtc2NvcmVzLXNob290b3V0LXBlbmFsdHktdG8tYnVyeS13b3JsZC1jdXAtZGVtb25zLTEuNjk1Mzk2NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvcmFjaGVscGVhY2htYW4vMjAyNC8wNy8wOS9tZWV0LWNhbmFkYXMtYmVzdC1lbXBsb3llcnMtZm9yLWRpdmVyc2l0eS0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Adam Zivo: Canada has the power (generators) to help beat Russia</t>
+          <t>Canada: grizzly bear hunting quietly reinstated in Alberta</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.446344</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9vcGluaW9uL3NlbmRpbmctZ2VuZXJhdG9ycy10by11a3JhaW5lLXdvdWxkLWJlLXdpbi13aW4tZm9yLWNhbmFkYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS93b3JsZC9hcnRpY2xlLzIwMjQvanVsLzA5L2FsYmVydGEtZ3JpenpseS1iZWFyLWh1bnRpbmfSAVJodHRwczovL2FtcC50aGVndWFyZGlhbi5jb20vd29ybGQvYXJ0aWNsZS8yMDI0L2p1bC8wOS9hbGJlcnRhLWdyaXp6bHktYmVhci1odW50aW5n?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Canada’s 1st female defence chief, a U.K. vote and top stories this week</t>
+          <t>How a new incubator is supercharging women-focused health startups in Canada</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2024-07-06 13:18:31.446344</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA2OTE3L2NhbmFkYXMtMXN0LWZlbWFsZS1kZWZlbmNlLXRvcC1zdG9yaWVzLXRoaXMtd2Vlay_SAVlodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYwNjkxNy9jYW5hZGFzLTFzdC1mZW1hbGUtZGVmZW5jZS10b3Atc3Rvcmllcy10aGlzLXdlZWsvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvaGVhbHRoL2hvdy1hLW5ldy1pbmN1YmF0b3ItaXMtc3VwZXJjaGFyZ2luZy13b21lbi1mb2N1c2VkLWhlYWx0aC1zdGFydHVwcy1pbi1jYW5hZGEtMS42OTU2Mjc00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Thinking about leaving Canada? Here are the financial considerations you need to know</t>
+          <t>Ontario court approves class-action by immigration detainees against federal government</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2024-07-07 13:14:39.565381</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vcGVyc29uYWwtZmluYW5jZS9sZWF2aW5nLWNhbmFkYS1uZWVkLXRvLWtub3fSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihwFodHRwczovL3d3dy5jYmMuY2EvbmV3cy9jYW5hZGEvb3R0YXdhL29udGFyaW8tY291cnQtYXBwcm92ZXMtY2xhc3MtYWN0aW9uLWJ5LWltbWlncmF0aW9uLWRldGFpbmVlcy1hZ2FpbnN0LWZlZGVyYWwtZ292ZXJubWVudC0xLjcyNTc2MDLSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzYwMg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Japan’s tourism tax sparks industry speculation in Canada</t>
+          <t>The philosophy — and politics — behind Canada's reluctance to meet NATO's spending target</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2024-07-07 13:14:39.565381</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2phcGFuLXMtdG91cmlzbS10YXgtc3BhcmtzLWluZHVzdHJ5LXNwZWN1bGF0aW9uLWluLWNhbmFkYS0xLjY5NTI0NzHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2NhbmFkYS1uYXRvLWpvbHktYmxhaXItdHJ1ZGVhdS1kZWZlbmNlLTEuNzI1NzczN9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3NzM3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Considering leaving Canada? Here's what you need to know</t>
+          <t>KFC's move to halal menu in most of Ontario sparks outrage, calls for boycott — and support</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.834503</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vcGVyc29uYWwtZmluYW5jZS9sZWF2aW5nLWNhbmFkYS1uZWVkLXRvLWtub3fSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9rZmMtaGFsYWwtbWVudS1ib3ljb3R0LTEuNzI1ODI4OdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4Mjg5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Canada tourism: Should Canada impose a tourist tax?</t>
+          <t>Where Did My Money Go? The Cost of Being Single in Canada</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.834503</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2phcGFuLXMtdG91cmlzbS10YXgtc3BhcmtzLWluZHVzdHJ5LXNwZWN1bGF0aW9uLWluLWNhbmFkYS0xLjY5NTI0NzHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikAFodHRwczovL3d3dy5yYmNyb3lhbGJhbmsuY29tL2VuLWNhL215LW1vbmV5LW1hdHRlcnMvbGlmZS1ldmVudHMvZmFtaWx5LWV2ZW50cy9tYXJyaWFnZS93aGVyZS1kaWQtbXktbW9uZXktZ28tdGhlLWNvc3Qtb2YtYmVpbmctc2luZ2xlLWluLWNhbmFkYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Extreme heat grips much of Western Canada</t>
+          <t>Ticketmaster notifies Canadian customers of May data breach</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.839124</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiNWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9iYy1oZWF0LWRvbWUtMS43MjU2NTk30gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTY1OTc?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMTMyL3RpY2tldG1hc3Rlci1oYWNrLWN1c3RvbWVycy1jYW5hZGEv0gFLaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTIxMzIvdGlja2V0bWFzdGVyLWhhY2stY3VzdG9tZXJzLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Copa America 2024: Canada advances to semifinals</t>
+          <t>Where to watch Canada vs. Argentina's Copa América semifinal: Streaming, TV channels, start time and more</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.839124</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL2NhbmFkYS1iZWF0cy12ZW5lenVlbGEtdG8tYWR2YW5jZS10by1jb3BhLWFtZXJpY2Etc2VtaWZpbmFscy0xLjY5NTMxOTXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL2NhLm5ld3MueWFob28uY29tL3doZXJlLXRvLXdhdGNoLWNhbmFkYS12cy1hcmdlbnRpbmFzLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtc3RyZWFtaW5nLXR2LWNoYW5uZWxzLXN0YXJ0LXRpbWUtYW5kLW1vcmUtMTgwNTQwODYxLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Badminton - 2024 YONEX Canada Open: Finals</t>
+          <t>28 one-day heat records tumble, Lytton hottest place in Canada</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.844117</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0MzY2MDTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDkvYmMtanVseS04LWhlYXQtcmVjb3Jkcy1seXR0b24tY2FuYWRhLWhvdC1zcG90L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Best slo-pitch players in Canada fight for spot in 2025 Canadian Championships | CTV News</t>
+          <t>Canada Soccer AccelerateHER Program Awards Grants and Funds All-Women C-Diploma Workshops</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.860352</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vbG9uZG9uLmN0dm5ld3MuY2EvYmVydGgtaW4tY2FuYWRpYW4tY2hhbXBpb25zaGlwcy1vbi10aGUtbGluZS1hdC1zbG8tcGl0Y2gtZWxpbWluYXRpb25zLXN1bmRheS0xLjY5NTQ1MjnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItYWNjZWxlcmF0ZWhlci1wcm9ncmFtLWF3YXJkcy1ncmFudHMtYW5kLWZ1bmRzLWFsbC13b21lbi1jLWRpcGxvbWEtd29ya3Nob3BzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>For Canadians, is it time to buy a new car? Experts say vehicle supply is building and prices are going down</t>
+          <t>Local colleges named in top 200 employers in Canada for diversity</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.864712</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiN2h0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9uZXdzL2NhbmFkYS9jYW5hZGlhbi1jYXItc2FsZXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbG9uZG9uLmN0dm5ld3MuY2EvbG9jYWwtY29sbGVnZXMtbmFtZWQtaW4tdG9wLTIwMC1lbXBsb3llcnMtaW4tY2FuYWRhLWZvci1kaXZlcnNpdHktMS42OTU3MTgx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Ontario mom and kids shot dead in what OPP describe as a case of intimate partner violence</t>
+          <t>A Final Rest for the Unknown Newfoundland Soldier</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.869285</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9uZXdzL2NhbmFkYS9vbnRhcmlvLW1vbS1jYXJseS13YWxzaC1hbmQta2lkcy1kZWF0aNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5jYW5hZGEuY2EvZW4vZGVwYXJ0bWVudC1uYXRpb25hbC1kZWZlbmNlL21hcGxlLWxlYWYvZGVmZW5jZS8yMDI0LzA3L2ZpbmFsLXJlc3QtZm9yLXVua25vd24tbmV3Zm91bmRsYW5kLXNvbGRpZXIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Extreme geomagnetic storm may spark widespread auroras over Canada on Friday</t>
+          <t>Meteorologists warn of "torrential downpour" as hurricane remnants head for southwestern Ontario</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.876046</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vY2EubmV3cy55YWhvby5jb20vc2V2ZXJlLWdlb21hZ25ldGljLXN0b3JtLW1heS1zcGFyay0yMzU3MTY3MDUuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9sb25kb24vaHVycmljYW5lLWJlcnlsLXNvdXRoZXJuLW9udGFyaW8tbG9uZG9uLXJhaW5mYWxsLTEuNzI1ODAyMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4MDIy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Copa America semifinals: What to know about Argentina vs. Canada and Colombia vs. Uruguay</t>
+          <t>Canada to provide NATO updated defence spending plan</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.878146</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LmNic3Nwb3J0cy5jb20vc29jY2VyL25ld3MvY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMtd2hhdC10by1rbm93LWFib3V0LWFyZ2VudGluYS12cy1jYW5hZGEtYW5kLWNvbG9tYmlhLXZzLXVydWd1YXkv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9uZXdzL3dvcmxkL2NhbmFkYS10by1wcm92aWRlLW5hdG8tdXBkYXRlZC1kZWZlbmNlLXNwZW5kaW5nLXBsYW7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>A winter surprise, does the U.S. see more snow than Canada?</t>
+          <t>Record 107 teams to qualify for Canada Soccer’s 2024 amateur competitions</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.880200</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vY2EubmV3cy55YWhvby5jb20vd2ludGVyLXN1cnByaXNlLWRvZXMtdS1zZWUtMDEzOTI0NDM0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL3JlY29yZC0xMDctdGVhbXMtdG8tcXVhbGlmeS1mb3ItY2FuYWRhLXNvY2NlcnMtMjAyNC1hbWF0ZXVyLWNvbXBldGl0aW9ucy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>‘Canada could be a world leader’: Indigenous people say their rapidly growing tourism sector needs more support from Ottawa</t>
+          <t>Drake bets $300K on Canada to beat Messi, Argentina in Copa America semifinal</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.884388</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiugFodHRwczovL3d3dy50aGVzdGFyLmNvbS9wb2xpdGljcy9mZWRlcmFsL2NhbmFkYS1jb3VsZC1iZS1hLXdvcmxkLWxlYWRlci1pbmRpZ2Vub3VzLXBlb3BsZS1zYXktdGhlaXItcmFwaWRseS1ncm93aW5nLXRvdXJpc20tc2VjdG9yLW5lZWRzL2FydGljbGVfOTllYjg2MDQtM2ExYS0xMWVmLTgyYTctYmYxMDU4NDcyY2U2Lmh0bWzSAb4BaHR0cHM6Ly93d3cudGhlc3Rhci5jb20vcG9saXRpY3MvZmVkZXJhbC9jYW5hZGEtY291bGQtYmUtYS13b3JsZC1sZWFkZXItaW5kaWdlbm91cy1wZW9wbGUtc2F5LXRoZWlyLXJhcGlkbHktZ3Jvd2luZy10b3VyaXNtLXNlY3Rvci1uZWVkcy9hcnRpY2xlXzk5ZWI4NjA0LTNhMWEtMTFlZi04MmE3LWJmMTA1ODQ3MmNlNi5hbXAuaHRtbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9kcmFrZS1iZXRzLTMwMGstb24tY2FuYWRhLXRvLWJlYXQtbWVzc2ktYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWwv0gFzaHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL3NvY2Nlci9kcmFrZS1iZXRzLTMwMGstb24tY2FuYWRhLXRvLWJlYXQtbWVzc2ktYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWwvc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Renters with disabilities live in fear of eviction. Now, this man with PTSD sleeps in a shed</t>
+          <t>'Tears come to my eyes': Track star and family granted extension to stay in Canada after deportation order</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.889468</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9kaXNhYmlsaXR5LXJlbnQtY2FuYWRhLTEuNzI1NDExONIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU0MTE4?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijAFodHRwczovL3Rvcm9udG8uY3R2bmV3cy5jYS90ZWFycy1jb21lLXRvLW15LWV5ZXMtdHJhY2stc3Rhci1hbmQtZmFtaWx5LWdyYW50ZWQtZXh0ZW5zaW9uLXRvLXN0YXktaW4tY2FuYWRhLWFmdGVyLWRlcG9ydGF0aW9uLW9yZGVyLTEuNjk1Njg4M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Key wildfire triggers in Canada and tips to prevent their ignition</t>
+          <t>How Canada’s dream supersonic interceptor became a national nightmare</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.889468</t>
+          <t>2024-07-09 16:26:45.127192</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20va2V5LXdpbGRmaXJlLXRyaWdnZXJzLWNhbmFkYS10aXBzLTE4MjMyNjA3MS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNubi5jb20vdHJhdmVsL2NhbmFkYS1kcmVhbS1zdXBlcnNvbmljLWJvbWJlci1hdnJvLWFycm93L2luZGV4Lmh0bWzSAUhodHRwczovL2FtcC5jbm4uY29tL2Nubi90cmF2ZWwvY2FuYWRhLWRyZWFtLXN1cGVyc29uaWMtYm9tYmVyLWF2cm8tYXJyb3c?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>'Canada's Drag Race: Canada vs. the World' named best reality TV, competition show in the country</t>
+          <t>Canada's landlords now asking an average of $2,185/month for rent</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.892765</t>
+          <t>2024-07-09 16:26:45.131608</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihAFodHRwczovL2NhLm5ld3MueWFob28uY29tL2NhbmFkYXMtZHJhZy1yYWNlLWNhbmFkYS12cy10aGUtd29ybGQtbmFtZWQtYmVzdC1yZWFsaXR5LXR2LWNvbXBldGl0aW9uLXNob3ctaW4tdGhlLWNvdW50cnktMTcxNzA1MTgyLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1zLWxhbmRsb3Jkcy1ub3ctYXNraW5nLWFuLWF2ZXJhZ2Utb2YtMi0xODUtbW9udGgtZm9yLXJlbnQtMS42OTU3MjI10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>El Niño's impact on Canada's winter: What to expect?</t>
+          <t>Canada urged to spend more on defence as NATO chief addresses summit</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.892765</t>
+          <t>2024-07-09 16:27:24.433908</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQGh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vZWwtbmktb3MtaW1wYWN0LWNhbmFkYXMtMDk0MDQ0MjQ4Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNTYwL25hdG8tc3VtbWl0LWRlZmVuY2Utc3BlbmRpbmctY2FuYWRhL9IBTGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNTYwL25hdG8tc3VtbWl0LWRlZmVuY2Utc3BlbmRpbmctY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>FIBA 3x3 Women's Series Edmonton semifinal: Canada vs. Barcelona Panthers</t>
+          <t>Key things to know about Canada vs. Argentina’s Copa America semi-final</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.894529</t>
+          <t>2024-07-09 16:27:24.433908</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDE3MDfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYmh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL3NvY2Nlci9hcnRpY2xlLWNhbmFkYS12cy1hcmdlbnRpbmEtc2VtaWZpbmFscy1ob3ctdG8td2F0Y2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Canada Soccer shows new way of doing business in hiring Jesse Marsch as men's coach</t>
+          <t>First Nations leaders from across Canada gather in Montreal for AFN annual general assembly</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2024-07-07 13:18:41.894529</t>
+          <t>2024-07-09 16:27:24.449599</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vbmV3c2FsZXJ0LWplc3NlLW1hcnNjaC1uYW1lZC1jYW5hZGlhbi0yMDI3MzE4OTkuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiPWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2luZGlnZW5vdXMvYWZuLWFnYS1tb250cmVhbC0xLjcyNTc1NTDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzU1MA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Canada's Got Talent 2024 winner to take stage at CreeFest</t>
+          <t>The United Church of Canada Releases First Strategic Plan Report</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2024-07-07 14:18:41.884388</t>
+          <t>2024-07-09 16:27:24.449599</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LnRpbW1pbnN0b2RheS5jb20vbG9jYWwtbmV3cy9jYW5hZGFzLWdvdC10YWxlbnQtMjAyNC13aW5uZXItdG8tdGFrZS1zdGFnZS1hdC1jcmVlZmVzdC05MTgzODMy0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdW5pdGVkLWNodXJjaC5jYS9uZXdzL3VuaXRlZC1jaHVyY2gtY2FuYWRhLXJlbGVhc2VzLWZpcnN0LXN0cmF0ZWdpYy1wbGFuLXJlcG9ydNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>FIBA 3x3 Women's Series Edmonton final: Canada vs. Dallas 3XBA</t>
+          <t>Moving truck driver says mechanical failure led to deadly crash on Trans-Canada Highway west of Calgary</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2024-07-07 14:18:41.889468</t>
+          <t>2024-07-09 16:27:24.465540</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDE3MDbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vY2FsZ2FyeWhlcmFsZC5jb20vbmV3cy9jcmltZS9tZWNoYW5pY2FsLWZhaWx1cmUtZGVhZGx5LWNyYXNoLXRyYW5zLWNhbmFkYS1oaWdod2F5LWRyaXZlctIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>No soccer-playing country is having a better summer than Canada at the Copa América – upsetting Americans is the ...</t>
+          <t>Ottawa aims to clear Phoenix backlog by 2025, spend nearly $1B more</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2024-07-07 15:18:41.842824</t>
+          <t>2024-07-09 17:26:45.128203</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL2FydGljbGUtbm8tc29jY2VyLXBsYXlpbmctY291bnRyeS1vbi1lYXJ0aC1pcy1oYXZpbmctYS1iZXR0ZXItc3VtbWVyLXRoYW4v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEzNDY0L3Bob2VuaXgtcGF5LXN5c3RlbS1iYWNrbG9nLW5ldy1zcGVuZGluZy1kZWFkbGluZS_SAVlodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYxMzQ2NC9waG9lbml4LXBheS1zeXN0ZW0tYmFja2xvZy1uZXctc3BlbmRpbmctZGVhZGxpbmUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Alberta RCMP catch 101 drunk drivers during Canada Day long weekend</t>
+          <t>Record rainfall expected for parts of southwestern Ontario on Wednesday</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2024-07-07 15:18:41.849194</t>
+          <t>2024-07-09 17:27:24.481180</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vZWRtb250b25qb3VybmFsLmNvbS9uZXdzL2xvY2FsLW5ld3MvYWxiZXJ0YS1kcnVuay1kcml2aW5nLWNhbmFkYS1kYXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS93aW5kc29yL3JhaW5mYWxsLXJlY29yZC1icmVha2luZy1zb3V0aHdlc3Rlcm4tb250YXJpby0xLjcyNTgzNznSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODM3OQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Argentina vs. Canada odds, lineup prediction, live stream, picks: Where to watch Leo Messi, Copa America on TV</t>
+          <t>Drake places $300,000 bet on Canada to beat Argentina in Copa America semifinals</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2024-07-07 15:18:41.860352</t>
+          <t>2024-07-09 17:27:24.481180</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5jYnNzcG9ydHMuY29tL3NvY2Nlci9uZXdzL2FyZ2VudGluYS12cy1jYW5hZGEtb2Rkcy1saW5ldXAtcHJlZGljdGlvbi1saXZlLXN0cmVhbS1waWNrcy13aGVyZS10by13YXRjaC1sZW8tbWVzc2ktY29wYS1hbWVyaWNhLW9uLXR2L9IBkwFodHRwczovL3d3dy5jYnNzcG9ydHMuY29tL3NvY2Nlci9uZXdzL2FyZ2VudGluYS12cy1jYW5hZGEtb2Rkcy1saW5ldXAtcHJlZGljdGlvbi1saXZlLXN0cmVhbS1waWNrcy13aGVyZS10by13YXRjaC1sZW8tbWVzc2ktY29wYS1hbWVyaWNhLW9uLXR2L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3LnVzYXRvZGF5LmNvbS9zdG9yeS9zcG9ydHMvc29jY2VyLzIwMjQvMDcvMDkvZHJha2UtMzAway1iZXQtY2FuYWRhLWFyZ2VudGluYS1jb3BhLWFtZXJpY2Etc2VtaWZpbmFscy83NDM0NDMxOTAwNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Your Canada Day weekend forecast holds a mix of gloom and fantastic days</t>
+          <t>Argentina 2-0 Canada: 2024 Copa América semi-final – as it happened</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2024-07-07 15:18:41.884388</t>
+          <t>2024-07-09 18:26:45.127192</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vY2FuYWRhLWRheS13ZWVrZW5kLWZvcmVjYXN0LWhvbGRzLTEwMDAwMjU4MS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9saXZlLzIwMjQvanVsLzA5L2FyZ2VudGluYS12LWNhbmFkYS0yMDI0LWNvcGEtYW1lcmljYS1zZW1pLWZpbmFsLWxpdmUtdXBkYXRlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>'Heat event' coming to much of southern Ontario early this week: Environment Canada</t>
+          <t>Ontario says nine listeriosis infections linked to recall of silk milk</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.834503</t>
+          <t>2024-07-09 18:26:45.131608</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvaGVhdC1ldmVudC1jb21pbmctdG8tbXVjaC1vZi1zb3V0aGVybi1vbnRhcmlvLWVhcmx5LXRoaXMtd2Vlay1lbnZpcm9ubWVudC1jYW5hZGEtMS42OTU0ODI40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vY2FuYWRhL2FydGljbGUtb250YXJpby1zYXlzLW5pbmUtbGlzdGVyaW9zaXMtaW5mZWN0aW9ucy1saW5rZWQtdG8tcmVjYWxsLW9mLXNpbGstbWlsay_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>NBA star Antetokounmpo leads Greece into Olympics and Group A date with Canada's men's basketball team</t>
+          <t>Canada’s Copa America dream run ends with 2-0 loss to Argentina in semi-final</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.839124</t>
+          <t>2024-07-09 18:27:24.426857</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvb2x5bXBpY3Mvc3VtbWVyL2Jhc2tldGJhbGwvb2x5bXBpYy1tZW5zLWJhc2tldGJhbGwtcXVhbGlmeWluZy0xLjcyNTY3NzDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1Njc3MA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL3NvY2Nlci9hcnRpY2xlLWNhbmFkYS1wcmltZWQtZm9yLXJvbGUtb2YtZ2lhbnQta2lsbGVycy1pbi1jb3BhLXNlbWlzLWNsYXNoLXdpdGgv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Canadian Rowers Dominate at FISU World University Rowing Championships and Henley Royal Regatta</t>
+          <t>Soccer frenzy in the nation’s capital</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.844117</t>
+          <t>2024-07-09 18:27:24.426857</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vcm93aW5nY2FuYWRhLm9yZy9jYW5hZGlhbi1yb3dlcnMtZG9taW5hdGUtYXQtZmlzdS13b3JsZC11bml2ZXJzaXR5LXJvd2luZy1jaGFtcGlvbnNoaXBzLWFuZC1oZW5sZXktcm95YWwtcmVnYXR0YS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vb3R0YXdhLmN0dm5ld3MuY2Evc29jY2VyLWZyZW56eS1pbi10aGUtbmF0aW9uLXMtY2FwaXRhbC0xLjY5NTc1MDfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Extreme temperatures across Alberta boost wildfire risk, prompt heat warnings</t>
+          <t>Drake bets big on Canada to upset Argentina in Copa America semifinals</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.859411</t>
+          <t>2024-07-09 18:27:24.433908</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9lZG1vbnRvbi9leHRyZW1lLXRlbXBlcmF0dXJlcy1hbGJlcnRhLTEuNzI1NjY3OdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU2Njc5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvZW50ZXJ0YWlubWVudC9kcmFrZS1iZXRzLWJpZy1vbi1jYW5hZGEtdG8tdXBzZXQtYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWxzLTEuNjk1NzUxMdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>'Heat event' coming to much of southwestern Ontario early this week: Environment Canada</t>
+          <t>Ontario reports five people hospitalized with listeriosis, as Silk and Great Value beverages recalled across Canada</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.864712</t>
+          <t>2024-07-09 18:27:24.449599</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMi6AFodHRwczovL3d3dy5jcDI0LmNvbS9tb2JpbGUvbmV3cy9oZWF0LWV2ZW50LWNvbWluZy10by1tdWNoLW9mLXNvdXRod2VzdGVybi1vbnRhcmlvLWVhcmx5LXRoaXMtd2Vlay1lbnZpcm9ubWVudC1jYW5hZGEtMS42OTU0ODI4P2NhY2hlPXllc2NsaXBJZDEwNDA2MjAwdGV4dC9odG1sO2NoYXJzZXQ9dXRmLTgwNDA0LzcuMjU4NDU0LzcuNjMyMjQzLzcuMzA0NTA1LzcuMzA0NTA1LzcuMzA0NTA1LzcuMzA0NTA10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiwQFodHRwczovL3d3dy50aGVzdGFyLmNvbS9uZXdzL2NhbmFkYS9vbnRhcmlvLXJlcG9ydHMtZml2ZS1wZW9wbGUtaG9zcGl0YWxpemVkLXdpdGgtbGlzdGVyaW9zaXMtYXMtc2lsay1hbmQtZ3JlYXQtdmFsdWUtYmV2ZXJhZ2VzLXJlY2FsbGVkLWFjcm9zcy9hcnRpY2xlX2Q0YmI0YmE4LTNlMTUtMTFlZi1hODhjLWZiMjczNGQ2MGFiYS5odG1s0gHFAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL25ld3MvY2FuYWRhL29udGFyaW8tcmVwb3J0cy1maXZlLXBlb3BsZS1ob3NwaXRhbGl6ZWQtd2l0aC1saXN0ZXJpb3Npcy1hcy1zaWxrLWFuZC1ncmVhdC12YWx1ZS1iZXZlcmFnZXMtcmVjYWxsZWQtYWNyb3NzL2FydGljbGVfZDRiYjRiYTgtM2UxNS0xMWVmLWE4OGMtZmIyNzM0ZDYwYWJhLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>ILWU Plans Strike at DP World Canada Starting Monday</t>
+          <t>Thunderstorms flood Trans-Canada Highway near Pasadena</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.864712</t>
+          <t>2024-07-09 18:27:24.462518</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiW2h0dHBzOi8vbWFyaXRpbWUtZXhlY3V0aXZlLmNvbS9hcnRpY2xlL2lsd3UtcGxhbnMtc3RyaWtlLWF0LWRwLXdvcmxkLWNhbmFkYS1zdGFydGluZy1tb25kYXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9uZXdmb3VuZGxhbmQtbGFicmFkb3IvcGFzYWRlbmEtaGlnaHdheS1mbG9vZGluZy0xLjcyNTg2NTLSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODY1Mg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Heat warning issued for Maritimes on Monday and Tuesday</t>
+          <t>Durant (calf) out for USA's friendly vs. Canada</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.869285</t>
+          <t>2024-07-09 18:27:24.465540</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9wcmluY2UtZWR3YXJkLWlzbGFuZC9wZWktZW52aXJvbm1lbnQtY2FuYWRhLWhlYXQtd2FybmluZy0xLjcyNTY3NDbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1Njc0Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmVzcG4uY29tL25iYS9zdG9yeS9fL2lkLzQwNTI4OTg3L2tldmluLWR1cmFudC1jYWxmLXRlYW0tdXNhLWZyaWVuZGx5LXZzLWNhbmFkYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>How can Canada stay sharp mentally, physically leading up to match vs. Argentina? - Video</t>
+          <t>Wildfire danger soars as heat wave envelops Western Canada</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2024-07-07 16:18:41.880334</t>
+          <t>2024-07-09 19:27:24.481180</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnRzbi5jYS92aWRlby9ob3ctY2FuLWNhbmFkYS1zdGF5LXNoYXJwLW1lbnRhbGx5LXBoeXNpY2FsbHktbGVhZGluZy11cC10by1tYXRjaC12cy1hcmdlbnRpbmF-Mjk1Mzk5N9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vY2FuYWRhL2FsYmVydGEvYXJ0aWNsZS13aWxkZmlyZS1kYW5nZXItc29hcnMtYXMtaGVhdC13YXZlLWVudmVsb3Blcy13ZXN0ZXJuLWNhbmFkYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Group A Finalized as Canada Prepares for Olympic Men's Basketball</t>
+          <t>Alvarez scores as Argentina leads Canada at halftime of Copa America semifinal</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2024-07-07 17:18:41.834503</t>
+          <t>2024-07-09 20:26:45.075148</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LnNpLmNvbS9uYmEvcmFwdG9ycy9ncmVlY2Utc3BhaW4tYWR2YW5jZS10by1wYXJpcy1vbHltcGljcy1pbi1ncm91cC1hLWFnYWluc3QtY2FuYWRh0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvanVsaWFuLWFsdmFyZXotc2NvcmVzLWFzLWFyZ2VudGluYS1sZWFkcy1jYW5hZGEtYXQtaGFsZnRpbWUtb2YtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC0xLjIxNDY1MDfSAXpodHRwczovL3d3dy50c24uY2EvanVsaWFuLWFsdmFyZXotc2NvcmVzLWFzLWFyZ2VudGluYS1sZWFkcy1jYW5hZGEtYXQtaGFsZnRpbWUtb2YtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC0xLjIxNDY1MDc_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Beryl's lingering impacts to reach southern Ontario and Quebec this week</t>
+          <t>Extreme June heatwave 'much more likely' caused by human-made climate change, says Environment Canada</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2024-07-07 17:18:41.844117</t>
+          <t>2024-07-09 20:27:24.465540</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3LnRoZXdlYXRoZXJuZXR3b3JrLmNvbS9lbi9uZXdzL3dlYXRoZXIvZm9yZWNhc3RzL2Jlcnlscy1saW5nZXJpbmctaW1wYWN0cy10by1yZWFjaC1zb3V0aGVybi1vbnRhcmlvLXRoaXMtd2Vla9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL2F0bGFudGljLmN0dm5ld3MuY2EvbW9yZS9leHRyZW1lLWp1bmUtaGVhdHdhdmUtbXVjaC1tb3JlLWxpa2VseS1jYXVzZWQtYnktaHVtYW4tbWFkZS1jbGltYXRlLWNoYW5nZS1zYXlzLWVudmlyb25tZW50LWNhbmFkYS0xLjY5NTc2MznSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Okotoks athletes start strong at Football Canada Cup</t>
+          <t>Argentina tops Canada 2-0 to advance to Copa América final</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2024-07-07 17:18:41.844117</t>
+          <t>2024-07-09 21:26:45.067635</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3Lndlc3Rlcm53aGVlbC5jYS9sb2NhbC1zcG9ydHMvb2tvdG9rcy1hdGhsZXRlcy1zdGFydC1zdHJvbmctYXQtZm9vdGJhbGwtY2FuYWRhLWN1cC05MTg3ODc00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vc3Rvcmllcy9zb2NjZXIvYXJnZW50aW5hLXRvcHMtY2FuYWRhLTItMC1hZHZhbmNlLWNvcGEtYW1lcmljYS1maW5hbNIBXWh0dHBzOi8vYW1wLmZveHNwb3J0cy5jb20vc3Rvcmllcy9zb2NjZXIvYXJnZW50aW5hLXRvcHMtY2FuYWRhLTItMC1hZHZhbmNlLWNvcGEtYW1lcmljYS1maW5hbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Heat warning issued in Toronto for Monday and Tuesday</t>
+          <t>The Breakdown | Nunavut grows up + Canada and NATO</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>2024-07-07 17:18:41.849194</t>
+          <t>2024-07-09 21:26:45.075148</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS90b3JvbnRvL2hlYXQtd2FybmluZy10b3JvbnRvLW1vbmRheS0xLjcyNTY3OTnSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1Njc5OQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDM4MzLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Police believe Sask. man wanted on Canada-wide warrant may be in Peel Region</t>
+          <t>Vote for Canada’s best litigation boutiques for 2024-25</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>2024-07-07 17:18:41.864712</t>
+          <t>2024-07-09 21:26:45.090846</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vdG9yb250by5jaXR5bmV3cy5jYS8yMDI0LzA3LzA3L3BvbGljZS1iZWxpZXZlLXNhc2stbWFuLXdhbnRlZC1vbi1jYW5hZGEtd2lkZS13YXJyYW50LW1heS1iZS1pbi1wZWVsLXJlZ2lvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmNhbmFkaWFubGF3eWVybWFnLmNvbS9uZXdzL2dlbmVyYWwvdm90ZS1mb3ItY2FuYWRhcy1iZXN0LWxpdGlnYXRpb24tYm91dGlxdWVzLWZvci0yMDI0LTI1LzM4NzIyONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Federal board finds longshore foremen union bargaining in bad faith</t>
+          <t>Government of Canada publishes a report to tackle anti-black racism in the justice system</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.827435</t>
+          <t>2024-07-09 21:26:45.090846</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA5NTIzL2ZlZGVyYWwtYm9hcmQtbG9uZ3Nob3JlLWZvcmVtYW4tdW5pb24v0gFOaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDk1MjMvZmVkZXJhbC1ib2FyZC1sb25nc2hvcmUtZm9yZW1hbi11bmlvbi9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5jYW5hZGlhbmxhd3llcm1hZy5jb20vbmV3cy9nZW5lcmFsL2dvdmVybm1lbnQtb2YtY2FuYWRhLXB1Ymxpc2hlcy1hLXJlcG9ydC10by10YWNrbGUtYW50aS1ibGFjay1yYWNpc20taW4tdGhlLWp1c3RpY2Utc3lzdGVtLzM4NzIyOdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Canada to face Argentina in Copa semi-finals</t>
+          <t>Supreme Court Justice recuses himself from Quebec secularism law case</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.844117</t>
+          <t>2024-07-09 21:26:45.127192</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vZWRtb250b24uY3R2bmV3cy5jYS92aWRlby9jMjk1NDEwMC1jYW5hZGEtdG8tZmFjZS1hcmdlbnRpbmEtaW4tY29wYS1zZW1pLWZpbmFsc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9tb250cmVhbC9zY2otbWFobXVkLWphbWFsLXJlY3VzYWwtMS43MjU5MDA40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTkwMDg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Canada sees its first 40°C reading this year as a prolonged heat wave hits B.C.</t>
+          <t>Argentina ends Canada's run to reach Copa America final again</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.860352</t>
+          <t>2024-07-09 21:26:45.131608</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vY2FuYWRhLW5vdGNoZXMtZmlyc3QtNDAtYy0wMDIyMTQ0NTIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiK2h0dHBzOi8vd3d3LnRoZXNjb3JlLmNvbS90b3Bzbi9uZXdzLzI5Mzc4NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Heat warning not keeping people away from first weekend of Stampede</t>
+          <t>Canada's historic Copa America run ends with semifinal loss to Argentina</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.860352</t>
+          <t>2024-07-09 21:27:24.417838</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9jYWxnYXJ5L2hlYXQtd2FybmluZy1zdGFtcGVkZS13YXRlci1hY2Nlc3Mtd2Vla2VuZC0xLjcyNTY4MTPSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjgxMw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXJlY2FwLWp1bHktOS0xLjcyNTg3MzHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODczMQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Life after Oilers: How Edmonton bar owners are benefiting from Euro, Canada’s Copa America run</t>
+          <t>Canada undone by Álvarez, Messi in hard-fought Copa América semifinal vs. Argentina</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.860352</t>
+          <t>2024-07-09 21:27:24.417838</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vZWRtb250b24uY2l0eW5ld3MuY2EvMjAyNC8wNy8wNy9lZG1vbnRvbi1iYXItb3duZXJzLWNhbmFkYS1jb3BhLWFtZXJpY2Ev0gFUaHR0cHM6Ly9lZG1vbnRvbi5jaXR5bmV3cy5jYS8yMDI0LzA3LzA3L2VkbW9udG9uLWJhci1vd25lcnMtY2FuYWRhLWNvcGEtYW1lcmljYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtdW5kb25lLWJ5LWFsdmFyZXotbWVzc2ktaW4taGFyZC1mb3VnaHQtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC12cy1hcmdlbnRpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>What to see and do on Canada Day 2024</t>
+          <t>Canada’s Alphonso Davies exits Copa America semifinal vs. Argentina</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.864712</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiPGh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vc2VlLWNhbmFkYS1kYXktMjAyNC0xNzEyNTYxMjQuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jYW5hZGFzLWFscGhvbnNvLWRhdmllcy1leGl0cy1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLXZzLWFyZ2VudGluYS_SAWlodHRwczovL3d3dy5zcG9ydHNuZXQuY2Evc29jY2VyL2NhbmFkYXMtYWxwaG9uc28tZGF2aWVzLWV4aXRzLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtdnMtYXJnZW50aW5hL3NuLWFtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Canada's Josh Naylor named to first All-Star Game</t>
+          <t>Messi scores first goal of Copa America against Canada</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.874467</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9tbGIvYXJ0aWNsZS9jYW5hZGFzLWpvc2gtbmF5bG9yLW5hbWVkLXRvLWZpcnN0LWFsbC1zdGFyLWdhbWUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvbGlvbmVsLW1lc3NpLXNjb3Jlcy1maXJzdC1nb2FsLW9mLWNvcGEtYW1lcmljYS1mb3ItYXJnZW50aW5hLWFnYWluc3QtY2FuYWRhLTEuMjE0NjUxNtIBcGh0dHBzOi8vd3d3LnRzbi5jYS9saW9uZWwtbWVzc2ktc2NvcmVzLWZpcnN0LWdvYWwtb2YtY29wYS1hbWVyaWNhLWZvci1hcmdlbnRpbmEtYWdhaW5zdC1jYW5hZGEtMS4yMTQ2NTE2P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Blustering winter storm continues for Atlantic Canada, next storm on its way</t>
+          <t>Lionel Messi scores goal, Argentina tops Canada to reach Copa America final</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.877058</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vY2EubmV3cy55YWhvby5jb20vaGVhdnktc25vdy13aW5kLXJhaW4tYmxhc3QtMTQ1NjQ4ODM3Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiAFodHRwczovL3d3dy51c2F0b2RheS5jb20vc3Rvcnkvc3BvcnRzL3NvY2Nlci8yMDI0LzA3LzA5L2FyZ2VudGluYS1jYW5hZGEtbGl2ZS1zY29yZS1oaWdobGlnaHRzLW1lc3NpLWNvcGEtYW1lcmljYS1zZW1pZmluYWwvNzQzMzc4NTMwMDcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Patriot Extends Vega Zone with Standout Intercepts including 9.7 m at 5.16% Li2O and 35.3 m at 2.40% Li2O</t>
+          <t>Canada falls to Argentina in Copa America semifinal</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.877425</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMinAFodHRwczovL3d3dy5uZXdzd2lyZS5jYS9uZXdzLXJlbGVhc2VzL3BhdHJpb3QtZXh0ZW5kcy12ZWdhLXpvbmUtd2l0aC1zdGFuZG91dC1pbnRlcmNlcHRzLWluY2x1ZGluZy05LTctbS1hdC01LTE2LWxpMm8tYW5kLTM1LTMtbS1hdC0yLTQwLWxpMm8tODg4MTQyNDY1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRhLWZhbGxzLXRvLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLTEuNjk1NzcxM9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Two Sask. women on roster for Canada's artistic swimming team at Paris Olympics</t>
+          <t>Argentina vs. Canada highlights: Messi and Álvarez goals send Argentina to the Copa América final</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.877425</t>
+          <t>2024-07-09 21:27:24.449599</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vdHdvLXNhc2std29tZW4tcm9zdGVyLWNhbmFkYXMtMjAxNTI0NjUyLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vbGl2ZS1ibG9nL3NvY2Nlci9hcmdlbnRpbmEtdnMtY2FuYWRhLWxpdmUtdXBkYXRlcy10b3AtbW9tZW50cy1mcm9tLWNvcGEtYW1lcmljYS1zZW1pZmluYWxz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Bonner hits career-high seven threes, scores 23 as Sun beat Dream</t>
+          <t>Canada loses to Argentina in Copa America semifinal, but the lessons have been golden</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.880334</t>
+          <t>2024-07-09 21:27:24.465540</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9kZXdhbm5hLWJvbm5lci1oaXRzLWNhcmVlci1oaWdoLXNldmVuLXRocmVlcy1zY29yZXMtMjMtYXMtY29ubmVjdGljdXQtc3VuLWJlYXQtYXRsYW50YS1kcmVhbS0xLjIxNDU3NzPSAYEBaHR0cHM6Ly93d3cudHNuLmNhL2Rld2FubmEtYm9ubmVyLWhpdHMtY2FyZWVyLWhpZ2gtc2V2ZW4tdGhyZWVzLXNjb3Jlcy0yMy1hcy1jb25uZWN0aWN1dC1zdW4tYmVhdC1hdGxhbnRhLWRyZWFtLTEuMjE0NTc3Mz90c24tYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMirAFodHRwczovL3d3dy50aGVzdGFyLmNvbS9zcG9ydHMvc29jY2VyL2NhbmFkYS1sb3Nlcy10by1hcmdlbnRpbmEtaW4tY29wYS1hbWVyaWNhLXNlbWlmaW5hbC1idXQtdGhlLWxlc3NvbnMtaGF2ZS1iZWVuLWdvbGRlbi9hcnRpY2xlX2ExZTAxMjRjLTNkZmYtMTFlZi04Y2UwLTQ3MWYxODY1MzRiNy5odG1s0gGwAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL3Nwb3J0cy9zb2NjZXIvY2FuYWRhLWxvc2VzLXRvLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLWJ1dC10aGUtbGVzc29ucy1oYXZlLWJlZW4tZ29sZGVuL2FydGljbGVfYTFlMDEyNGMtM2RmZi0xMWVmLThjZTAtNDcxZjE4NjUzNGI3LmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Trudeau to tell allies to stay resolute as Ukraine to at centre of NATO summit</t>
+          <t>Argentina vs. Canada Highlights | 2024 Copa América | Semifinals</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>2024-07-07 18:18:41.880334</t>
+          <t>2024-07-09 21:27:24.481180</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvdHJ1ZGVhdS10by10ZWxsLWFsbGllcy10by1zdGF5LXJlc29sdXRlLWFzLXVrcmFpbmUtdG8tYXQtY2VudHJlLW9mLW5hdG8tc3VtbWl0LTEuNjk1NDkwM9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLTY0eGF4NmE3bXpiOTNxOGzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Jocelyn Peterman - Team Canada - Official Olympic Team Website</t>
+          <t>Argentina 2-0 Canada (Jul 9, 2024) Game Analysis</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.827435</t>
+          <t>2024-07-09 22:26:45.075148</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMGh0dHBzOi8vb2x5bXBpYy5jYS90ZWFtLWNhbmFkYS9qb2NlbHluLXBldGVybWFuL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LmVzcG4uY29tL3NvY2Nlci9yZXBvcnQvXy9nYW1lSWQvNzAzOTUw0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Canada Industrial Relations Board deems port strike vote illegal</t>
+          <t>What's open and closed in Ottawa on Canada Day 2024</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.827435</t>
+          <t>2024-07-09 22:26:45.090846</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2JjLXBvcnQtbG9ja291dC1ub3RpY2UtMS43MjU2NzE20gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTY3MTY?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRWh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vd2hhdHMtb3Blbi1jbG9zZWQtY2FuYWRhLWRheS0wODAwMDA1MzEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Wings of Honour</t>
+          <t>‘Proud of this group’: Fans react to Canada’s historic run at Copa America</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.834503</t>
+          <t>2024-07-09 22:26:45.130208</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LmNwYWMuY2EvYXJ0aWNsZXMvZG9jcy93aW5ncy1vZi1ob25vdXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9wcm91ZC1vZi10aGlzLWdyb3VwLWZhbnMtcmVhY3QtdG8tY2FuYWRhcy1oaXN0b3JpYy1ydW4tYXQtY29wYS1hbWVyaWNhL9IBbmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvcHJvdWQtb2YtdGhpcy1ncm91cC1mYW5zLXJlYWN0LXRvLWNhbmFkYXMtaGlzdG9yaWMtcnVuLWF0LWNvcGEtYW1lcmljYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Alice Munro's daughter says her mom supported abusive stepfather</t>
+          <t>Copa América: Messi and Álvarez fire Argentina past Canada and into final</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.849194</t>
+          <t>2024-07-09 22:26:45.131608</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS90b3JvbnRvL2FsaWNlLW11bnJvLWRhdWdodGVyLXNleHVhbC1hYnVzZS0xLjcyNTY4MjnSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjgyOQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9hcnRpY2xlLzIwMjQvanVsLzA5L2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXNlbWktZmluYWwtbWF0Y2gtcmVwb3J0LXJlc3VsdNIBdWh0dHBzOi8vYW1wLnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9hcnRpY2xlLzIwMjQvanVsLzA5L2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXNlbWktZmluYWwtbWF0Y2gtcmVwb3J0LXJlc3VsdA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>B.C. longshore foreman strike averted after Industrial Relations Board steps in</t>
+          <t>At Copa America, Canada’s predictable defeat comes with the promise of something bigger</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.860352</t>
+          <t>2024-07-09 22:27:24.463530</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDcvYmMtZG9jay1zaGlwLWZvcmVtZW4tdW5pb24tc3RyaWtlL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL2FydGljbGUtY2FuYWRhLWFyZ2VudGluYS1jb3BhLWFtZXJpY2EtcmVzdWx0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Strike notice by B.C. ship and dock foremen contravenes the Canada Labour Code: CIRB</t>
+          <t>Regulatory framework of laboratory developed tests: Canada vs U.S.</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.864712</t>
+          <t>2024-07-09 23:26:45.075148</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vbmFuYWltb25ld3Nub3cuY29tLzIwMjQvMDcvMDcvc3RyaWtlLW5vdGljZS1ieS1iLWMtc2hpcC1hbmQtZG9jay1mb3JlbWVuLWNvbnRyYXZlbmVzLXRoZS1jYW5hZGEtbGFib3VyLWNvZGUtY2lyYi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmJsZy5jb20vZW4vaW5zaWdodHMvMjAyNC8wNy9yZWd1bGF0b3J5LWZyYW1ld29yay1vZi1sYWJvcmF0b3J5LWRldmVsb3BlZC10ZXN0cy1jYW5hZGEtdnMtdXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Nova Scotia’s Membertou First Nation and Indigenous Services Canada Announced Construction Projects That ...</t>
+          <t>Canada insurers investing in fossil fuels as climate risks grow, shareholder group says</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.880334</t>
+          <t>2024-07-09 23:26:45.090846</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiygFodHRwczovL2dldGZlYS5jb20vZW5naW5lZXJlZC13b29kLXByb2R1Y3RzLW1hc3MtdGltYmVyL25vdmEtc2NvdGlhcy1tZW1iZXJ0b3UtZmlyc3QtbmF0aW9uLWFuZC1pbmRpZ2Vub3VzLXNlcnZpY2VzLWNhbmFkYS1hbm5vdW5jZWQtY29uc3RydWN0aW9uLXByb2plY3RzLXRoYXQtaW5jbHVkZXMtYS1uZXctbWFzcy10aW1iZXItb2ZmaWNlLWJ1aWxkaW5n0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vY2EuZmluYW5jZS55YWhvby5jb20vbmV3cy9jYW5hZGEtaW5zdXJlcnMtaW52ZXN0aW5nLWZvc3NpbC1mdWVscy0wNDA5MzY4ODIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Canada Day fireworks petition aims to bring show back to Calgary</t>
+          <t>Heat wave bakes Texas amid power outages while Canada braces for wildfires</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>2024-07-07 19:18:41.884388</t>
+          <t>2024-07-09 23:26:45.130208</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijgFodHRwczovL2NhbGdhcnkuY3R2bmV3cy5jYS9tb2JpbGUvcHJvdGVzdC1vdmVyLWxvc3Mtb2YtbGFyZ2Utc2NhbGUtY2FuYWRhLWRheS1maXJld29ya3Mtc2hvdy1pbi1jYWxnYXJ5LWdyb3dzLTEuNjQwOTk5Nj9jYWNoZT15P2NsaXBJZD0xOTIxNzQ30gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy50aGV3ZWF0aGVybmV0d29yay5jb20vZW4vbmV3cy93ZWF0aGVyL3NldmVyZS9oZWF0LXdhdmUtYmFrZXMtdGV4YXMtYW1pZC1wb3dlci1vdXRhZ2VzLXdoaWxlLWNhbmFkYS1icmFjZXMtZm9yLXdpbGRmaXJlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Argentina vs. Canada: How to watch, stream Copa América semifinal | MLSSoccer.com</t>
+          <t>Copa America Takeaways: Canada learns valuable lesson in loss to Argentina</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>2024-07-07 20:18:41.827435</t>
+          <t>2024-07-09 23:27:24.417838</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3Lm1sc3NvY2Nlci5jb20vbmV3cy9hcmdlbnRpbmEtdnMtY2FuYWRhLWhvdy10by13YXRjaC1zdHJlYW0tY29wYS1hbWVyaWNhLXNlbWlmaW5hbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1sZWFybnMtdmFsdWFibGUtbGVzc29uLWluLWxvc3MtdG8tYXJnZW50aW5hL9IBcWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtbGVhcm5zLXZhbHVhYmxlLWxlc3Nvbi1pbi1sb3NzLXRvLWFyZ2VudGluYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>The Amazing Race Canada to feature the Sunshine Coast next week</t>
+          <t>Lionel Messi scores, Argentina brushes aside Canada, waltzes into Copa América final</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>2024-07-07 20:18:41.844117</t>
+          <t>2024-07-09 23:27:24.426857</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnBycGVhay5jb20vbG9jYWwtbmV3cy90aGUtYW1hemluZy1yYWNlLWNhbmFkYS10by1mZWF0dXJlLXRoZS1zdW5zaGluZS1jb2FzdC1uZXh0LXdlZWstOTE3NzU1OdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMif2h0dHBzOi8vc3BvcnRzLnlhaG9vLmNvbS9saXZlL2xpb25lbC1tZXNzaS1zY29yZXMtYXJnZW50aW5hLWJydXNoZXMtYXNpZGUtY2FuYWRhLXdhbHR6ZXMtaW50by1jb3BhLWFtZXJpY2EtZmluYWwtMjMzODA1Njk1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Canada urges dual citizens to leave Lebanon. Lebanese Montrealers say it's not that easy</t>
+          <t>Canada manager Jesse Marsch postgame presser after loss to Argentina in Copa América</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>2024-07-07 20:18:41.860352</t>
+          <t>2024-07-09 23:27:24.433908</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vY2FuYWRhLXVyZ2VzLWR1YWwtY2l0aXplbnMtbGVhdmUtMDgwMDAwMDU5Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLWJ0YjhhZG44ZzhwdWN0NjjSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Move over Prairies; Ontario is now Canada's tornado 'hotspot'</t>
+          <t>Canada’s discourse on finfish aquaculture is environmental extremism at its finest</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>2024-07-07 20:18:41.869285</t>
+          <t>2024-07-10 00:26:45.090846</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vY2EubmV3cy55YWhvby5jb20vbW92ZS1vdmVyLXByYWlyaWVzLW9udGFyaW8tbm93LTE2NDkzMzkxNy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMTAvY2FuYWRhcy1kaXNjb3Vyc2Utb24tZmluZmlzaC1hcXVhY3VsdHVyZS1pcy1lbnZpcm9ubWVudGFsLWV4dHJlbWlzbS1hdC1pdHMtZmluZXN0LzQyNzY4OS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Canada police charge woman with terrorism offenses two years after return</t>
+          <t>Opinion: Diversity trends, actions and results</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>2024-07-07 20:18:41.869285</t>
+          <t>2024-07-10 00:26:45.090846</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vd3d3Lmp1cmlzdC5vcmcvbmV3cy8yMDI0LzA3L2NhbmFkYS1wb2xpY2UtY2hhcmdlLXdvbWFuLXdpdGgtdGVycm9yaXNtLW9mZmVuc2VzLXR3by15ZWFycy1hZnRlci1yZXR1cm4v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LnB1bHBhbmRwYXBlcmNhbmFkYS5jb20vb3Bpbmlvbi1kaXZlcnNpdHktdHJlbmRzLWFjdGlvbnMtYW5kLXJlc3VsdHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Local athletes on Sask Volleyball roster for Canada Cup</t>
+          <t>Feds need to be accountable as Canadian diplomats’ health-care woes persist: union head</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>2024-07-07 20:18:41.884388</t>
+          <t>2024-07-10 00:26:45.106418</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3LnNhc2t0b2RheS5jYS9ub3J0aC9iYXR0bGVmb3Jkcy1uZXdzLW9wdGltaXN0L2xvY2FsLWF0aGxldGVzLW9uLXNhc2stdm9sbGV5YmFsbC1yb3N0ZXItZm9yLWNhbmFkYS1jdXAtOTE4NzM4MtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMTAvZmVkcy1uZWVkLXRvLXRha2UtYWNjb3VudGFiaWxpdHktYXMtY2FuYWRpYW4tZGlwbG9tYXRzLWhlYWx0aC1jYXJlLXdvZXMtcGVyc2lzdC11bmlvbi1oZWFkLzQyNzcwMy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Canada projected roster for 2025 NHL 4 Nations Face-Off</t>
+          <t>Messi's 109th goal leads defending champion Argentina over Canada 2-0 and into Copa America final</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>2024-07-07 21:18:41.827435</t>
+          <t>2024-07-10 00:27:24.426857</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3d3Lm5obC5jb20vbmV3cy80LW5hdGlvbnMtZmFjZS1vZmYtcHJvamVjdGVkLXJvc3Rlci1jYW5hZGHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYXBuZXdzLmNvbS9hcnRpY2xlL2NvcGEtYW1lcmljYS1tZXNzaS1jYW5hZGEtYXJnZW50aW5hLXNjb3JlLTQ4YWI4NjllODlmYWJjNzUyMGU3ZjZiMDdjYzRjMmQz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Women making an impact on Canadian Football League sidelines</t>
+          <t>The National | Canada’s historic Copa semifinal showdown</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>2024-07-07 21:18:41.844117</t>
+          <t>2024-07-10 00:27:24.433908</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS92aWRlby8xMDYwOTc2OS93b21lbi1tYWtpbmctYW4taW1wYWN0LW9uLWNhbmFkaWFuLWZvb3RiYWxsLWxlYWd1ZS1zaWRlbGluZXMv0gFmaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL3ZpZGVvLzEwNjA5NzY5L3dvbWVuLW1ha2luZy1hbi1pbXBhY3Qtb24tY2FuYWRpYW4tZm9vdGJhbGwtbGVhZ3VlLXNpZGVsaW5lcy9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjQyMzYxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Extreme heat becoming the usual for summer in Western Canada</t>
+          <t>Closing the gap</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>2024-07-07 21:18:41.876046</t>
+          <t>2024-07-10 00:27:24.461229</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vY2EubmV3cy55YWhvby5jb20vZXh0cmVtZS1oZWF0LWJlY29taW5nLXVzdWFsLXN1bW1lci0wMTUyNTQ4ODIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8va3BtZy5jb20vY2EvZW4vaG9tZS9pbnNpZ2h0cy8yMDI0LzA3L2Nsb3NpbmctdGhlLWdhcC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Team Canada wins 2024 Canada Cup gold medal-final in South Surrey</t>
+          <t>CTV National News: Sweltering heat in Canada</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>2024-07-07 22:18:41.839124</t>
+          <t>2024-07-10 01:26:45.106418</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LnN1cnJleW5vd2xlYWRlci5jb20vaG9tZS90ZWFtLWNhbmFkYS10YWtlcy1vbi1jb2xvcmFkby1vci1tZXhpY28taW4tY2FuYWRhLWN1cC1maW5hbC03NDMwODY40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vYXRsYW50aWMuY3R2bmV3cy5jYS92aWRlby9jMjk1NTc0My1jdHYtbmF0aW9uYWwtbmV3cy0tc3dlbHRlcmluZy1oZWF0LWluLWNhbmFkYT9wbGF5bGlzdElkPTEuNjk1Mzk3N9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Canada - Tax Authorities - Canada Enacts Digital Services Tax And Other Significant Tax Measures</t>
+          <t>FSC Canada approves updated Group Chain of Custody criteria</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>2024-07-07 22:18:41.849194</t>
+          <t>2024-07-10 01:26:45.106418</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3Lm1vbmRhcS5jb20vY2FuYWRhL3RheC1hdXRob3JpdGllcy8xNDg5MzMyL2NhbmFkYS1lbmFjdHMtZGlnaXRhbC1zZXJ2aWNlcy10YXgtYW5kLW90aGVyLXNpZ25pZmljYW50LXRheC1tZWFzdXJlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LnB1bHBhbmRwYXBlcmNhbmFkYS5jb20vZnNjLWNhbmFkYS1hcHByb3Zlcy11cGRhdGVkLWdyb3VwLWNoYWluLW9mLWN1c3RvZHktY3JpdGVyaWEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Picture-perfect places to visit in Canada</t>
+          <t>CTV National News: De Rosario on Canada's run</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>2024-07-07 22:18:41.869285</t>
+          <t>2024-07-10 01:26:45.131608</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vdGltZXNvZmluZGlhLmluZGlhdGltZXMuY29tL3RyYXZlbC93ZWItc3Rvcmllcy9waWN0dXJlLXBlcmZlY3QtcGxhY2VzLXRvLXZpc2l0LWluLWNhbmFkYS9waG90b3N0b3J5LzExMTU1OTc2NS5jbXPSAXlodHRwczovL3RpbWVzb2ZpbmRpYS5pbmRpYXRpbWVzLmNvbS90cmF2ZWwvd2ViLXN0b3JpZXMvcGljdHVyZS1wZXJmZWN0LXBsYWNlcy10by12aXNpdC1pbi1jYW5hZGEvcGhvdG9zdG9yeS8xMTE1NTk3NjUuY21z?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY3R2bmV3cy5jYS92aWRlby9jMjk1NTc0MC1jdHYtbmF0aW9uYWwtbmV3cy0tZGUtcm9zYXJpby1vbi1jYW5hZGEtcy1ydW7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>South American sides dominate for Day 4 women's play</t>
+          <t>What is teqball?</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>2024-07-07 22:18:41.878146</t>
+          <t>2024-07-10 01:27:24.433908</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3LmZpaC5ob2NrZXkvZXZlbnRzL2p1bmlvci1wYW4tYW1lcmljYW4tY2hhbXBpb25zaGlwLTIwMjQvbmV3cy9zb3V0aC1hbWVyaWNhbi1zaWRlcy1kb21pbmF0ZS1mb3ItZGF5LTQtd29tZW5zLXBsYXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDI1MjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Canada looking to 'stay fresh' ahead of a sharp training session on Monday - Video</t>
+          <t>Canada's Copa América success lays groundwork for World Cup: "The goal is 2026"</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>2024-07-07 22:18:41.880334</t>
+          <t>2024-07-10 01:27:24.465540</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnRzbi5jYS92aWRlby9jYW5hZGEtbG9va2luZy10by1zdGF5LWZyZXNoLWFoZWFkLW9mLWEtc2hhcnAtdHJhaW5pbmctc2Vzc2lvbi1vbi1tb25kYXl-Mjk1Mzk5ONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3Lm1sc3NvY2Nlci5jb20vbmV3cy9jYW5hZGEtcy1jb3BhLWFtZXJpY2Etc3VjY2Vzcy1sYXlzLWdyb3VuZHdvcmstZm9yLXdvcmxkLWN1cC10aGUtZ29hbC1pcy0yMDI20gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Canada's Pursuit Of Olympic Glory To Be Tested By 'Group Of Death'</t>
+          <t>Zachary Patterson: Canada must reclaim its wayward universities. Here’s how</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>2024-07-07 23:18:41.827435</t>
+          <t>2024-07-10 02:27:24.433908</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvZXNmYW5kaWFyYmFyYWhlbmkvMjAyNC8wNy8wOC9jYW5hZGFzLXB1cnN1aXQtb2Ytb2x5bXBpYy1nbG9yeS10by1iZS10ZXN0ZWQtYnktZ3JvdXAtb2YtZGVhdGgv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>Extreme temperatures trigger heat warnings in Western Canada</t>
-        </is>
-      </c>
-      <c r="B197" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.839124</t>
-        </is>
-      </c>
-      <c r="C197" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDE4ODTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>Bluesfest Day 4: Maroon 5, Carly Rae Jepsen and Tyler Shaw toil in the heat</t>
-        </is>
-      </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.844117</t>
-        </is>
-      </c>
-      <c r="C198" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMicWh0dHBzOi8vb3R0YXdhY2l0aXplbi5jb20vZW50ZXJ0YWlubWVudC9ibHVlc2Zlc3QtZGF5LTQtbWFyb29uLTUtY2FybHktcmFlLWplcHNlbi1hbmQtdHlsZXItc2hhdy10b2lsLWluLXRoZS1oZWF00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>James Arthur Lumley</t>
-        </is>
-      </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.844117</t>
-        </is>
-      </c>
-      <c r="C199" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LnRoZWNhbmFkaWFuZW5jeWNsb3BlZGlhLmNhL2VuL2FydGljbGUvbXBzYi1qYW1lcy1hcnRodXItbHVtbGV50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>Where is the emphasis on soft power and cultural exports in Canada's Indo-Pacific Strategy?</t>
-        </is>
-      </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.860352</t>
-        </is>
-      </c>
-      <c r="C200" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vcGFuY291dmVyLmNhL3doZXJlLWlzLXRoZS1lbXBoYXNpcy1vbi1zb2Z0LXBvd2VyLWFuZC1jdWx0dXJhbC1leHBvcnRzLWluLWNhbmFkYXMtaW5kby1wYWNpZmljLXN0cmF0ZWd5L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>Adams Jr. throws four touchdown passes to lead Lions past Ticats</t>
-        </is>
-      </c>
-      <c r="B201" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.864411</t>
-        </is>
-      </c>
-      <c r="C201" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LnRzbi5jYS9jZmwvdmVybm9uLWFkYW1zLWpyLXRocm93cy1mb3VyLXRvdWNoZG93bi1wYXNzZXMtdG8tbGVhZC1iYy1saW9ucy1wYXN0LWhhbWlsdG9uLXRpZ2VyLWNhdHMtMS4yMTQ1ODE20gF7aHR0cHM6Ly93d3cudHNuLmNhL3Zlcm5vbi1hZGFtcy1qci10aHJvd3MtZm91ci10b3VjaGRvd24tcGFzc2VzLXRvLWxlYWQtYmMtbGlvbnMtcGFzdC1oYW1pbHRvbi10aWdlci1jYXRzLTEuMjE0NTgxNj90c24tYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>Britain’s Right Is Following a Canadian Playbook</t>
-        </is>
-      </c>
-      <c r="B202" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.869285</t>
-        </is>
-      </c>
-      <c r="C202" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vdGhldHllZS5jYS9PcGluaW9uLzIwMjQvMDcvMDgvQnJpdGFpbi1SaWdodC1Gb2xsb3dpbmctQ2FuYWRpYW4tUGxheWJvb2sv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>Foremen at BC Port Give DP World Canada 72-Hour Strike Notice</t>
-        </is>
-      </c>
-      <c r="B203" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.878146</t>
-        </is>
-      </c>
-      <c r="C203" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMibWh0dHBzOi8vd3d3LnN1cHBseWNoYWluYnJhaW4uY29tL2FydGljbGVzLzM5OTkzLWZvcmVtZW4tYXQtYmMtcG9ydC1naXZlLWRwLXdvcmxkLWNhbmFkYS03Mi1ob3VyLXN0cmlrZS1ub3RpY2XSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>Canada - Distracting preschoolers with devices could cause trouble down the road, study suggests</t>
-        </is>
-      </c>
-      <c r="B204" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.889468</t>
-        </is>
-      </c>
-      <c r="C204" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMioQFodHRwczovL2VkdWNhdGlvbm5ld3NjYW5hZGEuY29tL2FydGljbGUvZWR1Y2F0aW9uL2xldmVsL2sxMi8zLzEwOTIyNDUvZGlzdHJhY3RpbmctcHJlc2Nob29sZXJzLXdpdGgtZGV2aWNlcy1jb3VsZC1jYXVzZS10cm91YmxlLWRvd24tdGhlLXJvYWQtc3R1ZHktc3VnZ2VzdHMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>INC gives assistance to Indigenous community in Calgary, Alberta, Canada</t>
-        </is>
-      </c>
-      <c r="B205" t="inlineStr">
-        <is>
-          <t>2024-07-07 23:18:41.894529</t>
-        </is>
-      </c>
-      <c r="C205" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMidmh0dHA6Ly93d3cuYWJubmV3c3dpcmUubmV0L3ByZXNzL2VuLzEyNjQxMS9JTkMtZ2l2ZXMtYXNzaXN0YW5jZS10by1JbmRpZ2Vub3VzLWNvbW11bml0eS1pbi1DYWxnYXJ5LUFsYmVydGEtQ2FuYWRhLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>If only our leaders would focus on what binds us, Canada has so much to offer: Ottawa reader</t>
-        </is>
-      </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>2024-07-08 00:18:41.827435</t>
-        </is>
-      </c>
-      <c r="C206" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LmhpbGx0aW1lcy5jb20vc3RvcnkvMjAyNC8wNy8wOC9pZi1vbmx5LW91ci1sZWFkZXJzLXdvdWxkLWZvY3VzLW9uLXdoYXQtYmluZHMtdXMtdG9nZXRoZXItb3R0YXdhLXJlYWRlci80MjcxMzAv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>Canada 'catching up' with NATO allies by bolstering air defence systems since 'wake-up call' in Ukraine, experts say</t>
-        </is>
-      </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>2024-07-08 00:18:41.839124</t>
-        </is>
-      </c>
-      <c r="C207" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiogFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMDgvY2FuYWRhLWNhdGNoaW5nLXVwLXdpdGgtbmF0by1hbGxpZXMtYnktYm9sc3RlcmluZy1haXItZGVmZW5jZS1zeXN0ZW1zLXNpbmNlLXdha2UtdXAtY2FsbC1pbi11a3JhaW5lLWV4cGVydHMtc2F5LzQyNzI2OS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>The National | France rejects far right</t>
-        </is>
-      </c>
-      <c r="B208" t="inlineStr">
-        <is>
-          <t>2024-07-08 00:18:41.849194</t>
-        </is>
-      </c>
-      <c r="C208" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjQyMzYxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>Affordable housing: Atlantic Canada to receive $98.7M | CTV News</t>
-        </is>
-      </c>
-      <c r="B209" t="inlineStr">
-        <is>
-          <t>2024-07-08 00:18:41.859411</t>
-        </is>
-      </c>
-      <c r="C209" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMifmh0dHBzOi8vYXRsYW50aWMuY3R2bmV3cy5jYS9hdGxhbnRpYy1jYW5hZGEtdG8tcmVjZWl2ZS05OC03LW0tZnJvbS1mb3ItYWZmb3JkYWJsZS1ob3VzaW5nLTEuNjkyNzUzNj9jYWNoZT15JTNGY2xpcElkJTNEMTkzMDExM9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>Three new books to keep an eye out for this fall</t>
-        </is>
-      </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>2024-07-08 00:18:41.874467</t>
-        </is>
-      </c>
-      <c r="C210" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3LmhpbGx0aW1lcy5jb20vc3RvcnkvMjAyNC8wNy8wOC90aHJlZS1uZXctYm9va3MtdG8ta2VlcC1hbi1leWUtb3V0LWZvci10aGlzLWZhbGwvNDI2NzI2L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>Malaysia's Petronas adds three new LNG vessels ahead of LNG Canada start-up</t>
-        </is>
-      </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>2024-07-08 00:18:41.880334</t>
-        </is>
-      </c>
-      <c r="C211" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3Lm5hdHVyYWxnYXN3b3JsZC5jb20vbWFsYXlzaWFzLXBldHJvbmFzLWluZHVjdHMtdGhyZWUtbmV3LWxuZy12ZXNzZWxzLWFoZWFkLW9mLWxuZy1jYW5hZGEtc3RhcnQtdXAtMTEyMDMw0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>Olympics-Team Canada goes for cool factor in Paris Games kit</t>
-        </is>
-      </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.834503</t>
-        </is>
-      </c>
-      <c r="C212" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vY2EubmV3cy55YWhvby5jb20vb2x5bXBpY3MtdGVhbS1jYW5hZGEtZ29lcy1jb29sLTIyMDg1OTQxOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>Bumpy road ahead for CUSMA negotiations</t>
-        </is>
-      </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.844117</t>
-        </is>
-      </c>
-      <c r="C213" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmhpbGx0aW1lcy5jb20vc3RvcnkvMjAyNC8wNy8wOC9idW1weS1yb2FkLWFoZWFkLWZvci1jdXNtYS1uZWdvdGlhdGlvbnMvNDI3MzgzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
-        <is>
-          <t>Cold Lake council raises concerns over Canada Community Building Fund delays</t>
-        </is>
-      </c>
-      <c r="B214" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.849194</t>
-        </is>
-      </c>
-      <c r="C214" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vY29sZC1sYWtlLWNvdW5jaWwtcmFpc2VzLWNvbmNlcm5zLTE2MDUxNjc0Mi5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t>Here are the Hot-Button Issues up for Discussion at the Seeds Canada Meeting in Edmonton This Week</t>
-        </is>
-      </c>
-      <c r="B215" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.849194</t>
-        </is>
-      </c>
-      <c r="C215" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMimAFodHRwczovL3d3dy5zZWVkd29ybGQuY29tL2NhbmFkYS9uZXdzLWNhbi8yMDI0LzA3LzA3L2hlcmUtYXJlLXRoZS1ob3QtYnV0dG9uLWlzc3Vlcy11cC1mb3ItZGlzY3Vzc2lvbi1hdC10aGUtc2VlZHMtY2FuYWRhLW1lZXRpbmctaW4tZWRtb250b24tdGhpcy13ZWVrL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t>Canada invests $120m in chips</t>
-        </is>
-      </c>
-      <c r="B216" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.860352</t>
-        </is>
-      </c>
-      <c r="C216" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmVsZWN0cm9uaWNzd2Vla2x5LmNvbS9uZXdzL2J1c2luZXNzL2NhbmFkYS1pbnZlc3RzLTEyMG0taW4tY2hpcHMtMjAyNC0wNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>Is Canada already below the net-zero level of carbon emissions due to its vast forest cover?</t>
-        </is>
-      </c>
-      <c r="B217" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.884388</t>
-        </is>
-      </c>
-      <c r="C217" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMihwFodHRwczovL3NyaWxhbmthLmZhY3RjcmVzY2VuZG8uY29tL2VuZ2xpc2gvaXMtY2FuYWRhLWFscmVhZHktYmVsb3ctdGhlLW5ldC16ZXJvLWxldmVsLW9mLWNhcmJvbi1lbWlzc2lvbnMtZHVlLXRvLWl0cy12YXN0LWZvcmVzdC1jb3Zlci_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t>Canada's Stephen Eustaquio finds purpose in Copa America after his parents' tragic deaths</t>
-        </is>
-      </c>
-      <c r="B218" t="inlineStr">
-        <is>
-          <t>2024-07-08 01:18:41.884388</t>
-        </is>
-      </c>
-      <c r="C218" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3Lm55dGltZXMuY29tL2F0aGxldGljLzU2MjI0NDAvMjAyNC8wNy8wOC9jYW5hZGEtc3RlcGhlbi1ldXN0YXF1aW8tY29wYS1hbWVyaWNhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>Canada's Andre De Grasse finishes 3rd in 100m at World Athletics Continental Tour Hengelo</t>
-        </is>
-      </c>
-      <c r="B219" t="inlineStr">
-        <is>
-          <t>2024-07-08 02:18:41.844117</t>
-        </is>
-      </c>
-      <c r="C219" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDE4MDXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="inlineStr">
-        <is>
-          <t>Canada unveils US$88.2 billion semiconductor funding</t>
-        </is>
-      </c>
-      <c r="B220" t="inlineStr">
-        <is>
-          <t>2024-07-08 02:18:41.864712</t>
-        </is>
-      </c>
-      <c r="C220" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vd3d3LmRpZ2l0aW1lcy5jb20vbmV3cy9hMjAyNDA3MDhQRDIwOS9ibG9vbWJlcmctY2FuYWRhLWZ1bmRpbmctZ292ZXJubWVudC1pbnZlc3RtZW50Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
-        </is>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
-        <is>
-          <t>Malaysia's Petronas adds new vessels to its fleet as LNG Canada launch nears</t>
-        </is>
-      </c>
-      <c r="B221" t="inlineStr">
-        <is>
-          <t>2024-07-08 02:18:41.889468</t>
-        </is>
-      </c>
-      <c r="C221" t="inlineStr">
-        <is>
-          <t>news.google.com/articles/CBMicWh0dHBzOi8vbG5ncHJpbWUuY29tL2FtZXJpY2FzL21hbGF5c2lhcy1wZXRyb25hcy1hZGRzLW5ldy12ZXNzZWxzLXRvLWl0cy1mbGVldC1hcy1sbmctY2FuYWRhLWxhdW5jaC1uZWFycy8xMTY2MjMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vdGhlaHViLmNhLzIwMjQvMDcvMTAvemFjaGFyeS1wYXR0ZXJzb24tY2FuYWRhLW11c3QtcmVjbGFpbS1pdHMtd2F5d2FyZC11bml2ZXJzaXRpZXMtaGVyZXMtaG93L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update app.py with demo
</commit_message>
<xml_diff>
--- a/canada_articles.xlsx
+++ b/canada_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C196"/>
+  <dimension ref="A1:C299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,7 +606,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Joint statement by Prime Minister Trudeau and President von der Leyen on the association of Canada to Horizon Europe</t>
+          <t>Here's how many medals Canada might win at the Olympics</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -616,14 +616,14 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3Mvc3RhdGVtZW50cy8yMDI0LzA3LzAzL2pvaW50LXN0YXRlbWVudC1wcmltZS1taW5pc3Rlci10cnVkZWF1LWFuZC1wcmVzaWRlbnQtdm9uLWRlci1sZXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvdGhlLWJ1enplci1uZXdzbGV0dGVyLWNhbmFkYS1tZWRhbC1wcmVkaWN0aW9uLW9seW1waWNzLTEuNzI1MzU2MdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzNTYx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cost of living has immigrants considering leaving Canada: poll</t>
+          <t>Lt.-Gen. Jennie Carignan named Canada's newest chief of the defence staff</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -633,14 +633,14 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDMvY29zdC1vZi1saXZpbmctY2FuYWRpYW4taW1taWdyYW50cy1sZWF2aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2plbm5pZS1jYXJpZ25hbi1uYW1lZC1jaGllZi1vZi10aGUtZGVmZW5jZS1zdGFmZi0xLjcyNTMyNTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1MzI1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lt.-Gen. Jennie Carignan will be Canada’s 1st female defence chief</t>
+          <t>Cost of living has immigrants considering leaving Canada: poll</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -650,14 +650,14 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjAxNjUyL2plbm5pZS1jYXJpZ25hbi1uZXctY2hpZWYtb2YtZGVmZW5jZS1jYW5hZGEv0gFUaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDE2NTIvamVubmllLWNhcmlnbmFuLW5ldy1jaGllZi1vZi1kZWZlbmNlLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDMvY29zdC1vZi1saXZpbmctY2FuYWRpYW4taW1taWdyYW50cy1sZWF2aW5nL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Lt.-Gen. Jennie Carignan named Canada's newest chief of the defence staff</t>
+          <t>Joint statement by Prime Minister Trudeau and President von der Leyen on the association of Canada to Horizon Europe</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -667,14 +667,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2plbm5pZS1jYXJpZ25hbi1uYW1lZC1jaGllZi1vZi10aGUtZGVmZW5jZS1zdGFmZi0xLjcyNTMyNTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1MzI1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnBtLmdjLmNhL2VuL25ld3Mvc3RhdGVtZW50cy8yMDI0LzA3LzAzL2pvaW50LXN0YXRlbWVudC1wcmltZS1taW5pc3Rlci10cnVkZWF1LWFuZC1wcmVzaWRlbnQtdm9uLWRlci1sZXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Here's how many medals Canada might win at the Olympics</t>
+          <t>Lt.-Gen. Jennie Carignan will be Canada’s 1st female defence chief</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvdGhlLWJ1enplci1uZXdzbGV0dGVyLWNhbmFkYS1tZWRhbC1wcmVkaWN0aW9uLW9seW1waWNzLTEuNzI1MzU2MdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzNTYx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjAxNjUyL2plbm5pZS1jYXJpZ25hbi1uZXctY2hpZWYtb2YtZGVmZW5jZS1jYW5hZGEv0gFUaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MDE2NTIvamVubmllLWNhcmlnbmFuLW5ldy1jaGllZi1vZi1kZWZlbmNlLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Proof point: Rental housing construction picks up in Canada but will it be enough?</t>
+          <t>MP Housefather denounces antisemitic poster telling him to 'get out of Canada'</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -735,14 +735,14 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3Rob3VnaHRsZWFkZXJzaGlwLnJiYy5jb20vcHJvb2YtcG9pbnQtcmVudGFsLWhvdXNpbmctY29uc3RydWN0aW9uLWlzLWZpbmFsbHktcGlja2luZy11cC1pbi1jYW5hZGEtYnV0LXdpbGwtaXQtYmUtZW5vdWdoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2hvdXNlZmF0aGVyLW1wLWFudGlzZW10aWMtcG9zdGVyLTEuNzI1MzAwNtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzMDA2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MP Housefather denounces antisemitic poster telling him to 'get out of Canada'</t>
+          <t>First-ever breaking athlete named to Canadian Olympic Team</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -752,14 +752,14 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2hvdXNlZmF0aGVyLW1wLWFudGlzZW10aWMtcG9zdGVyLTEuNzI1MzAwNtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjUzMDA2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy9maXJzdC1ldmVyLWJyZWFraW5nLWF0aGxldGUtbmFtZWQtdG8tY2FuYWRpYW4tb2x5bXBpYy10ZWFtL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>First-ever breaking athlete named to Canadian Olympic Team</t>
+          <t>Proof point: Rental housing construction picks up in Canada but will it be enough?</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy9maXJzdC1ldmVyLWJyZWFraW5nLWF0aGxldGUtbmFtZWQtdG8tY2FuYWRpYW4tb2x5bXBpYy10ZWFtL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3Rob3VnaHRsZWFkZXJzaGlwLnJiYy5jb20vcHJvb2YtcG9pbnQtcmVudGFsLWhvdXNpbmctY29uc3RydWN0aW9uLWlzLWZpbmFsbHktcGlja2luZy11cC1pbi1jYW5hZGEtYnV0LXdpbGwtaXQtYmUtZW5vdWdoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -793,7 +793,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Workers at Canada Border Services Agency ratify tentative agreement for more than 9,000 workers</t>
+          <t>Canada’s digital services tax is here. How could it affect you?</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcHNhY3VuaW9uLmNhL3dvcmtlcnMtY2FuYWRhLWJvcmRlci1zZXJ2aWNlcy1hZ2VuY3ktcmF0aWZ50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiOWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L9IBPWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Canada’s digital services tax is here. How could it affect you?</t>
+          <t>Workers at Canada Border Services Agency ratify tentative agreement for more than 9,000 workers</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiOWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L9IBPWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjA0OTEyL2RpZ2l0YWwtc2VydmljZXMtdGF4L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8vcHNhY3VuaW9uLmNhL3dvcmtlcnMtY2FuYWRhLWJvcmRlci1zZXJ2aWNlcy1hZ2VuY3ktcmF0aWZ50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Why Canada must act urgently to give undocumented migrants legal status</t>
+          <t>Permanent Residence in Canada is not guaranteed for international students</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -905,14 +905,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vdGhlY29udmVyc2F0aW9uLmNvbS93aHktY2FuYWRhLW11c3QtYWN0LXVyZ2VudGx5LXRvLWdpdmUtdW5kb2N1bWVudGVkLW1pZ3JhbnRzLWxlZ2FsLXN0YXR1cy0yMzI2ODbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmNpY25ld3MuY29tLzIwMjQvMDcvcGVybWFuZW50LXJlc2lkZW5jZS1pbi1jYW5hZGEtaXMtbm90LWd1YXJhbnRlZWQtZm9yLWludGVybmF0aW9uYWwtc3R1ZGVudHMtMDc0NDg1Ni5odG1s0gF7aHR0cHM6Ly93d3cuY2ljbmV3cy5jb20vMjAyNC8wNy9wZXJtYW5lbnQtcmVzaWRlbmNlLWluLWNhbmFkYS1pcy1ub3QtZ3VhcmFudGVlZC1mb3ItaW50ZXJuYXRpb25hbC1zdHVkZW50cy0wNzQ0ODU2Lmh0bWwvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Permanent Residence in Canada is not guaranteed for international students</t>
+          <t>Why Canada must act urgently to give undocumented migrants legal status</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -922,14 +922,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmNpY25ld3MuY29tLzIwMjQvMDcvcGVybWFuZW50LXJlc2lkZW5jZS1pbi1jYW5hZGEtaXMtbm90LWd1YXJhbnRlZWQtZm9yLWludGVybmF0aW9uYWwtc3R1ZGVudHMtMDc0NDg1Ni5odG1s0gF7aHR0cHM6Ly93d3cuY2ljbmV3cy5jb20vMjAyNC8wNy9wZXJtYW5lbnQtcmVzaWRlbmNlLWluLWNhbmFkYS1pcy1ub3QtZ3VhcmFudGVlZC1mb3ItaW50ZXJuYXRpb25hbC1zdHVkZW50cy0wNzQ0ODU2Lmh0bWwvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vdGhlY29udmVyc2F0aW9uLmNvbS93aHktY2FuYWRhLW11c3QtYWN0LXVyZ2VudGx5LXRvLWdpdmUtdW5kb2N1bWVudGVkLW1pZ3JhbnRzLWxlZ2FsLXN0YXR1cy0yMzI2ODbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Team Canada’s women’s water polo team seeks to make a splash at Paris 2024</t>
+          <t>Pro-Palestine protesters make pitch at disrupting Team Israel at Canada Cup women's softball tournament</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -939,14 +939,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA0L3RlYW0tY2FuYWRhcy13b21lbnMtd2F0ZXItcG9sby10ZWFtLXNlZWtzLXRvLW1ha2UtYS1zcGxhc2gtYXQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibWh0dHBzOi8vdGhlcHJvdmluY2UuY29tL3Nwb3J0cy9wcm8tcGFsZXN0aW5lLXByb3Rlc3RlcnMtZGlzcnVwdC10ZWFtLWlzcmFlbC1hdC1jYW5hZGEtY3VwLXNvZnRiYWxsLXRvdXJuYW1lbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Creating Online harms regulators expected to cost Canada $200 million: PBO</t>
+          <t>Liberal government enacts controversial digital services tax, raising trade concerns</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -956,14 +956,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY3JlYXRpbmctb25saW5lLWhhcm1zLXJlZ3VsYXRvcnMtZXhwZWN0ZWQtdG8tY29zdC1jYW5hZGEtMjAwLW1pbGxpb24tcGJvLTEuNjk1MTIyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2RpZ2l0YWwtc2VydmljZXMtdGF4LWltcGxlbWVudGVkLTEuNzI1NDM1NtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU0MzU2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Canada’s digital services tax enters into force</t>
+          <t>Canada's world junior team coming to Windsor for four days this month</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -973,14 +973,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWWh0dHBzOi8vd3d3Lm9zbGVyLmNvbS9lbi9pbnNpZ2h0cy91cGRhdGVzL2NhbmFkYXMtZGlnaXRhbC1zZXJ2aWNlcy10YXgtZW50ZXJzLWludG8tZm9yY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd2luZHNvcnN0YXIuY29tL3Nwb3J0cy9jYW5hZGFzLXdvcmxkLWp1bmlvci10ZWFtLWNvbWluZy10by13aW5kc29yLWZvci1mb3VyLWRheXMtdGhpcy1tb250aNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Liberal government enacts controversial digital services tax, raising trade concerns</t>
+          <t>Creating Online harms regulators expected to cost Canada $200 million: PBO</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -990,14 +990,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2RpZ2l0YWwtc2VydmljZXMtdGF4LWltcGxlbWVudGVkLTEuNzI1NDM1NtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU0MzU2?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY3JlYXRpbmctb25saW5lLWhhcm1zLXJlZ3VsYXRvcnMtZXhwZWN0ZWQtdG8tY29zdC1jYW5hZGEtMjAwLW1pbGxpb24tcGJvLTEuNjk1MTIyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Canada's world junior team coming to Windsor for four days this month</t>
+          <t>Team Canada’s women’s water polo team seeks to make a splash at Paris 2024</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1007,14 +1007,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd2luZHNvcnN0YXIuY29tL3Nwb3J0cy9jYW5hZGFzLXdvcmxkLWp1bmlvci10ZWFtLWNvbWluZy10by13aW5kc29yLWZvci1mb3VyLWRheXMtdGhpcy1tb250aNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA0L3RlYW0tY2FuYWRhcy13b21lbnMtd2F0ZXItcG9sby10ZWFtLXNlZWtzLXRvLW1ha2UtYS1zcGxhc2gtYXQtcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Pro-Palestine protesters make pitch at disrupting Team Israel at Canada Cup women's softball tournament</t>
+          <t>Canada’s digital services tax enters into force</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibWh0dHBzOi8vdGhlcHJvdmluY2UuY29tL3Nwb3J0cy9wcm8tcGFsZXN0aW5lLXByb3Rlc3RlcnMtZGlzcnVwdC10ZWFtLWlzcmFlbC1hdC1jYW5hZGEtY3VwLXNvZnRiYWxsLXRvdXJuYW1lbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vd3d3Lm9zbGVyLmNvbS9lbi9pbnNpZ2h0cy91cGRhdGVzL2NhbmFkYXMtZGlnaXRhbC1zZXJ2aWNlcy10YXgtZW50ZXJzLWludG8tZm9yY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Nutrition labelling: List of ingredients</t>
+          <t>Team Canada’s Athletics Squad Grows Ahead of Paris 2024</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1058,14 +1058,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9oZWFsdGgtY2FuYWRhL3NlcnZpY2VzL2Zvb2QtbnV0cml0aW9uL251dHJpdGlvbi1sYWJlbGxpbmcvaW5ncmVkaWVudC1saXN0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vYXRobGV0aWNzLmNhL2Jsb2cvMjAyNC8wNy8wNS90ZWFtLWNhbmFkYXMtYXRobGV0aWNzLXNxdWFkLWdyb3dzLWFoZWFkLW9mLXBhcmlzLTIwMjQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Dressage and eventing athletes and horses named to Team Canada for Paris 2024</t>
+          <t>Canada beats Venezuela in penalty kicks, reaches semis in 1st Copa America</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1075,14 +1075,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA1L2RyZXNzYWdlLWFuZC1ldmVudGluZy1hdGhsZXRlcy1hbmQtaG9yc2VzLW5hbWVkLXRvLXRlYW0tY2FuYWRhLWZvci1wYXJpcy0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS12ZW5lenVlbGEtY29wYS1hbWVyaWNhLXJlY2FwLWp1bHktNS0xLjcyNTYyNTjSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjI1OA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Air Canada has new policy on sacred items in the cabin after incident with national chief's headdress</t>
+          <t>Team Canada’s Paris 2024 equestrian dressage and eventing teams unveiled</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1092,14 +1092,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2luZGlnZW5vdXMvYWlyLWNhbmFkYS1uZXctcG9saWN5LXNhY3JlZC1pdGVtcy0xLjcyNTYwNzHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjA3MQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1lcXVlc3RyaWFuLWRyZXNzYWdlLWFuZC1ldmVudGluZy10ZWFtcy11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Team Canada’s Athletics Squad Grows Ahead of Paris 2024</t>
+          <t>Canada semi-final bound after heart-stopping penalty shootout win over Venezuela in Copa América QF</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1109,14 +1109,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vYXRobGV0aWNzLmNhL2Jsb2cvMjAyNC8wNy8wNS90ZWFtLWNhbmFkYXMtYXRobGV0aWNzLXNxdWFkLWdyb3dzLWFoZWFkLW9mLXBhcmlzLTIwMjQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtYm91bmQtZm9yLXNlbWktZmluYWxzLWFmdGVyLXRocmlsbGluZy1wZW5hbHR5LXNob290b3V0LXdpbi1vdmVyLXZlbmV6dWVsYS1pbi1jb3BhLWFtZXJpY2EtcWbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Canada semi-final bound after heart-stopping penalty shootout win over Venezuela in Copa América QF</t>
+          <t>Nutrition labelling: List of ingredients</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1126,14 +1126,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtYm91bmQtZm9yLXNlbWktZmluYWxzLWFmdGVyLXRocmlsbGluZy1wZW5hbHR5LXNob290b3V0LXdpbi1vdmVyLXZlbmV6dWVsYS1pbi1jb3BhLWFtZXJpY2EtcWbSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9oZWFsdGgtY2FuYWRhL3NlcnZpY2VzL2Zvb2QtbnV0cml0aW9uL251dHJpdGlvbi1sYWJlbGxpbmcvaW5ncmVkaWVudC1saXN0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Canada beats Venezuela in penalty kicks, reaches semis in 1st Copa America</t>
+          <t>Air Canada has new policy on sacred items in the cabin after incident with national chief's headdress</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1143,14 +1143,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS12ZW5lenVlbGEtY29wYS1hbWVyaWNhLXJlY2FwLWp1bHktNS0xLjcyNTYyNTjSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjI1OA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2luZGlnZW5vdXMvYWlyLWNhbmFkYS1uZXctcG9saWN5LXNhY3JlZC1pdGVtcy0xLjcyNTYwNzHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjA3MQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Team Canada’s Paris 2024 equestrian dressage and eventing teams unveiled</t>
+          <t>Dressage and eventing athletes and horses named to Team Canada for Paris 2024</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1160,14 +1160,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1lcXVlc3RyaWFuLWRyZXNzYWdlLWFuZC1ldmVudGluZy10ZWFtcy11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA1L2RyZXNzYWdlLWFuZC1ldmVudGluZy1hdGhsZXRlcy1hbmQtaG9yc2VzLW5hbWVkLXRvLXRlYW0tY2FuYWRhLWZvci1wYXJpcy0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Canadian unemployment rate rose to 6.4% in June as jobs market stalls</t>
+          <t>A new U.K. government renews hopes for a free trade deal with Canada</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1177,14 +1177,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRpYW4tdW5lbXBsb3ltZW50LXJhdGUtcm9zZS10by02LTQtaW4tanVuZS1hcy1qb2JzLW1hcmtldC1zdGFsbHMtMS42OTUyNDkx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2xhYm91ci11ay1lbGVjdGlvbi1mcmVlLXRyYWRlLWNhbmFkYS0xLjcyNTU3NzPSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTc3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Canada beat Venezuela on penalties to reach Copa America semifinals</t>
+          <t>Canada Soccer delivers new level of competition with PDP Championship</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1194,14 +1194,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL2NhbmFkYS1iZWF0LXZlbmV6dWVsYS1vbi1wZW5hbHRpZXMtdG8tcmVhY2gtY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMtMS42OTUzMTk10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItZGVsaXZlcnMtbmV3LWxldmVsLW9mLWNvbXBldGl0aW9uLXdpdGgtcGRwLWNoYW1waW9uc2hpcC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>A new U.K. government renews hopes for a free trade deal with Canada</t>
+          <t>Canadian unemployment rate rose to 6.4% in June as jobs market stalls</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1211,14 +1211,14 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2xhYm91ci11ay1lbGVjdGlvbi1mcmVlLXRyYWRlLWNhbmFkYS0xLjcyNTU3NzPSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NTc3Mw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRpYW4tdW5lbXBsb3ltZW50LXJhdGUtcm9zZS10by02LTQtaW4tanVuZS1hcy1qb2JzLW1hcmtldC1zdGFsbHMtMS42OTUyNDkx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Canada Soccer delivers new level of competition with PDP Championship</t>
+          <t>Canada beat Venezuela on penalties to reach Copa America semifinals</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItZGVsaXZlcnMtbmV3LWxldmVsLW9mLWNvbXBldGl0aW9uLXdpdGgtcGRwLWNoYW1waW9uc2hpcC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL2NhbmFkYS1iZWF0LXZlbmV6dWVsYS1vbi1wZW5hbHRpZXMtdG8tcmVhY2gtY29wYS1hbWVyaWNhLXNlbWlmaW5hbHMtMS42OTUzMTk10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>In Canada for 7 years, family fights deportation to Nigeria</t>
+          <t>Canada captures four medals at World Cup Super Final in Hungary</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1483,14 +1483,14 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvZmFtaWx5LWZpZ2h0cy1kZXBvcnRhdGlvbi1uaWdlcmlhLTEuNzI1NTUzMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU1NTMy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA2L3RlYW0tY2FuYWRhLXdvcmxkLWN1cC1zdXBlcmZpbmFsLXBhcmlzLTIwMi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Young Scottish side shows its class in rugby win over Canadian men</t>
+          <t>Copa America Takeaways: Canada continues sensational run in its debut</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1500,14 +1500,14 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvcnVnYnkvc2NvdGxhbmQtY2FuYWRhLXJ1Z2J5LTEuNzI1NjUxMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU2NTEx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1jb250aW51ZXMtc2Vuc2F0aW9uYWwtcnVuLWluLWRlYnV0L9IBaGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtY29udGludWVzLXNlbnNhdGlvbmFsLXJ1bi1pbi1kZWJ1dC9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Copa America Takeaways: Canada continues sensational run in its debut</t>
+          <t>In Canada for 7 years, family fights deportation to Nigeria</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1517,14 +1517,14 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1jb250aW51ZXMtc2Vuc2F0aW9uYWwtcnVuLWluLWRlYnV0L9IBaGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtY29udGludWVzLXNlbnNhdGlvbmFsLXJ1bi1pbi1kZWJ1dC9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvZmFtaWx5LWZpZ2h0cy1kZXBvcnRhdGlvbi1uaWdlcmlhLTEuNzI1NTUzMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU1NTMy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Canada captures four medals at World Cup Super Final in Hungary</t>
+          <t>Young Scottish side shows its class in rugby win over Canadian men</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzA2L3RlYW0tY2FuYWRhLXdvcmxkLWN1cC1zdXBlcmZpbmFsLXBhcmlzLTIwMi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvcnVnYnkvc2NvdGxhbmQtY2FuYWRhLXJ1Z2J5LTEuNzI1NjUxMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU2NTEx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1609,34 +1609,34 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>U of T ranks 17th globally, first in Canada in U.S. News &amp; World Report university rankings</t>
+          <t>Immigration Updates for International Students - International Centre</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.426857</t>
+          <t>2024-07-08 12:19:55.928216</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LnV0b3JvbnRvLmNhL25ld3MvdS10LXJhbmtzLTE3dGgtZ2xvYmFsbHktZmlyc3QtY2FuYWRhLXVzLW5ld3Mtd29ybGQtcmVwb3J0LXVuaXZlcnNpdHktcmFua2luZ3PSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LmRhbC5jYS9jYW1wdXNfbGlmZS9pbnRlcm5hdGlvbmFsLWNlbnRyZS9pbW1pZ3JhdGlvbi11cGRhdGVzLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Inventories rebuilding fast in Canada’s largest housing markets</t>
+          <t>How Canada became a car theft capital of the world</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.426857</t>
+          <t>2024-07-08 12:19:55.928216</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vdGhvdWdodGxlYWRlcnNoaXAucmJjLmNvbS9pbnZlbnRvcmllcy1yZWJ1aWxkaW5nLWZhc3QtaW4tY2FuYWRhcy1sYXJnZXN0LWhvdXNpbmctbWFya2V0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy9hcnRpY2xlcy9jeTc5ZHEybjA5M2_SATJodHRwczovL3d3dy5iYmMuY29tL25ld3MvYXJ0aWNsZXMvY3k3OWRxMm4wOTNvLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.433908</t>
+          <t>2024-07-08 12:19:55.945371</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1660,17 +1660,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Canada can’t catch a break from the heat. Will it last all summer?</t>
+          <t>U of T ranks 17th globally, first in Canada in U.S. News &amp; World Report university rankings</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.433908</t>
+          <t>2024-07-08 12:19:55.945371</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwNjI3L2hlYXQtd2F2ZS1jYW5hZGEtaG90dGVzdC1qdW5lL9IBRmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwNjI3L2hlYXQtd2F2ZS1jYW5hZGEtaG90dGVzdC1qdW5lL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LnV0b3JvbnRvLmNhL25ld3MvdS10LXJhbmtzLTE3dGgtZ2xvYmFsbHktZmlyc3QtY2FuYWRhLXVzLW5ld3Mtd29ybGQtcmVwb3J0LXVuaXZlcnNpdHktcmFua2luZ3PSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.433908</t>
+          <t>2024-07-08 12:19:55.945371</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -1694,102 +1694,102 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>5 things to know as Canada meets Argentina in 'David vs. Goliath' Copa semifinal</t>
+          <t>Inventories rebuilding fast in Canada’s largest housing markets</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.433908</t>
+          <t>2024-07-08 12:19:55.945371</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzLzUtdGhpbmdzLXRvLWtub3ctYXMtY2FuYWRhLW1lZXRzLWFyZ2VudGluYS1pbi1kYXZpZC12cy1nb2xpYXRoLWNvcGEtc2VtaWZpbmFsLTEuNjk1NTY4NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vdGhvdWdodGxlYWRlcnNoaXAucmJjLmNvbS9pbnZlbnRvcmllcy1yZWJ1aWxkaW5nLWZhc3QtaW4tY2FuYWRhcy1sYXJnZXN0LWhvdXNpbmctbWFya2V0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Liberal government hopes changes to dental care program will increase uptake</t>
+          <t>Marsch says he 'feels home' with Canada after being overlooked by U.S. Soccer Federation</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.433908</t>
+          <t>2024-07-08 12:19:55.945371</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvbGliZXJhbC1nb3Zlcm5tZW50LWhvcGVzLWNoYW5nZXMtdG8tZGVudGFsLWNhcmUtcHJvZ3JhbS13aWxsLWluY3JlYXNlLXVwdGFrZS0xLjY5NTU0NznSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS1jb3BhLWFtZXJpY2EtamVzc2UtbWFyc2NoLWp1bHktOC0xLjcyNTc4NjbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1Nzg2Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Team Canada’s Paris 2024 men’s volleyball team unveiled</t>
+          <t>PREVIEW: Canada look to continue dream run at Copa América in semifinal rematch with Argentina</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.449599</t>
+          <t>2024-07-08 12:19:55.966502</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1tZW5zLXZvbGxleWJhbGwtdGVhbS11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijAFodHRwczovL2NhbnBsLmNhL2FydGljbGUvcHJldmlldy1jYW5hZGEtbG9va2luZy10by1jb250aW51ZS1kcmVhbS1ydW4tYXQtMjAyNC1jb3BhLWFtZXJpY2EtaW4tc2VtaWZpbmFsLXJlbWF0Y2gtd2l0aC1saW9uZWwtbWVzc2lzLWFyZ2VudGluYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>PREVIEW: Canada look to continue dream run at Copa América in semifinal rematch with Argentina</t>
+          <t>Liberal government hopes changes to dental care program will increase uptake</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.449599</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijAFodHRwczovL2NhbnBsLmNhL2FydGljbGUvcHJldmlldy1jYW5hZGEtbG9va2luZy10by1jb250aW51ZS1kcmVhbS1ydW4tYXQtMjAyNC1jb3BhLWFtZXJpY2EtaW4tc2VtaWZpbmFsLXJlbWF0Y2gtd2l0aC1saW9uZWwtbWVzc2lzLWFyZ2VudGluYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvbGliZXJhbC1nb3Zlcm5tZW50LWhvcGVzLWNoYW5nZXMtdG8tZGVudGFsLWNhcmUtcHJvZ3JhbS13aWxsLWluY3JlYXNlLXVwdGFrZS0xLjY5NTU0NznSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Silk, Great Value plant-based beverages recalled across Canada</t>
+          <t>Canada can’t catch a break from the heat. Will it last all summer?</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.449599</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtYmV2ZXJhZ2UtcmVjYWxsLTEuNzI1NzgyMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3ODIx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwNjI3L2hlYXQtd2F2ZS1jYW5hZGEtaG90dGVzdC1qdW5lL9IBRmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwNjI3L2hlYXQtd2F2ZS1jYW5hZGEtaG90dGVzdC1qdW5lL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Messi fit for Argentina's Copa America semifinal showdown with Canada</t>
+          <t>5 things to know as Canada meets Argentina in 'David vs. Goliath' Copa semifinal</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.449599</t>
+          <t>2024-07-08 15:27:24.433908</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2xpb25lbC1tZXNzaS1maXQtYXJnZW50aW5hLWNhbmFkYS1jb3BhLWFtZXJpY2EtanVseS04LTEuNzI1Nzc0MtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3NzQy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzLzUtdGhpbmdzLXRvLWtub3ctYXMtY2FuYWRhLW1lZXRzLWFyZ2VudGluYS1pbi1kYXZpZC12cy1nb2xpYXRoLWNvcGEtc2VtaWZpbmFsLTEuNjk1NTY4NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1813,75 +1813,75 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Opinion: Once the envy of the world, Canada’s immigration system now lies dismantled</t>
+          <t>Messi fit for Argentina's Copa America semifinal showdown with Canada</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.460215</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vYnVzaW5lc3MvY29tbWVudGFyeS9hcnRpY2xlLW9uY2UtdGhlLWVudnktb2YtdGhlLXdvcmxkLWNhbmFkYXMtaW1taWdyYXRpb24tc3lzdGVtLW5vdy1sYXlzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2xpb25lbC1tZXNzaS1maXQtYXJnZW50aW5hLWNhbmFkYS1jb3BhLWFtZXJpY2EtanVseS04LTEuNzI1Nzc0MtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3NzQy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Letters July 8: Canada is best country on Earth; lack of courteous driving; desperate housing strategy</t>
+          <t>Silk, Great Value plant-based beverages recalled across Canada</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.465540</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy50aW1lc2NvbG9uaXN0LmNvbS9vcGluaW9uL2xldHRlcnMtanVseS04LWNhbmFkYS1pcy1iZXN0LWNvdW50cnktb24tZWFydGgtbGFjay1vZi1jb3VydGVvdXMtZHJpdmluZy1kZXNwZXJhdGUtaG91c2luZy1zdHJhdGVneS05MTg4MDQ00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtYmV2ZXJhZ2UtcmVjYWxsLTEuNzI1NzgyMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3ODIx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Marsch says he 'feels home' with Canada after being overlooked by U.S. Soccer Federation</t>
+          <t>Team Canada’s Paris 2024 men’s volleyball team unveiled</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.465540</t>
+          <t>2024-07-08 15:27:24.449599</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS1jb3BhLWFtZXJpY2EtamVzc2UtbWFyc2NoLWp1bHktOC0xLjcyNTc4NjbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1Nzg2Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1tZW5zLXZvbGxleWJhbGwtdGVhbS11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>B.C. municipalities struggle with what to do with RV dwellers</t>
+          <t>Opinion: Once the envy of the world, Canada’s immigration system now lies dismantled</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.465540</t>
+          <t>2024-07-08 15:27:24.460215</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2xvbmctdGVybS1ydi1mdXR1cmUtMS43MjU2MTQ00gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTYxNDQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vYnVzaW5lc3MvY29tbWVudGFyeS9hcnRpY2xlLW9uY2UtdGhlLWVudnktb2YtdGhlLXdvcmxkLWNhbmFkYXMtaW1taWdyYXRpb24tc3lzdGVtLW5vdy1sYXlzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Canada Averts New Threat of Strikes at British Columbia Ports</t>
+          <t>Rival Watch: Is Canada earning respect ahead of Copa America semifinal vs. Argentina?</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1891,14 +1891,14 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lndzai5jb20vYXJ0aWNsZXMvY2FuYWRhLWF2ZXJ0cy1uZXctdGhyZWF0LW9mLXN0cmlrZXMtYXQtYnJpdGlzaC1jb2x1bWJpYS1wb3J0cy00NGI4MTJmZtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9yaXZhbC13YXRjaC1pcy1jYW5hZGEtZWFybmluZy1yZXNwZWN0LWFoZWFkLW9mLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtdnMtYXJnZW50aW5hL9IBemh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvcml2YWwtd2F0Y2gtaXMtY2FuYWRhLWVhcm5pbmctcmVzcGVjdC1haGVhZC1vZi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLXZzLWFyZ2VudGluYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Canada-Argentina headlines Copa, Euro semifinal action starting Tuesday on TSN</t>
+          <t>Monday Digest: Dabrowski Carries Canadian Hopes at Wimbledon</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -1908,14 +1908,14 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy50c24uY2Evc29jY2VyL2NhbmFkYS1hcmdlbnRpbmEtaGVhZGxpbmVzLWNvcGEtYW1lcmljYS11ZWZhLWV1cm8tMjAyNC1zZW1pZmluYWwtYWN0aW9uLXN0YXJ0aW5nLXR1ZXNkYXktb24tdHNuLTEuMjE0NTkyOdIBhAFodHRwczovL3d3dy50c24uY2EvY2FuYWRhLWFyZ2VudGluYS1oZWFkbGluZXMtY29wYS1hbWVyaWNhLXVlZmEtZXVyby0yMDI0LXNlbWlmaW5hbC1hY3Rpb24tc3RhcnRpbmctdHVlc2RheS1vbi10c24tMS4yMTQ1OTI5P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnRlbm5pc2NhbmFkYS5jb20vbmV3cy9tb25kYXktZGlnZXN0LWRhYnJvd3NraS1jYXJyaWVzLWNhbmFkaWFuLWhvcGVzLWF0LXdpbWJsZWRvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Monday Digest: Dabrowski Carries Canadian Hopes at Wimbledon</t>
+          <t>B.C. municipalities struggle with what to do with RV dwellers</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -1925,14 +1925,14 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LnRlbm5pc2NhbmFkYS5jb20vbmV3cy9tb25kYXktZGlnZXN0LWRhYnJvd3NraS1jYXJyaWVzLWNhbmFkaWFuLWhvcGVzLWF0LXdpbWJsZWRvbi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2xvbmctdGVybS1ydi1mdXR1cmUtMS43MjU2MTQ00gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTYxNDQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Trudeau heads for the hot seat at NATO summit as allies question Canada's defence commitments</t>
+          <t>Letters July 8: Canada is best country on Earth; lack of courteous driving; desperate housing strategy</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -1942,14 +1942,14 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL3RydWRlYXUtbmF0by1kZWZlbmNlLXNwZW5kaW5nLXN1bW1pdC0xLjcyNTYwMjfSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjAyNw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy50aW1lc2NvbG9uaXN0LmNvbS9vcGluaW9uL2xldHRlcnMtanVseS04LWNhbmFkYS1pcy1iZXN0LWNvdW50cnktb24tZWFydGgtbGFjay1vZi1jb3VydGVvdXMtZHJpdmluZy1kZXNwZXJhdGUtaG91c2luZy1zdHJhdGVneS05MTg4MDQ00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Rival Watch: Is Canada earning respect ahead of Copa America semifinal vs. Argentina?</t>
+          <t>Canada Averts New Threat of Strikes at British Columbia Ports</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -1959,48 +1959,48 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9yaXZhbC13YXRjaC1pcy1jYW5hZGEtZWFybmluZy1yZXNwZWN0LWFoZWFkLW9mLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtdnMtYXJnZW50aW5hL9IBemh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvcml2YWwtd2F0Y2gtaXMtY2FuYWRhLWVhcm5pbmctcmVzcGVjdC1haGVhZC1vZi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLXZzLWFyZ2VudGluYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3Lndzai5jb20vYXJ0aWNsZXMvY2FuYWRhLWF2ZXJ0cy1uZXctdGhyZWF0LW9mLXN0cmlrZXMtYXQtYnJpdGlzaC1jb2x1bWJpYS1wb3J0cy00NGI4MTJmZtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Theo Argitis: Carney speculation summer mirage for disgruntled corporate Canada</t>
+          <t>Trudeau heads for the hot seat at NATO summit as allies question Canada's defence commitments</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.481180</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9lY29ub215L21hcmstY2FybmV5LXNwZWN1bGF0aW9uLXN1bW1lci1taXJhZ2UtZm9yLWNvcnBvcmF0ZS1jYW5hZGHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL3RydWRlYXUtbmF0by1kZWZlbmNlLXNwZW5kaW5nLXN1bW1pdC0xLjcyNTYwMjfSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NjAyNw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Minister Joly to travel to the United Kingdom</t>
+          <t>Canada-Argentina headlines Copa, Euro semifinal action starting Tuesday on TSN</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2024-07-08 15:27:24.481180</t>
+          <t>2024-07-08 15:27:24.465540</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9nbG9iYWwtYWZmYWlycy9uZXdzLzIwMjQvMDcvbWluaXN0ZXItam9seS10by10cmF2ZWwtdG8tdGhlLXVuaXRlZC1raW5nZG9tLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy50c24uY2Evc29jY2VyL2NhbmFkYS1hcmdlbnRpbmEtaGVhZGxpbmVzLWNvcGEtYW1lcmljYS11ZWZhLWV1cm8tMjAyNC1zZW1pZmluYWwtYWN0aW9uLXN0YXJ0aW5nLXR1ZXNkYXktb24tdHNuLTEuMjE0NTkyOdIBhAFodHRwczovL3d3dy50c24uY2EvY2FuYWRhLWFyZ2VudGluYS1oZWFkbGluZXMtY29wYS1hbWVyaWNhLXVlZmEtZXVyby0yMDI0LXNlbWlmaW5hbC1hY3Rpb24tc3RhcnRpbmctdHVlc2RheS1vbi10c24tMS4yMTQ1OTI5P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Remnants of Hurricane Beryl could bring downpours to Ottawa-Gatineau</t>
+          <t>Unable to work in their official language of choice, some public servants are quitting — to Canada’s detriment</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2010,14 +2010,14 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvcmVtbmFudHMtb2YtaHVycmljYW5lLWJlcnlsLWNvdWxkLWJyaW5nLWRvd25wb3Vycy10by1vdHRhd2EtZ2F0aW5lYXUtMS43MjU3NjE10gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTc2MTU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vdW5hYmxlLXRvLXdvcmstaW4tdGhlaXItb2ZmaWNpYWwtbGFuZ3VhZ2Utb2YtY2hvaWNlLXNvbWUtcHVibGljLXNlcnZhbnRzLWFyZS1xdWl0dGluZy10by1jYW5hZGFzLWRldHJpbWVudC0yMzMxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>VIDA Launches $300M Fund to Combat Canada's Affordable Housing Crisis</t>
+          <t>Canada to Share Plan for Reaching NATO’s Spending Target, Defense Minister Says</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2027,14 +2027,14 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm5ld3N3aXJlLmNhL25ld3MtcmVsZWFzZXMvdmlkYS1sYXVuY2hlcy0zMDBtLWZ1bmQtdG8tY29tYmF0LWNhbmFkYS1zLWFmZm9yZGFibGUtaG91c2luZy1jcmlzaXMtODgzNDk1ODQ2Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigQFodHRwczovL3d3dy5ibG9vbWJlcmcuY29tL25ld3MvYXJ0aWNsZXMvMjAyNC0wNy0wOC9jYW5hZGEtdG8tc2hhcmUtcGxhbi1mb3ItcmVhY2hpbmctbmF0by1zLXNwZW5kaW5nLXRhcmdldC1kZWZlbnNlLW1pbmlzdGVyLXNheXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Canada to Share Plan for Reaching NATO’s Spending Target, Defense Minister Says</t>
+          <t>VIDA Launches $300M Fund to Combat Canada's Affordable Housing Crisis</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2044,14 +2044,14 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigQFodHRwczovL3d3dy5ibG9vbWJlcmcuY29tL25ld3MvYXJ0aWNsZXMvMjAyNC0wNy0wOC9jYW5hZGEtdG8tc2hhcmUtcGxhbi1mb3ItcmVhY2hpbmctbmF0by1zLXNwZW5kaW5nLXRhcmdldC1kZWZlbnNlLW1pbmlzdGVyLXNheXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3Lm5ld3N3aXJlLmNhL25ld3MtcmVsZWFzZXMvdmlkYS1sYXVuY2hlcy0zMDBtLWZ1bmQtdG8tY29tYmF0LWNhbmFkYS1zLWFmZm9yZGFibGUtaG91c2luZy1jcmlzaXMtODgzNDk1ODQ2Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Unable to work in their official language of choice, some public servants are quitting — to Canada’s detriment</t>
+          <t>Minister Joly to travel to the United Kingdom</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2061,14 +2061,14 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3RoZWNvbnZlcnNhdGlvbi5jb20vdW5hYmxlLXRvLXdvcmstaW4tdGhlaXItb2ZmaWNpYWwtbGFuZ3VhZ2Utb2YtY2hvaWNlLXNvbWUtcHVibGljLXNlcnZhbnRzLWFyZS1xdWl0dGluZy10by1jYW5hZGFzLWRldHJpbWVudC0yMzMxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9nbG9iYWwtYWZmYWlycy9uZXdzLzIwMjQvMDcvbWluaXN0ZXItam9seS10by10cmF2ZWwtdG8tdGhlLXVuaXRlZC1raW5nZG9tLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Canada's gold exports to China rise, shining through the trade tensions</t>
+          <t>Remnants of Hurricane Beryl could bring downpours to Ottawa-Gatineau</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2078,643 +2078,643 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vY29tbW9kaXRpZXMvbWluaW5nL2NhbmFkYS1nb2xkLWV4cG9ydHMtY2hpbmEtcmlzZS10cmFkZS10ZW5zaW9uc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvcmVtbmFudHMtb2YtaHVycmljYW5lLWJlcnlsLWNvdWxkLWJyaW5nLWRvd25wb3Vycy10by1vdHRhd2EtZ2F0aW5lYXUtMS43MjU3NjE10gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTc2MTU?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Standing Senate Committee on Agriculture and Forestry (44th Parliament, 1st Session)</t>
+          <t>Canada's gold exports to China rise, shining through the trade tensions</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2024-07-09 15:26:45.075148</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLGh0dHBzOi8vc2VuY2FuYWRhLmNhL2VuL2NvbW1pdHRlZXMvYWdmby80NC0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vY29tbW9kaXRpZXMvbWluaW5nL2NhbmFkYS1nb2xkLWV4cG9ydHMtY2hpbmEtcmlzZS10cmFkZS10ZW5zaW9uc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Copa America Preview: Messi, Argentina rematch stand between Canada and glory</t>
+          <t>Theo Argitis: Carney speculation summer mirage for disgruntled corporate Canada</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2024-07-09 15:26:45.106418</t>
+          <t>2024-07-08 15:27:24.481180</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdG9yb250by5jaXR5bmV3cy5jYS8yMDI0LzA3LzA5L2NhbmFkYS1jb3BhLWFtZXJpY2Etc2VtaS1maW5hbHMtYXJnZW50aW5hLW1hdGNoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9lY29ub215L21hcmstY2FybmV5LXNwZWN1bGF0aW9uLXN1bW1lci1taXJhZ2UtZm9yLWNvcnBvcmF0ZS1jYW5hZGHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Niagara Health is hiring!</t>
+          <t>News</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2024-07-09 15:26:45.106418</t>
+          <t>2024-07-09 12:19:55.895030</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiKWh0dHBzOi8vd3d3Lm5pYWdhcmFoZWFsdGgub24uY2Evc2l0ZS9ob21l0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiImh0dHBzOi8vd3d3LmNhbmFkYS5jYS9lbi9uZXdzLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Canada vs. Messi, Argentina - Transcript</t>
+          <t>Canada’s average rents just saw their biggest drop in 3 years</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2024-07-09 15:26:45.106418</t>
+          <t>2024-07-09 12:19:55.911666</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiU2h0dHBzOi8vd3d3LmNiYy5jYS9yYWRpby9mcm9udGJ1cm5lci9jYW5hZGEtdnMtbWVzc2ktYXJnZW50aW5hLXRyYW5zY3JpcHQtMS43MjU4NTI40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTg1Mjg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyODAwL3JlbnRhbC1tYXJrZXQtY2FuYWRhLXJlbnRzLWp1bmUtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Canada’s average rents just saw their biggest drop in 3 years</t>
+          <t>East Coast RV trip features family, food and a few bumps</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.426857</t>
+          <t>2024-07-09 12:19:55.911666</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyODAwL3JlbnRhbC1tYXJrZXQtY2FuYWRhLXJlbnRzLWp1bmUtMjAyNC_SAU1odHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYxMjgwMC9yZW50YWwtbWFya2V0LWNhbmFkYS1yZW50cy1qdW5lLTIwMjQvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vby5jYW5hZGEuY29tL3RyYXZlbC9lYXN0LWNvYXN0LXJ2LXRyaXAtZmVhdHVyZXMtZmFtaWx5LWZvb2QtYW5kLWEtZmV3LWJ1bXBz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>How Canada became a car theft capital of the world</t>
+          <t>Canada draws link between June heat wave and climate change with new attribution analysis</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.426857</t>
+          <t>2024-07-09 12:19:55.911666</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy9hcnRpY2xlcy9jeTc5ZHEybjA5M2_SATJodHRwczovL3d3dy5iYmMuY29tL25ld3MvYXJ0aWNsZXMvY3k3OWRxMm4wOTNvLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NsaW1hdGUvY2FuYWRhLWVjY2MtcmFwaWQtYXR0cmlidXRpb24taGVhdC0xLjcyNTc0NTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzQ1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Canada’s Men’s Rugby Team’s match day roster named ahead of match against Romania in Ottawa</t>
+          <t>Standing Senate Committee on Agriculture and Forestry (44th Parliament, 1st Session)</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.426857</t>
+          <t>2024-07-09 12:19:55.911666</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L2NhbmFkYS1zLW1lbi1zLXJ1Z2J5LXRlYW0tcy1tYXRjaC1kYXktcm9zdGVyLW5hbWVkLWFoZWFkLW9mLW1hdGNoLWFnYWluc3Qtcm9tYW5pYS1pbi1vdHRhd2HSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLGh0dHBzOi8vc2VuY2FuYWRhLmNhL2VuL2NvbW1pdHRlZXMvYWdmby80NC0x0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Canada ready for rematch with Messi, Argentina in Copa America semifinal on TSN</t>
+          <t>Canada urged to spend more on defence as NATO chief addresses summit</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.928216</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY2FuYWRhLXJlYWR5LWZvci1yZW1hdGNoLXdpdGgtbGlvbmVsLW1lc3NpLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLW9uLXRzbi0xLjIxNDYxNzHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNTYwL25hdG8tc3VtbWl0LWRlZmVuY2Utc3BlbmRpbmctY2FuYWRhL9IBTGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNTYwL25hdG8tc3VtbWl0LWRlZmVuY2Utc3BlbmRpbmctY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Nato allies pressure Canada to step up spending at Washington summit</t>
+          <t>Copa America Takeaways: Canada learns valuable lesson in loss to Argentina</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.928216</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy9hcnRpY2xlcy9jbDR5Z3psejRtem_SATJodHRwczovL3d3dy5iYmMuY29tL25ld3MvYXJ0aWNsZXMvY2w0eWd6bHo0bXpvLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1sZWFybnMtdmFsdWFibGUtbGVzc29uLWluLWxvc3MtdG8tYXJnZW50aW5hL9IBcWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtbGVhcm5zLXZhbHVhYmxlLWxlc3Nvbi1pbi1sb3NzLXRvLWFyZ2VudGluYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>TIFF announces five more World Premieres from Canada, France, India, UK, and USA</t>
+          <t>The philosophy — and politics — behind Canada's reluctance to meet NATO's spending target</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.928216</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vdGlmZi5uZXQvcHJlc3MvbmV3cy90aWZmLWFubm91bmNlcy1maXZlLW1vcmUtd29ybGQtcHJlbWllcmVzLWZyb20tY2FuYWRhLWZyYW5jZS1pbmRpYS11ay1hbmQtdXNh0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2NhbmFkYS1uYXRvLWpvbHktYmxhaXItdHJ1ZGVhdS1kZWZlbmNlLTEuNzI1NzczN9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3NzM3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Silk, Great Value plant-based milks recalled in Canada</t>
+          <t>Canada’s priorities at NATO summit take backseat to spending concerns</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.928216</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMjUwL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtbWlsay1yZWNhbGwtY2FuYWRhL9IBWGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMjUwL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtbWlsay1yZWNhbGwtY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwMzIzL2NhbmFkYS1uYXRvLXN1bW1pdC13YXNoaW5ndG9uLWRlZmVuY2Utc3BlbmRpbmcv0gFXaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTAzMjMvY2FuYWRhLW5hdG8tc3VtbWl0LXdhc2hpbmd0b24tZGVmZW5jZS1zcGVuZGluZy9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>The remnants of hurricane Beryl are heading to Canada. Here's where it's expected to land</t>
+          <t>Canada vs. Argentina: Your guide to historic Copa America semifinal showdown</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.944289</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy5jdHZuZXdzLmNhL2NsaW1hdGUtYW5kLWVudmlyb25tZW50L3RoZS1yZW1uYW50cy1vZi1odXJyaWNhbmUtYmVyeWwtYXJlLWhlYWRpbmctdG8tY2FuYWRhLWhlcmUtcy13aGVyZS1pdC1zLWV4cGVjdGVkLXRvLWxhbmQtMS42OTU2OTE40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjExMDA1L2NhbmFkYS1hcmdlbnRpbmEtY29wYS1hbWVyaWNhL9IBRmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjExMDA1L2NhbmFkYS1hcmdlbnRpbmEtY29wYS1hbWVyaWNhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Canada’s priorities at NATO summit take backseat to spending concerns</t>
+          <t>Canada loses to Argentina in Copa America semifinal, but the lessons have been golden</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.945371</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiU2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEwMzIzL2NhbmFkYS1uYXRvLXN1bW1pdC13YXNoaW5ndG9uLWRlZmVuY2Utc3BlbmRpbmcv0gFXaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTAzMjMvY2FuYWRhLW5hdG8tc3VtbWl0LXdhc2hpbmd0b24tZGVmZW5jZS1zcGVuZGluZy9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMirAFodHRwczovL3d3dy50aGVzdGFyLmNvbS9zcG9ydHMvc29jY2VyL2NhbmFkYS1sb3Nlcy10by1hcmdlbnRpbmEtaW4tY29wYS1hbWVyaWNhLXNlbWlmaW5hbC1idXQtdGhlLWxlc3NvbnMtaGF2ZS1iZWVuLWdvbGRlbi9hcnRpY2xlX2ExZTAxMjRjLTNkZmYtMTFlZi04Y2UwLTQ3MWYxODY1MzRiNy5odG1s0gGwAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL3Nwb3J0cy9zb2NjZXIvY2FuYWRhLWxvc2VzLXRvLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLWJ1dC10aGUtbGVzc29ucy1oYXZlLWJlZW4tZ29sZGVuL2FydGljbGVfYTFlMDEyNGMtM2RmZi0xMWVmLThjZTAtNDcxZjE4NjUzNGI3LmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Canada vs. Argentina: Your guide to historic Copa America semifinal showdown</t>
+          <t>Silk, Great Value plant-based milks recalled in Canada</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.433908</t>
+          <t>2024-07-09 12:19:55.945371</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjExMDA1L2NhbmFkYS1hcmdlbnRpbmEtY29wYS1hbWVyaWNhL9IBRmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjExMDA1L2NhbmFkYS1hcmdlbnRpbmEtY29wYS1hbWVyaWNhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMjUwL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtbWlsay1yZWNhbGwtY2FuYWRhL9IBWGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMjUwL3NpbGstZ3JlYXQtdmFsdWUtcGxhbnQtYmFzZWQtbWlsay1yZWNhbGwtY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>BLOG: Canada unlikely to meet NATO commitments without significant debt accumulation</t>
+          <t>The remnants of hurricane Beryl are heading to Canada. Here's where it's expected to land</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.449599</t>
+          <t>2024-07-09 12:19:55.945371</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmZyYXNlcmluc3RpdHV0ZS5vcmcvYmxvZ3MvY2FuYWRhLXVubGlrZWx5LXRvLW1lZXQtbmF0by1jb21taXRtZW50cy13aXRob3V0LXNpZ25pZmljYW50LWRlYnQtYWNjdW11bGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikQFodHRwczovL3d3dy5jdHZuZXdzLmNhL2NsaW1hdGUtYW5kLWVudmlyb25tZW50L3RoZS1yZW1uYW50cy1vZi1odXJyaWNhbmUtYmVyeWwtYXJlLWhlYWRpbmctdG8tY2FuYWRhLWhlcmUtcy13aGVyZS1pdC1zLWV4cGVjdGVkLXRvLWxhbmQtMS42OTU2OTE40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Tory leader widens gap over Trudeau on economy in Canada poll</t>
+          <t>Soccer frenzy in the nation’s capital</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.449599</t>
+          <t>2024-07-09 12:19:55.961451</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmJubmJsb29tYmVyZy5jYS9idXNpbmVzcy9wb2xpdGljcy8yMDI0LzA3LzA5L3RvcnktbGVhZGVyLXdpZGVucy1nYXAtb3Zlci10cnVkZWF1LW9uLWVjb25vbXktaW4tY2FuYWRhLXBvbGwv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vb3R0YXdhLmN0dm5ld3MuY2Evc29jY2VyLWZyZW56eS1pbi10aGUtbmF0aW9uLXMtY2FwaXRhbC0xLjY5NTc1MDfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>East Coast RV trip features family, food and a few bumps</t>
+          <t>Ironman Canada race moving from Penticton to Ottawa</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.449599</t>
+          <t>2024-07-09 12:19:55.961451</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiU2h0dHBzOi8vby5jYW5hZGEuY29tL3RyYXZlbC9lYXN0LWNvYXN0LXJ2LXRyaXAtZmVhdHVyZXMtZmFtaWx5LWZvb2QtYW5kLWEtZmV3LWJ1bXBz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNzQ0L2lyb25tYW4tY2FuYWRhLW1vdmluZy1wZW50aWN0b24tdG8tb3R0YXdhL9IBUmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNzQ0L2lyb25tYW4tY2FuYWRhLW1vdmluZy1wZW50aWN0b24tdG8tb3R0YXdhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Posthaste: Sellers are swarming Canada's housing market — especially in these cities</t>
+          <t>Canada’s Men’s Rugby Team’s match day roster named ahead of match against Romania in Ottawa</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.449599</t>
+          <t>2024-07-09 12:19:55.961451</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9zZWxsZXJzLXJ1c2gtYmFjay1jYW5hZGEtaG91c2luZy1tYXJrZXTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vcnVnYnkuY2EvZW4vbmV3cy8yMDI0LzA3L2NhbmFkYS1zLW1lbi1zLXJ1Z2J5LXRlYW0tcy1tYXRjaC1kYXktcm9zdGVyLW5hbWVkLWFoZWFkLW9mLW1hdGNoLWFnYWluc3Qtcm9tYW5pYS1pbi1vdHRhd2HSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Alberta firefighters facing challenging conditions as heat wave sweeps Western Canada</t>
+          <t>Copa America Preview: Messi, Argentina rematch stand between Canada and glory</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.449599</t>
+          <t>2024-07-09 15:26:45.106418</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9lZG1vbnRvbi9hbGJlcnRhLXdpbGRmaXJlcy1oZWF0LTEuNzI1Nzk0MtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3OTQy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdG9yb250by5jaXR5bmV3cy5jYS8yMDI0LzA3LzA5L2NhbmFkYS1jb3BhLWFtZXJpY2Etc2VtaS1maW5hbHMtYXJnZW50aW5hLW1hdGNoL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Nova Scotia soccer star Shaffelburg at Copa America an 'achievement for whole family'</t>
+          <t>Niagara Health is hiring!</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.462518</t>
+          <t>2024-07-09 15:26:45.106418</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2phY29iLXNoYWZmZWxidXJnLWNhbmFkYS1jb3BhLWFtZXJpY2EtZmFtaWx5LWFjaGlldmVtZW50LTEuNzI1ODE4N9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4MTg3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiKWh0dHBzOi8vd3d3Lm5pYWdhcmFoZWFsdGgub24uY2Evc2l0ZS9ob21l0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Suspect in Carling Avenue homicide wanted on Canada-wide warrant</t>
+          <t>Canada vs. Messi, Argentina - Transcript</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.463530</t>
+          <t>2024-07-09 15:26:45.106418</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb3R0YXdhY2l0aXplbi5jb20vbmV3cy9sb2NhbC1uZXdzL3N1c3BlY3QtaW4tY2FybGluZy1hdmUtaG9taWNpZGUtd2FudGVkLW9uLWNhbmFkYS13aWRlLXdhcnJhbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vd3d3LmNiYy5jYS9yYWRpby9mcm9udGJ1cm5lci9jYW5hZGEtdnMtbWVzc2ktYXJnZW50aW5hLXRyYW5zY3JpcHQtMS43MjU4NTI40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTg1Mjg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Canada draws link between June heat wave and climate change with new attribution analysis</t>
+          <t>TIFF announces five more World Premieres from Canada, France, India, UK, and USA</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.463530</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NsaW1hdGUvY2FuYWRhLWVjY2MtcmFwaWQtYXR0cmlidXRpb24taGVhdC0xLjcyNTc0NTbSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzQ1Ng?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vdGlmZi5uZXQvcHJlc3MvbmV3cy90aWZmLWFubm91bmNlcy1maXZlLW1vcmUtd29ybGQtcHJlbWllcmVzLWZyb20tY2FuYWRhLWZyYW5jZS1pbmRpYS11ay1hbmQtdXNh0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Meet Canada’s Best Employers For Diversity 2024</t>
+          <t>Canada ready for rematch with Messi, Argentina in Copa America semifinal on TSN</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvcmFjaGVscGVhY2htYW4vMjAyNC8wNy8wOS9tZWV0LWNhbmFkYXMtYmVzdC1lbXBsb3llcnMtZm9yLWRpdmVyc2l0eS0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY2FuYWRhLXJlYWR5LWZvci1yZW1hdGNoLXdpdGgtbGlvbmVsLW1lc3NpLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLW9uLXRzbi0xLjIxNDYxNzHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Canada: grizzly bear hunting quietly reinstated in Alberta</t>
+          <t>Nato allies pressure Canada to step up spending at Washington summit</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.433908</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS93b3JsZC9hcnRpY2xlLzIwMjQvanVsLzA5L2FsYmVydGEtZ3JpenpseS1iZWFyLWh1bnRpbmfSAVJodHRwczovL2FtcC50aGVndWFyZGlhbi5jb20vd29ybGQvYXJ0aWNsZS8yMDI0L2p1bC8wOS9hbGJlcnRhLWdyaXp6bHktYmVhci1odW50aW5n?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmJiYy5jb20vbmV3cy9hcnRpY2xlcy9jbDR5Z3psejRtem_SATJodHRwczovL3d3dy5iYmMuY29tL25ld3MvYXJ0aWNsZXMvY2w0eWd6bHo0bXpvLmFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>How a new incubator is supercharging women-focused health startups in Canada</t>
+          <t>Tory leader widens gap over Trudeau on economy in Canada poll</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvaGVhbHRoL2hvdy1hLW5ldy1pbmN1YmF0b3ItaXMtc3VwZXJjaGFyZ2luZy13b21lbi1mb2N1c2VkLWhlYWx0aC1zdGFydHVwcy1pbi1jYW5hZGEtMS42OTU2Mjc00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmJubmJsb29tYmVyZy5jYS9idXNpbmVzcy9wb2xpdGljcy8yMDI0LzA3LzA5L3RvcnktbGVhZGVyLXdpZGVucy1nYXAtb3Zlci10cnVkZWF1LW9uLWVjb25vbXktaW4tY2FuYWRhLXBvbGwv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Ontario court approves class-action by immigration detainees against federal government</t>
+          <t>Alberta firefighters facing challenging conditions as heat wave sweeps Western Canada</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihwFodHRwczovL3d3dy5jYmMuY2EvbmV3cy9jYW5hZGEvb3R0YXdhL29udGFyaW8tY291cnQtYXBwcm92ZXMtY2xhc3MtYWN0aW9uLWJ5LWltbWlncmF0aW9uLWRldGFpbmVlcy1hZ2FpbnN0LWZlZGVyYWwtZ292ZXJubWVudC0xLjcyNTc2MDLSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzYwMg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9lZG1vbnRvbi9hbGJlcnRhLXdpbGRmaXJlcy1oZWF0LTEuNzI1Nzk0MtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3OTQy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>The philosophy — and politics — behind Canada's reluctance to meet NATO's spending target</t>
+          <t>Posthaste: Sellers are swarming Canada's housing market — especially in these cities</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2NhbmFkYS1uYXRvLWpvbHktYmxhaXItdHJ1ZGVhdS1kZWZlbmNlLTEuNzI1NzczN9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU3NzM3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vbmV3cy9zZWxsZXJzLXJ1c2gtYmFjay1jYW5hZGEtaG91c2luZy1tYXJrZXTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>KFC's move to halal menu in most of Ontario sparks outrage, calls for boycott — and support</t>
+          <t>BLOG: Canada unlikely to meet NATO commitments without significant debt accumulation</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.449599</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9rZmMtaGFsYWwtbWVudS1ib3ljb3R0LTEuNzI1ODI4OdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4Mjg5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmZyYXNlcmluc3RpdHV0ZS5vcmcvYmxvZ3MvY2FuYWRhLXVubGlrZWx5LXRvLW1lZXQtbmF0by1jb21taXRtZW50cy13aXRob3V0LXNpZ25pZmljYW50LWRlYnQtYWNjdW11bGF0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Where Did My Money Go? The Cost of Being Single in Canada</t>
+          <t>Nova Scotia soccer star Shaffelburg at Copa America an 'achievement for whole family'</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.462518</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMikAFodHRwczovL3d3dy5yYmNyb3lhbGJhbmsuY29tL2VuLWNhL215LW1vbmV5LW1hdHRlcnMvbGlmZS1ldmVudHMvZmFtaWx5LWV2ZW50cy9tYXJyaWFnZS93aGVyZS1kaWQtbXktbW9uZXktZ28tdGhlLWNvc3Qtb2YtYmVpbmctc2luZ2xlLWluLWNhbmFkYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiY2h0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2phY29iLXNoYWZmZWxidXJnLWNhbmFkYS1jb3BhLWFtZXJpY2EtZmFtaWx5LWFjaGlldmVtZW50LTEuNzI1ODE4N9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4MTg3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Ticketmaster notifies Canadian customers of May data breach</t>
+          <t>Suspect in Carling Avenue homicide wanted on Canada-wide warrant</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.465540</t>
+          <t>2024-07-09 15:27:24.463530</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMTMyL3RpY2tldG1hc3Rlci1oYWNrLWN1c3RvbWVycy1jYW5hZGEv0gFLaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTIxMzIvdGlja2V0bWFzdGVyLWhhY2stY3VzdG9tZXJzLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vb3R0YXdhY2l0aXplbi5jb20vbmV3cy9sb2NhbC1uZXdzL3N1c3BlY3QtaW4tY2FybGluZy1hdmUtaG9taWNpZGUtd2FudGVkLW9uLWNhbmFkYS13aWRlLXdhcnJhbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Where to watch Canada vs. Argentina's Copa América semifinal: Streaming, TV channels, start time and more</t>
+          <t>Canada: grizzly bear hunting quietly reinstated in Alberta</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL2NhLm5ld3MueWFob28uY29tL3doZXJlLXRvLXdhdGNoLWNhbmFkYS12cy1hcmdlbnRpbmFzLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtc3RyZWFtaW5nLXR2LWNoYW5uZWxzLXN0YXJ0LXRpbWUtYW5kLW1vcmUtMTgwNTQwODYxLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS93b3JsZC9hcnRpY2xlLzIwMjQvanVsLzA5L2FsYmVydGEtZ3JpenpseS1iZWFyLWh1bnRpbmfSAVJodHRwczovL2FtcC50aGVndWFyZGlhbi5jb20vd29ybGQvYXJ0aWNsZS8yMDI0L2p1bC8wOS9hbGJlcnRhLWdyaXp6bHktYmVhci1odW50aW5n?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>28 one-day heat records tumble, Lytton hottest place in Canada</t>
+          <t>How a new incubator is supercharging women-focused health startups in Canada</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDkvYmMtanVseS04LWhlYXQtcmVjb3Jkcy1seXR0b24tY2FuYWRhLWhvdC1zcG90L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvaGVhbHRoL2hvdy1hLW5ldy1pbmN1YmF0b3ItaXMtc3VwZXJjaGFyZ2luZy13b21lbi1mb2N1c2VkLWhlYWx0aC1zdGFydHVwcy1pbi1jYW5hZGEtMS42OTU2Mjc00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Canada Soccer AccelerateHER Program Awards Grants and Funds All-Women C-Diploma Workshops</t>
+          <t>KFC's move to halal menu in most of Ontario sparks outrage, calls for boycott — and support</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItYWNjZWxlcmF0ZWhlci1wcm9ncmFtLWF3YXJkcy1ncmFudHMtYW5kLWZ1bmRzLWFsbC13b21lbi1jLWRpcGxvbWEtd29ya3Nob3BzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9rZmMtaGFsYWwtbWVudS1ib3ljb3R0LTEuNzI1ODI4OdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4Mjg5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Local colleges named in top 200 employers in Canada for diversity</t>
+          <t>Ticketmaster notifies Canadian customers of May data breach</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbG9uZG9uLmN0dm5ld3MuY2EvbG9jYWwtY29sbGVnZXMtbmFtZWQtaW4tdG9wLTIwMC1lbXBsb3llcnMtaW4tY2FuYWRhLWZvci1kaXZlcnNpdHktMS42OTU3MTgx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyMTMyL3RpY2tldG1hc3Rlci1oYWNrLWN1c3RvbWVycy1jYW5hZGEv0gFLaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTIxMzIvdGlja2V0bWFzdGVyLWhhY2stY3VzdG9tZXJzLWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>A Final Rest for the Unknown Newfoundland Soldier</t>
+          <t>Where Did My Money Go? The Cost of Being Single in Canada</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5jYW5hZGEuY2EvZW4vZGVwYXJ0bWVudC1uYXRpb25hbC1kZWZlbmNlL21hcGxlLWxlYWYvZGVmZW5jZS8yMDI0LzA3L2ZpbmFsLXJlc3QtZm9yLXVua25vd24tbmV3Zm91bmRsYW5kLXNvbGRpZXIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikAFodHRwczovL3d3dy5yYmNyb3lhbGJhbmsuY29tL2VuLWNhL215LW1vbmV5LW1hdHRlcnMvbGlmZS1ldmVudHMvZmFtaWx5LWV2ZW50cy9tYXJyaWFnZS93aGVyZS1kaWQtbXktbW9uZXktZ28tdGhlLWNvc3Qtb2YtYmVpbmctc2luZ2xlLWluLWNhbmFkYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Meteorologists warn of "torrential downpour" as hurricane remnants head for southwestern Ontario</t>
+          <t>Ontario court approves class-action by immigration detainees against federal government</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9sb25kb24vaHVycmljYW5lLWJlcnlsLXNvdXRoZXJuLW9udGFyaW8tbG9uZG9uLXJhaW5mYWxsLTEuNzI1ODAyMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4MDIy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihwFodHRwczovL3d3dy5jYmMuY2EvbmV3cy9jYW5hZGEvb3R0YXdhL29udGFyaW8tY291cnQtYXBwcm92ZXMtY2xhc3MtYWN0aW9uLWJ5LWltbWlncmF0aW9uLWRldGFpbmVlcy1hZ2FpbnN0LWZlZGVyYWwtZ292ZXJubWVudC0xLjcyNTc2MDLSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzYwMg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Canada to provide NATO updated defence spending plan</t>
+          <t>Meet Canada’s Best Employers For Diversity 2024</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2024-07-09 15:27:24.481180</t>
+          <t>2024-07-09 15:27:24.465540</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9uZXdzL3dvcmxkL2NhbmFkYS10by1wcm92aWRlLW5hdG8tdXBkYXRlZC1kZWZlbmNlLXNwZW5kaW5nLXBsYW7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvcmFjaGVscGVhY2htYW4vMjAyNC8wNy8wOS9tZWV0LWNhbmFkYXMtYmVzdC1lbXBsb3llcnMtZm9yLWRpdmVyc2l0eS0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Record 107 teams to qualify for Canada Soccer’s 2024 amateur competitions</t>
+          <t>28 one-day heat records tumble, Lytton hottest place in Canada</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -2724,14 +2724,14 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL3JlY29yZC0xMDctdGVhbXMtdG8tcXVhbGlmeS1mb3ItY2FuYWRhLXNvY2NlcnMtMjAyNC1hbWF0ZXVyLWNvbXBldGl0aW9ucy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdmFuY291dmVyLmNpdHluZXdzLmNhLzIwMjQvMDcvMDkvYmMtanVseS04LWhlYXQtcmVjb3Jkcy1seXR0b24tY2FuYWRhLWhvdC1zcG90L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Drake bets $300K on Canada to beat Messi, Argentina in Copa America semifinal</t>
+          <t>'Tears come to my eyes': Track star and family granted extension to stay in Canada after deportation order</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -2741,14 +2741,14 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9kcmFrZS1iZXRzLTMwMGstb24tY2FuYWRhLXRvLWJlYXQtbWVzc2ktYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWwv0gFzaHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL3NvY2Nlci9kcmFrZS1iZXRzLTMwMGstb24tY2FuYWRhLXRvLWJlYXQtbWVzc2ktYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWwvc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijAFodHRwczovL3Rvcm9udG8uY3R2bmV3cy5jYS90ZWFycy1jb21lLXRvLW15LWV5ZXMtdHJhY2stc3Rhci1hbmQtZmFtaWx5LWdyYW50ZWQtZXh0ZW5zaW9uLXRvLXN0YXktaW4tY2FuYWRhLWFmdGVyLWRlcG9ydGF0aW9uLW9yZGVyLTEuNjk1Njg4M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>'Tears come to my eyes': Track star and family granted extension to stay in Canada after deportation order</t>
+          <t>Drake bets $300K on Canada to beat Messi, Argentina in Copa America semifinal</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -2758,1010 +2758,2761 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijAFodHRwczovL3Rvcm9udG8uY3R2bmV3cy5jYS90ZWFycy1jb21lLXRvLW15LWV5ZXMtdHJhY2stc3Rhci1hbmQtZmFtaWx5LWdyYW50ZWQtZXh0ZW5zaW9uLXRvLXN0YXktaW4tY2FuYWRhLWFmdGVyLWRlcG9ydGF0aW9uLW9yZGVyLTEuNjk1Njg4M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9kcmFrZS1iZXRzLTMwMGstb24tY2FuYWRhLXRvLWJlYXQtbWVzc2ktYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWwv0gFzaHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL3NvY2Nlci9kcmFrZS1iZXRzLTMwMGstb24tY2FuYWRhLXRvLWJlYXQtbWVzc2ktYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWwvc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>How Canada’s dream supersonic interceptor became a national nightmare</t>
+          <t>Record 107 teams to qualify for Canada Soccer’s 2024 amateur competitions</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2024-07-09 16:26:45.127192</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNubi5jb20vdHJhdmVsL2NhbmFkYS1kcmVhbS1zdXBlcnNvbmljLWJvbWJlci1hdnJvLWFycm93L2luZGV4Lmh0bWzSAUhodHRwczovL2FtcC5jbm4uY29tL2Nubi90cmF2ZWwvY2FuYWRhLWRyZWFtLXN1cGVyc29uaWMtYm9tYmVyLWF2cm8tYXJyb3c?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL3JlY29yZC0xMDctdGVhbXMtdG8tcXVhbGlmeS1mb3ItY2FuYWRhLXNvY2NlcnMtMjAyNC1hbWF0ZXVyLWNvbXBldGl0aW9ucy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Canada's landlords now asking an average of $2,185/month for rent</t>
+          <t>Canada to provide NATO updated defence spending plan</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2024-07-09 16:26:45.131608</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1zLWxhbmRsb3Jkcy1ub3ctYXNraW5nLWFuLWF2ZXJhZ2Utb2YtMi0xODUtbW9udGgtZm9yLXJlbnQtMS42OTU3MjI10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9uZXdzL3dvcmxkL2NhbmFkYS10by1wcm92aWRlLW5hdG8tdXBkYXRlZC1kZWZlbmNlLXNwZW5kaW5nLXBsYW7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Canada urged to spend more on defence as NATO chief addresses summit</t>
+          <t>Meteorologists warn of "torrential downpour" as hurricane remnants head for southwestern Ontario</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2024-07-09 16:27:24.433908</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNTYwL25hdG8tc3VtbWl0LWRlZmVuY2Utc3BlbmRpbmctY2FuYWRhL9IBTGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEyNTYwL25hdG8tc3VtbWl0LWRlZmVuY2Utc3BlbmRpbmctY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9sb25kb24vaHVycmljYW5lLWJlcnlsLXNvdXRoZXJuLW9udGFyaW8tbG9uZG9uLXJhaW5mYWxsLTEuNzI1ODAyMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU4MDIy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Key things to know about Canada vs. Argentina’s Copa America semi-final</t>
+          <t>A Final Rest for the Unknown Newfoundland Soldier</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2024-07-09 16:27:24.433908</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYmh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL3NvY2Nlci9hcnRpY2xlLWNhbmFkYS12cy1hcmdlbnRpbmEtc2VtaWZpbmFscy1ob3ctdG8td2F0Y2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5jYW5hZGEuY2EvZW4vZGVwYXJ0bWVudC1uYXRpb25hbC1kZWZlbmNlL21hcGxlLWxlYWYvZGVmZW5jZS8yMDI0LzA3L2ZpbmFsLXJlc3QtZm9yLXVua25vd24tbmV3Zm91bmRsYW5kLXNvbGRpZXIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>First Nations leaders from across Canada gather in Montreal for AFN annual general assembly</t>
+          <t>Local colleges named in top 200 employers in Canada for diversity</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2024-07-09 16:27:24.449599</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiPWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2luZGlnZW5vdXMvYWZuLWFnYS1tb250cmVhbC0xLjcyNTc1NTDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzU1MA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbG9uZG9uLmN0dm5ld3MuY2EvbG9jYWwtY29sbGVnZXMtbmFtZWQtaW4tdG9wLTIwMC1lbXBsb3llcnMtaW4tY2FuYWRhLWZvci1kaXZlcnNpdHktMS42OTU3MTgx0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>The United Church of Canada Releases First Strategic Plan Report</t>
+          <t>Canada Soccer AccelerateHER Program Awards Grants and Funds All-Women C-Diploma Workshops</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2024-07-09 16:27:24.449599</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdW5pdGVkLWNodXJjaC5jYS9uZXdzL3VuaXRlZC1jaHVyY2gtY2FuYWRhLXJlbGVhc2VzLWZpcnN0LXN0cmF0ZWdpYy1wbGFuLXJlcG9ydNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vY2FuYWRhc29jY2VyLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItYWNjZWxlcmF0ZWhlci1wcm9ncmFtLWF3YXJkcy1ncmFudHMtYW5kLWZ1bmRzLWFsbC13b21lbi1jLWRpcGxvbWEtd29ya3Nob3BzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Moving truck driver says mechanical failure led to deadly crash on Trans-Canada Highway west of Calgary</t>
+          <t>Where to watch Canada vs. Argentina's Copa América semifinal: Streaming, TV channels, start time and more</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2024-07-09 16:27:24.465540</t>
+          <t>2024-07-09 15:27:24.481180</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vY2FsZ2FyeWhlcmFsZC5jb20vbmV3cy9jcmltZS9tZWNoYW5pY2FsLWZhaWx1cmUtZGVhZGx5LWNyYXNoLXRyYW5zLWNhbmFkYS1oaWdod2F5LWRyaXZlctIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL2NhLm5ld3MueWFob28uY29tL3doZXJlLXRvLXdhdGNoLWNhbmFkYS12cy1hcmdlbnRpbmFzLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtc3RyZWFtaW5nLXR2LWNoYW5uZWxzLXN0YXJ0LXRpbWUtYW5kLW1vcmUtMTgwNTQwODYxLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Ottawa aims to clear Phoenix backlog by 2025, spend nearly $1B more</t>
+          <t>How Canada’s dream supersonic interceptor became a national nightmare</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2024-07-09 17:26:45.128203</t>
+          <t>2024-07-09 16:26:45.127192</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEzNDY0L3Bob2VuaXgtcGF5LXN5c3RlbS1iYWNrbG9nLW5ldy1zcGVuZGluZy1kZWFkbGluZS_SAVlodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYxMzQ2NC9waG9lbml4LXBheS1zeXN0ZW0tYmFja2xvZy1uZXctc3BlbmRpbmctZGVhZGxpbmUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmNubi5jb20vdHJhdmVsL2NhbmFkYS1kcmVhbS1zdXBlcnNvbmljLWJvbWJlci1hdnJvLWFycm93L2luZGV4Lmh0bWzSAUhodHRwczovL2FtcC5jbm4uY29tL2Nubi90cmF2ZWwvY2FuYWRhLWRyZWFtLXN1cGVyc29uaWMtYm9tYmVyLWF2cm8tYXJyb3c?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Record rainfall expected for parts of southwestern Ontario on Wednesday</t>
+          <t>Canada's landlords now asking an average of $2,185/month for rent</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2024-07-09 17:27:24.481180</t>
+          <t>2024-07-09 16:26:45.131608</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS93aW5kc29yL3JhaW5mYWxsLXJlY29yZC1icmVha2luZy1zb3V0aHdlc3Rlcm4tb250YXJpby0xLjcyNTgzNznSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODM3OQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvY2FuYWRhL2NhbmFkYS1zLWxhbmRsb3Jkcy1ub3ctYXNraW5nLWFuLWF2ZXJhZ2Utb2YtMi0xODUtbW9udGgtZm9yLXJlbnQtMS42OTU3MjI10gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Drake places $300,000 bet on Canada to beat Argentina in Copa America semifinals</t>
+          <t>Key things to know about Canada vs. Argentina’s Copa America semi-final</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2024-07-09 17:27:24.481180</t>
+          <t>2024-07-09 16:27:24.433908</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3LnVzYXRvZGF5LmNvbS9zdG9yeS9zcG9ydHMvc29jY2VyLzIwMjQvMDcvMDkvZHJha2UtMzAway1iZXQtY2FuYWRhLWFyZ2VudGluYS1jb3BhLWFtZXJpY2Etc2VtaWZpbmFscy83NDM0NDMxOTAwNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYmh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL3NvY2Nlci9hcnRpY2xlLWNhbmFkYS12cy1hcmdlbnRpbmEtc2VtaWZpbmFscy1ob3ctdG8td2F0Y2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Argentina 2-0 Canada: 2024 Copa América semi-final – as it happened</t>
+          <t>First Nations leaders from across Canada gather in Montreal for AFN annual general assembly</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2024-07-09 18:26:45.127192</t>
+          <t>2024-07-09 16:27:24.449599</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9saXZlLzIwMjQvanVsLzA5L2FyZ2VudGluYS12LWNhbmFkYS0yMDI0LWNvcGEtYW1lcmljYS1zZW1pLWZpbmFsLWxpdmUtdXBkYXRlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiPWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2luZGlnZW5vdXMvYWZuLWFnYS1tb250cmVhbC0xLjcyNTc1NTDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1NzU1MA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Ontario says nine listeriosis infections linked to recall of silk milk</t>
+          <t>The United Church of Canada Releases First Strategic Plan Report</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2024-07-09 18:26:45.131608</t>
+          <t>2024-07-09 16:27:24.449599</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vY2FuYWRhL2FydGljbGUtb250YXJpby1zYXlzLW5pbmUtbGlzdGVyaW9zaXMtaW5mZWN0aW9ucy1saW5rZWQtdG8tcmVjYWxsLW9mLXNpbGstbWlsay_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdW5pdGVkLWNodXJjaC5jYS9uZXdzL3VuaXRlZC1jaHVyY2gtY2FuYWRhLXJlbGVhc2VzLWZpcnN0LXN0cmF0ZWdpYy1wbGFuLXJlcG9ydNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Canada’s Copa America dream run ends with 2-0 loss to Argentina in semi-final</t>
+          <t>Moving truck driver says mechanical failure led to deadly crash on Trans-Canada Highway west of Calgary</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2024-07-09 18:27:24.426857</t>
+          <t>2024-07-09 16:27:24.465540</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL3NvY2Nlci9hcnRpY2xlLWNhbmFkYS1wcmltZWQtZm9yLXJvbGUtb2YtZ2lhbnQta2lsbGVycy1pbi1jb3BhLXNlbWlzLWNsYXNoLXdpdGgv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vY2FsZ2FyeWhlcmFsZC5jb20vbmV3cy9jcmltZS9tZWNoYW5pY2FsLWZhaWx1cmUtZGVhZGx5LWNyYXNoLXRyYW5zLWNhbmFkYS1oaWdod2F5LWRyaXZlctIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Soccer frenzy in the nation’s capital</t>
+          <t>Ottawa aims to clear Phoenix backlog by 2025, spend nearly $1B more</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2024-07-09 18:27:24.426857</t>
+          <t>2024-07-09 17:26:45.128203</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vb3R0YXdhLmN0dm5ld3MuY2Evc29jY2VyLWZyZW56eS1pbi10aGUtbmF0aW9uLXMtY2FwaXRhbC0xLjY5NTc1MDfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjEzNDY0L3Bob2VuaXgtcGF5LXN5c3RlbS1iYWNrbG9nLW5ldy1zcGVuZGluZy1kZWFkbGluZS_SAVlodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYxMzQ2NC9waG9lbml4LXBheS1zeXN0ZW0tYmFja2xvZy1uZXctc3BlbmRpbmctZGVhZGxpbmUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Drake bets big on Canada to upset Argentina in Copa America semifinals</t>
+          <t>Drake places $300,000 bet on Canada to beat Argentina in Copa America semifinals</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2024-07-09 18:27:24.433908</t>
+          <t>2024-07-09 17:27:24.481180</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvZW50ZXJ0YWlubWVudC9kcmFrZS1iZXRzLWJpZy1vbi1jYW5hZGEtdG8tdXBzZXQtYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWxzLTEuNjk1NzUxMdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3LnVzYXRvZGF5LmNvbS9zdG9yeS9zcG9ydHMvc29jY2VyLzIwMjQvMDcvMDkvZHJha2UtMzAway1iZXQtY2FuYWRhLWFyZ2VudGluYS1jb3BhLWFtZXJpY2Etc2VtaWZpbmFscy83NDM0NDMxOTAwNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Ontario reports five people hospitalized with listeriosis, as Silk and Great Value beverages recalled across Canada</t>
+          <t>Record rainfall expected for parts of southwestern Ontario on Wednesday</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2024-07-09 18:27:24.449599</t>
+          <t>2024-07-09 17:27:24.481180</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiwQFodHRwczovL3d3dy50aGVzdGFyLmNvbS9uZXdzL2NhbmFkYS9vbnRhcmlvLXJlcG9ydHMtZml2ZS1wZW9wbGUtaG9zcGl0YWxpemVkLXdpdGgtbGlzdGVyaW9zaXMtYXMtc2lsay1hbmQtZ3JlYXQtdmFsdWUtYmV2ZXJhZ2VzLXJlY2FsbGVkLWFjcm9zcy9hcnRpY2xlX2Q0YmI0YmE4LTNlMTUtMTFlZi1hODhjLWZiMjczNGQ2MGFiYS5odG1s0gHFAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL25ld3MvY2FuYWRhL29udGFyaW8tcmVwb3J0cy1maXZlLXBlb3BsZS1ob3NwaXRhbGl6ZWQtd2l0aC1saXN0ZXJpb3Npcy1hcy1zaWxrLWFuZC1ncmVhdC12YWx1ZS1iZXZlcmFnZXMtcmVjYWxsZWQtYWNyb3NzL2FydGljbGVfZDRiYjRiYTgtM2UxNS0xMWVmLWE4OGMtZmIyNzM0ZDYwYWJhLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS93aW5kc29yL3JhaW5mYWxsLXJlY29yZC1icmVha2luZy1zb3V0aHdlc3Rlcm4tb250YXJpby0xLjcyNTgzNznSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODM3OQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Thunderstorms flood Trans-Canada Highway near Pasadena</t>
+          <t>Argentina 2-0 Canada: 2024 Copa América semi-final – as it happened</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2024-07-09 18:27:24.462518</t>
+          <t>2024-07-09 18:26:45.127192</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9uZXdmb3VuZGxhbmQtbGFicmFkb3IvcGFzYWRlbmEtaGlnaHdheS1mbG9vZGluZy0xLjcyNTg2NTLSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODY1Mg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9saXZlLzIwMjQvanVsLzA5L2FyZ2VudGluYS12LWNhbmFkYS0yMDI0LWNvcGEtYW1lcmljYS1zZW1pLWZpbmFsLWxpdmUtdXBkYXRlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Durant (calf) out for USA's friendly vs. Canada</t>
+          <t>Ontario says nine listeriosis infections linked to recall of silk milk</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2024-07-09 18:27:24.465540</t>
+          <t>2024-07-09 18:26:45.131608</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmVzcG4uY29tL25iYS9zdG9yeS9fL2lkLzQwNTI4OTg3L2tldmluLWR1cmFudC1jYWxmLXRlYW0tdXNhLWZyaWVuZGx5LXZzLWNhbmFkYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vY2FuYWRhL2FydGljbGUtb250YXJpby1zYXlzLW5pbmUtbGlzdGVyaW9zaXMtaW5mZWN0aW9ucy1saW5rZWQtdG8tcmVjYWxsLW9mLXNpbGstbWlsay_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Wildfire danger soars as heat wave envelops Western Canada</t>
+          <t>Canada’s Copa America dream run ends with 2-0 loss to Argentina in semi-final</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2024-07-09 19:27:24.481180</t>
+          <t>2024-07-09 18:27:24.426857</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vY2FuYWRhL2FsYmVydGEvYXJ0aWNsZS13aWxkZmlyZS1kYW5nZXItc29hcnMtYXMtaGVhdC13YXZlLWVudmVsb3Blcy13ZXN0ZXJuLWNhbmFkYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL3NvY2Nlci9hcnRpY2xlLWNhbmFkYS1wcmltZWQtZm9yLXJvbGUtb2YtZ2lhbnQta2lsbGVycy1pbi1jb3BhLXNlbWlzLWNsYXNoLXdpdGgv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Alvarez scores as Argentina leads Canada at halftime of Copa America semifinal</t>
+          <t>Drake bets big on Canada to upset Argentina in Copa America semifinals</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2024-07-09 20:26:45.075148</t>
+          <t>2024-07-09 18:27:24.433908</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvanVsaWFuLWFsdmFyZXotc2NvcmVzLWFzLWFyZ2VudGluYS1sZWFkcy1jYW5hZGEtYXQtaGFsZnRpbWUtb2YtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC0xLjIxNDY1MDfSAXpodHRwczovL3d3dy50c24uY2EvanVsaWFuLWFsdmFyZXotc2NvcmVzLWFzLWFyZ2VudGluYS1sZWFkcy1jYW5hZGEtYXQtaGFsZnRpbWUtb2YtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC0xLjIxNDY1MDc_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvZW50ZXJ0YWlubWVudC9kcmFrZS1iZXRzLWJpZy1vbi1jYW5hZGEtdG8tdXBzZXQtYXJnZW50aW5hLWluLWNvcGEtYW1lcmljYS1zZW1pZmluYWxzLTEuNjk1NzUxMdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Extreme June heatwave 'much more likely' caused by human-made climate change, says Environment Canada</t>
+          <t>Ontario reports five people hospitalized with listeriosis, as Silk and Great Value beverages recalled across Canada</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2024-07-09 20:27:24.465540</t>
+          <t>2024-07-09 18:27:24.449599</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL2F0bGFudGljLmN0dm5ld3MuY2EvbW9yZS9leHRyZW1lLWp1bmUtaGVhdHdhdmUtbXVjaC1tb3JlLWxpa2VseS1jYXVzZWQtYnktaHVtYW4tbWFkZS1jbGltYXRlLWNoYW5nZS1zYXlzLWVudmlyb25tZW50LWNhbmFkYS0xLjY5NTc2MznSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiwQFodHRwczovL3d3dy50aGVzdGFyLmNvbS9uZXdzL2NhbmFkYS9vbnRhcmlvLXJlcG9ydHMtZml2ZS1wZW9wbGUtaG9zcGl0YWxpemVkLXdpdGgtbGlzdGVyaW9zaXMtYXMtc2lsay1hbmQtZ3JlYXQtdmFsdWUtYmV2ZXJhZ2VzLXJlY2FsbGVkLWFjcm9zcy9hcnRpY2xlX2Q0YmI0YmE4LTNlMTUtMTFlZi1hODhjLWZiMjczNGQ2MGFiYS5odG1s0gHFAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL25ld3MvY2FuYWRhL29udGFyaW8tcmVwb3J0cy1maXZlLXBlb3BsZS1ob3NwaXRhbGl6ZWQtd2l0aC1saXN0ZXJpb3Npcy1hcy1zaWxrLWFuZC1ncmVhdC12YWx1ZS1iZXZlcmFnZXMtcmVjYWxsZWQtYWNyb3NzL2FydGljbGVfZDRiYjRiYTgtM2UxNS0xMWVmLWE4OGMtZmIyNzM0ZDYwYWJhLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Argentina tops Canada 2-0 to advance to Copa América final</t>
+          <t>Thunderstorms flood Trans-Canada Highway near Pasadena</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2024-07-09 21:26:45.067635</t>
+          <t>2024-07-09 18:27:24.462518</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vc3Rvcmllcy9zb2NjZXIvYXJnZW50aW5hLXRvcHMtY2FuYWRhLTItMC1hZHZhbmNlLWNvcGEtYW1lcmljYS1maW5hbNIBXWh0dHBzOi8vYW1wLmZveHNwb3J0cy5jb20vc3Rvcmllcy9zb2NjZXIvYXJnZW50aW5hLXRvcHMtY2FuYWRhLTItMC1hZHZhbmNlLWNvcGEtYW1lcmljYS1maW5hbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9uZXdmb3VuZGxhbmQtbGFicmFkb3IvcGFzYWRlbmEtaGlnaHdheS1mbG9vZGluZy0xLjcyNTg2NTLSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODY1Mg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>The Breakdown | Nunavut grows up + Canada and NATO</t>
+          <t>Durant (calf) out for USA's friendly vs. Canada</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>2024-07-09 21:26:45.075148</t>
+          <t>2024-07-09 18:27:24.465540</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDM4MzLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vd3d3LmVzcG4uY29tL25iYS9zdG9yeS9fL2lkLzQwNTI4OTg3L2tldmluLWR1cmFudC1jYWxmLXRlYW0tdXNhLWZyaWVuZGx5LXZzLWNhbmFkYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Vote for Canada’s best litigation boutiques for 2024-25</t>
+          <t>Wildfire danger soars as heat wave envelops Western Canada</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>2024-07-09 21:26:45.090846</t>
+          <t>2024-07-09 19:27:24.481180</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmNhbmFkaWFubGF3eWVybWFnLmNvbS9uZXdzL2dlbmVyYWwvdm90ZS1mb3ItY2FuYWRhcy1iZXN0LWxpdGlnYXRpb24tYm91dGlxdWVzLWZvci0yMDI0LTI1LzM4NzIyONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vY2FuYWRhL2FsYmVydGEvYXJ0aWNsZS13aWxkZmlyZS1kYW5nZXItc29hcnMtYXMtaGVhdC13YXZlLWVudmVsb3Blcy13ZXN0ZXJuLWNhbmFkYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Government of Canada publishes a report to tackle anti-black racism in the justice system</t>
+          <t>Alvarez scores as Argentina leads Canada at halftime of Copa America semifinal</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>2024-07-09 21:26:45.090846</t>
+          <t>2024-07-09 20:26:45.075148</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5jYW5hZGlhbmxhd3llcm1hZy5jb20vbmV3cy9nZW5lcmFsL2dvdmVybm1lbnQtb2YtY2FuYWRhLXB1Ymxpc2hlcy1hLXJlcG9ydC10by10YWNrbGUtYW50aS1ibGFjay1yYWNpc20taW4tdGhlLWp1c3RpY2Utc3lzdGVtLzM4NzIyOdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvanVsaWFuLWFsdmFyZXotc2NvcmVzLWFzLWFyZ2VudGluYS1sZWFkcy1jYW5hZGEtYXQtaGFsZnRpbWUtb2YtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC0xLjIxNDY1MDfSAXpodHRwczovL3d3dy50c24uY2EvanVsaWFuLWFsdmFyZXotc2NvcmVzLWFzLWFyZ2VudGluYS1sZWFkcy1jYW5hZGEtYXQtaGFsZnRpbWUtb2YtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC0xLjIxNDY1MDc_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Supreme Court Justice recuses himself from Quebec secularism law case</t>
+          <t>Extreme June heatwave 'much more likely' caused by human-made climate change, says Environment Canada</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>2024-07-09 21:26:45.127192</t>
+          <t>2024-07-09 20:27:24.465540</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9tb250cmVhbC9zY2otbWFobXVkLWphbWFsLXJlY3VzYWwtMS43MjU5MDA40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTkwMDg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL2F0bGFudGljLmN0dm5ld3MuY2EvbW9yZS9leHRyZW1lLWp1bmUtaGVhdHdhdmUtbXVjaC1tb3JlLWxpa2VseS1jYXVzZWQtYnktaHVtYW4tbWFkZS1jbGltYXRlLWNoYW5nZS1zYXlzLWVudmlyb25tZW50LWNhbmFkYS0xLjY5NTc2MznSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Argentina ends Canada's run to reach Copa America final again</t>
+          <t>Argentina tops Canada 2-0 to advance to Copa América final</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>2024-07-09 21:26:45.131608</t>
+          <t>2024-07-09 21:26:45.067635</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiK2h0dHBzOi8vd3d3LnRoZXNjb3JlLmNvbS90b3Bzbi9uZXdzLzI5Mzc4NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vc3Rvcmllcy9zb2NjZXIvYXJnZW50aW5hLXRvcHMtY2FuYWRhLTItMC1hZHZhbmNlLWNvcGEtYW1lcmljYS1maW5hbNIBXWh0dHBzOi8vYW1wLmZveHNwb3J0cy5jb20vc3Rvcmllcy9zb2NjZXIvYXJnZW50aW5hLXRvcHMtY2FuYWRhLTItMC1hZHZhbmNlLWNvcGEtYW1lcmljYS1maW5hbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Canada's historic Copa America run ends with semifinal loss to Argentina</t>
+          <t>The Breakdown | Nunavut grows up + Canada and NATO</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.417838</t>
+          <t>2024-07-09 21:26:45.075148</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXJlY2FwLWp1bHktOS0xLjcyNTg3MzHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODczMQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDM4MzLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Canada undone by Álvarez, Messi in hard-fought Copa América semifinal vs. Argentina</t>
+          <t>Vote for Canada’s best litigation boutiques for 2024-25</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.417838</t>
+          <t>2024-07-09 21:26:45.090846</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtdW5kb25lLWJ5LWFsdmFyZXotbWVzc2ktaW4taGFyZC1mb3VnaHQtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC12cy1hcmdlbnRpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmNhbmFkaWFubGF3eWVybWFnLmNvbS9uZXdzL2dlbmVyYWwvdm90ZS1mb3ItY2FuYWRhcy1iZXN0LWxpdGlnYXRpb24tYm91dGlxdWVzLWZvci0yMDI0LTI1LzM4NzIyONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Canada’s Alphonso Davies exits Copa America semifinal vs. Argentina</t>
+          <t>Government of Canada publishes a report to tackle anti-black racism in the justice system</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.433908</t>
+          <t>2024-07-09 21:26:45.090846</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jYW5hZGFzLWFscGhvbnNvLWRhdmllcy1leGl0cy1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLXZzLWFyZ2VudGluYS_SAWlodHRwczovL3d3dy5zcG9ydHNuZXQuY2Evc29jY2VyL2NhbmFkYXMtYWxwaG9uc28tZGF2aWVzLWV4aXRzLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtdnMtYXJnZW50aW5hL3NuLWFtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5jYW5hZGlhbmxhd3llcm1hZy5jb20vbmV3cy9nZW5lcmFsL2dvdmVybm1lbnQtb2YtY2FuYWRhLXB1Ymxpc2hlcy1hLXJlcG9ydC10by10YWNrbGUtYW50aS1ibGFjay1yYWNpc20taW4tdGhlLWp1c3RpY2Utc3lzdGVtLzM4NzIyOdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Messi scores first goal of Copa America against Canada</t>
+          <t>Supreme Court Justice recuses himself from Quebec secularism law case</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.433908</t>
+          <t>2024-07-09 21:26:45.127192</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvbGlvbmVsLW1lc3NpLXNjb3Jlcy1maXJzdC1nb2FsLW9mLWNvcGEtYW1lcmljYS1mb3ItYXJnZW50aW5hLWFnYWluc3QtY2FuYWRhLTEuMjE0NjUxNtIBcGh0dHBzOi8vd3d3LnRzbi5jYS9saW9uZWwtbWVzc2ktc2NvcmVzLWZpcnN0LWdvYWwtb2YtY29wYS1hbWVyaWNhLWZvci1hcmdlbnRpbmEtYWdhaW5zdC1jYW5hZGEtMS4yMTQ2NTE2P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9tb250cmVhbC9zY2otbWFobXVkLWphbWFsLXJlY3VzYWwtMS43MjU5MDA40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTkwMDg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Lionel Messi scores goal, Argentina tops Canada to reach Copa America final</t>
+          <t>Argentina ends Canada's run to reach Copa America final again</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.433908</t>
+          <t>2024-07-09 21:26:45.131608</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiiAFodHRwczovL3d3dy51c2F0b2RheS5jb20vc3Rvcnkvc3BvcnRzL3NvY2Nlci8yMDI0LzA3LzA5L2FyZ2VudGluYS1jYW5hZGEtbGl2ZS1zY29yZS1oaWdobGlnaHRzLW1lc3NpLWNvcGEtYW1lcmljYS1zZW1pZmluYWwvNzQzMzc4NTMwMDcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiK2h0dHBzOi8vd3d3LnRoZXNjb3JlLmNvbS90b3Bzbi9uZXdzLzI5Mzc4NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Canada falls to Argentina in Copa America semifinal</t>
+          <t>Canada's historic Copa America run ends with semifinal loss to Argentina</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.433908</t>
+          <t>2024-07-09 21:27:24.417838</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRhLWZhbGxzLXRvLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLTEuNjk1NzcxM9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXJlY2FwLWp1bHktOS0xLjcyNTg3MzHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODczMQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Argentina vs. Canada highlights: Messi and Álvarez goals send Argentina to the Copa América final</t>
+          <t>Canada undone by Álvarez, Messi in hard-fought Copa América semifinal vs. Argentina</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.449599</t>
+          <t>2024-07-09 21:27:24.417838</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vbGl2ZS1ibG9nL3NvY2Nlci9hcmdlbnRpbmEtdnMtY2FuYWRhLWxpdmUtdXBkYXRlcy10b3AtbW9tZW50cy1mcm9tLWNvcGEtYW1lcmljYS1zZW1pZmluYWxz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vY2FucGwuY2EvYXJ0aWNsZS9jYW5hZGEtdW5kb25lLWJ5LWFsdmFyZXotbWVzc2ktaW4taGFyZC1mb3VnaHQtY29wYS1hbWVyaWNhLXNlbWlmaW5hbC12cy1hcmdlbnRpbmHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Canada loses to Argentina in Copa America semifinal, but the lessons have been golden</t>
+          <t>Messi scores first goal of Copa America against Canada</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.465540</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirAFodHRwczovL3d3dy50aGVzdGFyLmNvbS9zcG9ydHMvc29jY2VyL2NhbmFkYS1sb3Nlcy10by1hcmdlbnRpbmEtaW4tY29wYS1hbWVyaWNhLXNlbWlmaW5hbC1idXQtdGhlLWxlc3NvbnMtaGF2ZS1iZWVuLWdvbGRlbi9hcnRpY2xlX2ExZTAxMjRjLTNkZmYtMTFlZi04Y2UwLTQ3MWYxODY1MzRiNy5odG1s0gGwAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL3Nwb3J0cy9zb2NjZXIvY2FuYWRhLWxvc2VzLXRvLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLWJ1dC10aGUtbGVzc29ucy1oYXZlLWJlZW4tZ29sZGVuL2FydGljbGVfYTFlMDEyNGMtM2RmZi0xMWVmLThjZTAtNDcxZjE4NjUzNGI3LmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvbGlvbmVsLW1lc3NpLXNjb3Jlcy1maXJzdC1nb2FsLW9mLWNvcGEtYW1lcmljYS1mb3ItYXJnZW50aW5hLWFnYWluc3QtY2FuYWRhLTEuMjE0NjUxNtIBcGh0dHBzOi8vd3d3LnRzbi5jYS9saW9uZWwtbWVzc2ktc2NvcmVzLWZpcnN0LWdvYWwtb2YtY29wYS1hbWVyaWNhLWZvci1hcmdlbnRpbmEtYWdhaW5zdC1jYW5hZGEtMS4yMTQ2NTE2P3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Argentina vs. Canada Highlights | 2024 Copa América | Semifinals</t>
+          <t>Lionel Messi scores goal, Argentina tops Canada to reach Copa America final</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>2024-07-09 21:27:24.481180</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLTY0eGF4NmE3bXpiOTNxOGzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiAFodHRwczovL3d3dy51c2F0b2RheS5jb20vc3Rvcnkvc3BvcnRzL3NvY2Nlci8yMDI0LzA3LzA5L2FyZ2VudGluYS1jYW5hZGEtbGl2ZS1zY29yZS1oaWdobGlnaHRzLW1lc3NpLWNvcGEtYW1lcmljYS1zZW1pZmluYWwvNzQzMzc4NTMwMDcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Argentina 2-0 Canada (Jul 9, 2024) Game Analysis</t>
+          <t>Canada’s Alphonso Davies exits Copa America semifinal vs. Argentina</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>2024-07-09 22:26:45.075148</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LmVzcG4uY29tL3NvY2Nlci9yZXBvcnQvXy9nYW1lSWQvNzAzOTUw0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jYW5hZGFzLWFscGhvbnNvLWRhdmllcy1leGl0cy1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLXZzLWFyZ2VudGluYS_SAWlodHRwczovL3d3dy5zcG9ydHNuZXQuY2Evc29jY2VyL2NhbmFkYXMtYWxwaG9uc28tZGF2aWVzLWV4aXRzLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtdnMtYXJnZW50aW5hL3NuLWFtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>What's open and closed in Ottawa on Canada Day 2024</t>
+          <t>Canada falls to Argentina in Copa America semifinal</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>2024-07-09 22:26:45.090846</t>
+          <t>2024-07-09 21:27:24.433908</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRWh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vd2hhdHMtb3Blbi1jbG9zZWQtY2FuYWRhLWRheS0wODAwMDA1MzEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmNwMjQuY29tL25ld3MvY2FuYWRhLWZhbGxzLXRvLWFyZ2VudGluYS1pbi1jb3BhLWFtZXJpY2Etc2VtaWZpbmFsLTEuNjk1NzcxM9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>‘Proud of this group’: Fans react to Canada’s historic run at Copa America</t>
+          <t>Argentina vs. Canada highlights: Messi and Álvarez goals send Argentina to the Copa América final</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>2024-07-09 22:26:45.130208</t>
+          <t>2024-07-09 21:27:24.449599</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9wcm91ZC1vZi10aGlzLWdyb3VwLWZhbnMtcmVhY3QtdG8tY2FuYWRhcy1oaXN0b3JpYy1ydW4tYXQtY29wYS1hbWVyaWNhL9IBbmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvcHJvdWQtb2YtdGhpcy1ncm91cC1mYW5zLXJlYWN0LXRvLWNhbmFkYXMtaGlzdG9yaWMtcnVuLWF0LWNvcGEtYW1lcmljYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vbGl2ZS1ibG9nL3NvY2Nlci9hcmdlbnRpbmEtdnMtY2FuYWRhLWxpdmUtdXBkYXRlcy10b3AtbW9tZW50cy1mcm9tLWNvcGEtYW1lcmljYS1zZW1pZmluYWxz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Copa América: Messi and Álvarez fire Argentina past Canada and into final</t>
+          <t>Argentina vs. Canada Highlights | 2024 Copa América | Semifinals</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>2024-07-09 22:26:45.131608</t>
+          <t>2024-07-09 21:27:24.481180</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9hcnRpY2xlLzIwMjQvanVsLzA5L2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXNlbWktZmluYWwtbWF0Y2gtcmVwb3J0LXJlc3VsdNIBdWh0dHBzOi8vYW1wLnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9hcnRpY2xlLzIwMjQvanVsLzA5L2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXNlbWktZmluYWwtbWF0Y2gtcmVwb3J0LXJlc3VsdA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLTY0eGF4NmE3bXpiOTNxOGzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>At Copa America, Canada’s predictable defeat comes with the promise of something bigger</t>
+          <t>Argentina 2-0 Canada (Jul 9, 2024) Game Analysis</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>2024-07-09 22:27:24.463530</t>
+          <t>2024-07-09 22:26:45.075148</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL2FydGljbGUtY2FuYWRhLWFyZ2VudGluYS1jb3BhLWFtZXJpY2EtcmVzdWx0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMmh0dHBzOi8vd3d3LmVzcG4uY29tL3NvY2Nlci9yZXBvcnQvXy9nYW1lSWQvNzAzOTUw0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Regulatory framework of laboratory developed tests: Canada vs U.S.</t>
+          <t>What's open and closed in Ottawa on Canada Day 2024</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>2024-07-09 23:26:45.075148</t>
+          <t>2024-07-09 22:26:45.090846</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmJsZy5jb20vZW4vaW5zaWdodHMvMjAyNC8wNy9yZWd1bGF0b3J5LWZyYW1ld29yay1vZi1sYWJvcmF0b3J5LWRldmVsb3BlZC10ZXN0cy1jYW5hZGEtdnMtdXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRWh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vd2hhdHMtb3Blbi1jbG9zZWQtY2FuYWRhLWRheS0wODAwMDA1MzEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Canada insurers investing in fossil fuels as climate risks grow, shareholder group says</t>
+          <t>‘Proud of this group’: Fans react to Canada’s historic run at Copa America</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>2024-07-09 23:26:45.090846</t>
+          <t>2024-07-09 22:26:45.130208</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vY2EuZmluYW5jZS55YWhvby5jb20vbmV3cy9jYW5hZGEtaW5zdXJlcnMtaW52ZXN0aW5nLWZvc3NpbC1mdWVscy0wNDA5MzY4ODIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9wcm91ZC1vZi10aGlzLWdyb3VwLWZhbnMtcmVhY3QtdG8tY2FuYWRhcy1oaXN0b3JpYy1ydW4tYXQtY29wYS1hbWVyaWNhL9IBbmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvcHJvdWQtb2YtdGhpcy1ncm91cC1mYW5zLXJlYWN0LXRvLWNhbmFkYXMtaGlzdG9yaWMtcnVuLWF0LWNvcGEtYW1lcmljYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Heat wave bakes Texas amid power outages while Canada braces for wildfires</t>
+          <t>Copa América: Messi and Álvarez fire Argentina past Canada and into final</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>2024-07-09 23:26:45.130208</t>
+          <t>2024-07-09 22:26:45.131608</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy50aGV3ZWF0aGVybmV0d29yay5jb20vZW4vbmV3cy93ZWF0aGVyL3NldmVyZS9oZWF0LXdhdmUtYmFrZXMtdGV4YXMtYW1pZC1wb3dlci1vdXRhZ2VzLXdoaWxlLWNhbmFkYS1icmFjZXMtZm9yLXdpbGRmaXJlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9hcnRpY2xlLzIwMjQvanVsLzA5L2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXNlbWktZmluYWwtbWF0Y2gtcmVwb3J0LXJlc3VsdNIBdWh0dHBzOi8vYW1wLnRoZWd1YXJkaWFuLmNvbS9mb290YmFsbC9hcnRpY2xlLzIwMjQvanVsLzA5L2NvcGEtYW1lcmljYS1jYW5hZGEtYXJnZW50aW5hLXNlbWktZmluYWwtbWF0Y2gtcmVwb3J0LXJlc3VsdA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Copa America Takeaways: Canada learns valuable lesson in loss to Argentina</t>
+          <t>At Copa America, Canada’s predictable defeat comes with the promise of something bigger</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>2024-07-09 23:27:24.417838</t>
+          <t>2024-07-09 22:27:24.463530</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9jb3BhLWFtZXJpY2EtdGFrZWF3YXlzLWNhbmFkYS1sZWFybnMtdmFsdWFibGUtbGVzc29uLWluLWxvc3MtdG8tYXJnZW50aW5hL9IBcWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvY29wYS1hbWVyaWNhLXRha2Vhd2F5cy1jYW5hZGEtbGVhcm5zLXZhbHVhYmxlLWxlc3Nvbi1pbi1sb3NzLXRvLWFyZ2VudGluYS9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vc3BvcnRzL2FydGljbGUtY2FuYWRhLWFyZ2VudGluYS1jb3BhLWFtZXJpY2EtcmVzdWx0cy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Lionel Messi scores, Argentina brushes aside Canada, waltzes into Copa América final</t>
+          <t>Regulatory framework of laboratory developed tests: Canada vs U.S.</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>2024-07-09 23:27:24.426857</t>
+          <t>2024-07-09 23:26:45.075148</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMif2h0dHBzOi8vc3BvcnRzLnlhaG9vLmNvbS9saXZlL2xpb25lbC1tZXNzaS1zY29yZXMtYXJnZW50aW5hLWJydXNoZXMtYXNpZGUtY2FuYWRhLXdhbHR6ZXMtaW50by1jb3BhLWFtZXJpY2EtZmluYWwtMjMzODA1Njk1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmJsZy5jb20vZW4vaW5zaWdodHMvMjAyNC8wNy9yZWd1bGF0b3J5LWZyYW1ld29yay1vZi1sYWJvcmF0b3J5LWRldmVsb3BlZC10ZXN0cy1jYW5hZGEtdnMtdXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Canada manager Jesse Marsch postgame presser after loss to Argentina in Copa América</t>
+          <t>Canada insurers investing in fossil fuels as climate risks grow, shareholder group says</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>2024-07-09 23:27:24.433908</t>
+          <t>2024-07-09 23:26:45.090846</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLWJ0YjhhZG44ZzhwdWN0NjjSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vY2EuZmluYW5jZS55YWhvby5jb20vbmV3cy9jYW5hZGEtaW5zdXJlcnMtaW52ZXN0aW5nLWZvc3NpbC1mdWVscy0wNDA5MzY4ODIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Canada’s discourse on finfish aquaculture is environmental extremism at its finest</t>
+          <t>Heat wave bakes Texas amid power outages while Canada braces for wildfires</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>2024-07-10 00:26:45.090846</t>
+          <t>2024-07-09 23:26:45.130208</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMTAvY2FuYWRhcy1kaXNjb3Vyc2Utb24tZmluZmlzaC1hcXVhY3VsdHVyZS1pcy1lbnZpcm9ubWVudGFsLWV4dHJlbWlzbS1hdC1pdHMtZmluZXN0LzQyNzY4OS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy50aGV3ZWF0aGVybmV0d29yay5jb20vZW4vbmV3cy93ZWF0aGVyL3NldmVyZS9oZWF0LXdhdmUtYmFrZXMtdGV4YXMtYW1pZC1wb3dlci1vdXRhZ2VzLXdoaWxlLWNhbmFkYS1icmFjZXMtZm9yLXdpbGRmaXJlc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Opinion: Diversity trends, actions and results</t>
+          <t>Lionel Messi scores, Argentina brushes aside Canada, waltzes into Copa América final</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>2024-07-10 00:26:45.090846</t>
+          <t>2024-07-09 23:27:24.426857</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LnB1bHBhbmRwYXBlcmNhbmFkYS5jb20vb3Bpbmlvbi1kaXZlcnNpdHktdHJlbmRzLWFjdGlvbnMtYW5kLXJlc3VsdHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMif2h0dHBzOi8vc3BvcnRzLnlhaG9vLmNvbS9saXZlL2xpb25lbC1tZXNzaS1zY29yZXMtYXJnZW50aW5hLWJydXNoZXMtYXNpZGUtY2FuYWRhLXdhbHR6ZXMtaW50by1jb3BhLWFtZXJpY2EtZmluYWwtMjMzODA1Njk1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Feds need to be accountable as Canadian diplomats’ health-care woes persist: union head</t>
+          <t>Canada manager Jesse Marsch postgame presser after loss to Argentina in Copa América</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>2024-07-10 00:26:45.106418</t>
+          <t>2024-07-09 23:27:24.433908</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMTAvZmVkcy1uZWVkLXRvLXRha2UtYWNjb3VudGFiaWxpdHktYXMtY2FuYWRpYW4tZGlwbG9tYXRzLWhlYWx0aC1jYXJlLXdvZXMtcGVyc2lzdC11bmlvbi1oZWFkLzQyNzcwMy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLWJ0YjhhZG44ZzhwdWN0NjjSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Messi's 109th goal leads defending champion Argentina over Canada 2-0 and into Copa America final</t>
+          <t>Canada’s discourse on finfish aquaculture is environmental extremism at its finest</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>2024-07-10 00:27:24.426857</t>
+          <t>2024-07-10 00:26:45.090846</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYXBuZXdzLmNvbS9hcnRpY2xlL2NvcGEtYW1lcmljYS1tZXNzaS1jYW5hZGEtYXJnZW50aW5hLXNjb3JlLTQ4YWI4NjllODlmYWJjNzUyMGU3ZjZiMDdjYzRjMmQz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMTAvY2FuYWRhcy1kaXNjb3Vyc2Utb24tZmluZmlzaC1hcXVhY3VsdHVyZS1pcy1lbnZpcm9ubWVudGFsLWV4dHJlbWlzbS1hdC1pdHMtZmluZXN0LzQyNzY4OS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>The National | Canada’s historic Copa semifinal showdown</t>
+          <t>Opinion: Diversity trends, actions and results</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>2024-07-10 00:27:24.433908</t>
+          <t>2024-07-10 00:26:45.090846</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjQyMzYxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LnB1bHBhbmRwYXBlcmNhbmFkYS5jb20vb3Bpbmlvbi1kaXZlcnNpdHktdHJlbmRzLWFjdGlvbnMtYW5kLXJlc3VsdHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Closing the gap</t>
+          <t>Feds need to be accountable as Canadian diplomats’ health-care woes persist: union head</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>2024-07-10 00:27:24.461229</t>
+          <t>2024-07-10 00:26:45.106418</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8va3BtZy5jb20vY2EvZW4vaG9tZS9pbnNpZ2h0cy8yMDI0LzA3L2Nsb3NpbmctdGhlLWdhcC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5oaWxsdGltZXMuY29tL3N0b3J5LzIwMjQvMDcvMTAvZmVkcy1uZWVkLXRvLXRha2UtYWNjb3VudGFiaWxpdHktYXMtY2FuYWRpYW4tZGlwbG9tYXRzLWhlYWx0aC1jYXJlLXdvZXMtcGVyc2lzdC11bmlvbi1oZWFkLzQyNzcwMy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>CTV National News: Sweltering heat in Canada</t>
+          <t>Messi's 109th goal leads defending champion Argentina over Canada 2-0 and into Copa America final</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>2024-07-10 01:26:45.106418</t>
+          <t>2024-07-10 00:27:24.426857</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vYXRsYW50aWMuY3R2bmV3cy5jYS92aWRlby9jMjk1NTc0My1jdHYtbmF0aW9uYWwtbmV3cy0tc3dlbHRlcmluZy1oZWF0LWluLWNhbmFkYT9wbGF5bGlzdElkPTEuNjk1Mzk3N9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYXBuZXdzLmNvbS9hcnRpY2xlL2NvcGEtYW1lcmljYS1tZXNzaS1jYW5hZGEtYXJnZW50aW5hLXNjb3JlLTQ4YWI4NjllODlmYWJjNzUyMGU3ZjZiMDdjYzRjMmQz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>FSC Canada approves updated Group Chain of Custody criteria</t>
+          <t>The National | Canada’s historic Copa semifinal showdown</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>2024-07-10 01:26:45.106418</t>
+          <t>2024-07-10 00:27:24.433908</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LnB1bHBhbmRwYXBlcmNhbmFkYS5jb20vZnNjLWNhbmFkYS1hcHByb3Zlcy11cGRhdGVkLWdyb3VwLWNoYWluLW9mLWN1c3RvZHktY3JpdGVyaWEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjQyMzYxNjTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>CTV National News: De Rosario on Canada's run</t>
+          <t>Closing the gap</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>2024-07-10 01:26:45.131608</t>
+          <t>2024-07-10 00:27:24.461229</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY3R2bmV3cy5jYS92aWRlby9jMjk1NTc0MC1jdHYtbmF0aW9uYWwtbmV3cy0tZGUtcm9zYXJpby1vbi1jYW5hZGEtcy1ydW7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8va3BtZy5jb20vY2EvZW4vaG9tZS9pbnNpZ2h0cy8yMDI0LzA3L2Nsb3NpbmctdGhlLWdhcC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>What is teqball?</t>
+          <t>CTV National News: Sweltering heat in Canada</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>2024-07-10 01:27:24.433908</t>
+          <t>2024-07-10 01:26:45.106418</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDI1MjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vYXRsYW50aWMuY3R2bmV3cy5jYS92aWRlby9jMjk1NTc0My1jdHYtbmF0aW9uYWwtbmV3cy0tc3dlbHRlcmluZy1oZWF0LWluLWNhbmFkYT9wbGF5bGlzdElkPTEuNjk1Mzk3N9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Canada's Copa América success lays groundwork for World Cup: "The goal is 2026"</t>
+          <t>FSC Canada approves updated Group Chain of Custody criteria</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>2024-07-10 01:27:24.465540</t>
+          <t>2024-07-10 01:26:45.106418</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3Lm1sc3NvY2Nlci5jb20vbmV3cy9jYW5hZGEtcy1jb3BhLWFtZXJpY2Etc3VjY2Vzcy1sYXlzLWdyb3VuZHdvcmstZm9yLXdvcmxkLWN1cC10aGUtZ29hbC1pcy0yMDI20gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LnB1bHBhbmRwYXBlcmNhbmFkYS5jb20vZnNjLWNhbmFkYS1hcHByb3Zlcy11cGRhdGVkLWdyb3VwLWNoYWluLW9mLWN1c3RvZHktY3JpdGVyaWEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
+          <t>CTV National News: De Rosario on Canada's run</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>2024-07-10 01:26:45.131608</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vY3R2bmV3cy5jYS92aWRlby9jMjk1NTc0MC1jdHYtbmF0aW9uYWwtbmV3cy0tZGUtcm9zYXJpby1vbi1jYW5hZGEtcy1ydW7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>What is teqball?</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>2024-07-10 01:27:24.433908</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDI1MjHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Canada's Copa América success lays groundwork for World Cup: "The goal is 2026"</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>2024-07-10 01:27:24.465540</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3Lm1sc3NvY2Nlci5jb20vbmV3cy9jYW5hZGEtcy1jb3BhLWFtZXJpY2Etc3VjY2Vzcy1sYXlzLWdyb3VuZHdvcmstZm9yLXdvcmxkLWN1cC10aGUtZ29hbC1pcy0yMDI20gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
           <t>Zachary Patterson: Canada must reclaim its wayward universities. Here’s how</t>
         </is>
       </c>
-      <c r="B196" t="inlineStr">
+      <c r="B199" t="inlineStr">
         <is>
           <t>2024-07-10 02:27:24.433908</t>
         </is>
       </c>
-      <c r="C196" t="inlineStr">
+      <c r="C199" t="inlineStr">
         <is>
           <t>news.google.com/articles/CBMiZmh0dHBzOi8vdGhlaHViLmNhLzIwMjQvMDcvMTAvemFjaGFyeS1wYXR0ZXJzb24tY2FuYWRhLW11c3QtcmVjbGFpbS1pdHMtd2F5d2FyZC11bml2ZXJzaXRpZXMtaGVyZXMtaG93L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Team Canada’s Paris 2024 women’s rugby sevens team unveiled</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:45.448172</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC13b21lbnMtcnVnYnktc2V2ZW5zLXRlYW0tdW52ZWlsZWQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Argentina earns 2-0 win over gutsy Canada in Copa America semifinal</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE0MzUwL2FyZ2VudGluYS13aW5zLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtY2FuYWRhL9IBVWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE0MzUwL2FyZ2VudGluYS13aW5zLWNvcGEtYW1lcmljYS1zZW1pZmluYWwtY2FuYWRhL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Team Canada unveils men's basketball roster for Paris Olympics</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9vbHltcGljcy9hcnRpY2xlL3RlYW0tY2FuYWRhLXVudmVpbHMtbWVucy1iYXNrZXRiYWxsLXJvc3Rlci1mb3ItcGFyaXMtb2x5bXBpY3Mv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Israeli arms firm taking Canada to court after military contract disqualification</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvaXNyYWVsaS1hcm1zLWZpcm0tdGFraW5nLWNhbmFkYS10by1jb3VydC1hZnRlci1taWxpdGFyeS1jb250cmFjdC1kaXNxdWFsaWZpY2F0aW9uLTEuNjk1Nzg1M9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Prince of Wales Fort National Historic Site</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiKWh0dHBzOi8vcGFya3MuY2FuYWRhLmNhL2xobi1uaHMvbWIvcHJpbmNl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Canada pledges Ukraine aid, plan to buy submarines as NATO spending questions follow Trudeau</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.927128</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5jdHZuZXdzLmNhL3BvbGl0aWNzL2NhbmFkYS1wbGVkZ2VzLXVrcmFpbmUtYWlkLXBsYW4tdG8tYnV5LXN1Ym1hcmluZXMtYXMtbmF0by1zcGVuZGluZy1xdWVzdGlvbnMtZm9sbG93LXRydWRlYXUtMS42OTU4MTQ40gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Team Canada reveals women’s rugby sevens squad for Paris 2024</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzEwL3RlYW0tY2FuYWRhLXJldmVhbHMtd29tZW5zLXJ1Z2J5LXNldmVucy1zcXVhZC1mb3ItcGFyaXMtMjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Team Canada men’s basketball ready to compete at first Olympic Games since 2000</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibWh0dHBzOi8vb2x5bXBpYy5jYS8yMDI0LzA3LzEwL3RlYW0tY2FuYWRhLW1lbnMtYmFza2V0YmFsbC1yZWFkeS10by1jb21wZXRlLWF0LWZpcnN0LW9seW1waWMtZ2FtZXMtc2luY2UtMjAwMC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Water safety, by the numbers</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LnN0YXRjYW4uZ2MuY2EvbzEvZW4vcGx1cy82NjI0LXdhdGVyLXNhZmV0eS1udW1iZXJzP3diZGlzYWJsZT10cnVl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Canada to stop processing study permits for colleges, universities that fail to track international students</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiwQFodHRwczovL3d3dy50aGVzdGFyLmNvbS9uZXdzL2NhbmFkYS9jYW5hZGEtdG8tc3RvcC1wcm9jZXNzaW5nLXN0dWR5LXBlcm1pdHMtZm9yLWNvbGxlZ2VzLXVuaXZlcnNpdGllcy10aGF0LWZhaWwtdG8tdHJhY2staW50ZXJuYXRpb25hbC1zdHVkZW50cy9hcnRpY2xlXzdjNmU3NTdlLTNkN2YtMTFlZi05MjhmLWQ3ZjM2ZWQ1ZTA3MC5odG1s0gHFAWh0dHBzOi8vd3d3LnRoZXN0YXIuY29tL25ld3MvY2FuYWRhL2NhbmFkYS10by1zdG9wLXByb2Nlc3Npbmctc3R1ZHktcGVybWl0cy1mb3ItY29sbGVnZXMtdW5pdmVyc2l0aWVzLXRoYXQtZmFpbC10by10cmFjay1pbnRlcm5hdGlvbmFsLXN0dWRlbnRzL2FydGljbGVfN2M2ZTc1N2UtM2Q3Zi0xMWVmLTkyOGYtZDdmMzZlZDVlMDcwLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Some plant-based milks recalled in Canada due to listeria risk</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vY2FiaW5yYWRpby5jYS8xOTIxMDkvbmV3cy9oZWFsdGgvc29tZS1wbGFudC1iYXNlZC1taWxrcy1yZWNhbGxlZC1pbi1jYW5hZGEtZHVlLXRvLWxpc3RlcmlhLXJpc2sv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Windsor soccer fans proud of 'absolutely electric' run by Team Canada at Copa America</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vd2luZHNvci5jdHZuZXdzLmNhL3dpbmRzb3Itc29jY2VyLWZhbnMtcHJvdWQtb2YtYWJzb2x1dGVseS1lbGVjdHJpYy1ydW4tYnktdGVhbS1jYW5hZGEtYXQtY29wYS1hbWVyaWNhLTEuNjk1NzgzONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Canada's airport fire rules risking passengers' lives, firefighters warn</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9vdHRhd2EvY2FuYWRhLXMtYWlycG9ydC1maXJlLXJ1bGVzLXJpc2tpbmctcGFzc2VuZ2Vycy1saXZlcy1maXJlZmlnaHRlcnMtd2Fybi0xLjcyNTg1MzjSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1ODUzOA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Canada's defence spending is 'shameful,' says U.S. Speaker, falling at bottom of the pack at NATO</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy5jdHZuZXdzLmNhL3BvbGl0aWNzL2NhbmFkYS1zLWRlZmVuY2Utc3BlbmRpbmctaXMtc2hhbWVmdWwtc2F5cy11LXMtc3BlYWtlci1mYWxsaW5nLWF0LWJvdHRvbS1vZi10aGUtcGFjay1hdC1uYXRvLTEuNjk1Nzk2NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>iHeartRadio Canada (@iheartradioca)</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.960576</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiKGh0dHBzOi8vd3d3Lmluc3RhZ3JhbS5jb20vaWhlYXJ0cmFkaW9jYS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Team USA opens USA Basketball Showcase vs. Canada</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.961451</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3Lm5iYS5jb20vbmV3cy90ZWFtLXVzYS1vcGVucy11c2EtYmFza2V0YmFsbC1zaG93Y2FzZS12cy1jYW5hZGHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Chinese Ambassador to Canada H.E. Wang Di met with Ms. Larissa Bezo, President and CEO of the Canadian Bureau of International Education, and Ms. Karen Dalkie, Vice President of CBIE_Embassy of the People's Republic of China in Canada</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>2024-07-10 12:19:55.966502</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiRWh0dHA6Ly9jYS5jaGluYS1lbWJhc3N5Lmdvdi5jbi9lbmcvc2d4dy8yMDI0MDcvdDIwMjQwNzExXzExNDUxODIwLmh0bdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>Canada finalizes its men’s Olympic basketball roster, with 8 returnees from World Cup team</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>2024-07-10 13:19:45.422934</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vYXBuZXdzLmNvbS9hcnRpY2xlL29seW1waWNzLWNhbmFkYS1iYXNrZXRiYWxsLTIwMjQtcGFyaXMtZjdhZWM2MDlmNDBhMzI2ZDY5MDgyMGRkYzYxYWJkNWXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>GTA under flood watch amid heavy rain</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>2024-07-10 13:19:45.422934</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS90b3JvbnRvL3JhaW5mYWxsLXdhcm5pbmctdG9yb250by1odXJyaWNhbi1iZXJ5bC0xLjcyNTkxMDDSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1OTEwMA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Canada Announces 12 Man Roster for Paris Olympics</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>2024-07-10 13:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vd3d3LnNpLmNvbS9uYmEvcmFwdG9ycy9jYW5hZGEtYW5ub3VuY2VzLWl0cy0xMi1tYW4tcm9zdGVyLWZvci1wYXJpcy1vbHltcGljc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Canadian men's basketball team faces U.S. in exhibition ahead of Paris Olympics</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>2024-07-10 13:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvb2x5bXBpY3Mvc3VtbWVyL2Jhc2tldGJhbGwvY2FuYWRhLXVzYS1vbHltcGljLW1lbnMtYmFza2V0YmFsbC1leGhpYml0aW9uLTEuNzI1OTEyMtIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU5MTIy?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Air Canada must inform public that some Canadians are excluded from class action: Quebec judge</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>2024-07-10 13:19:55.961451</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMigwFodHRwczovL21vbnRyZWFsLmN0dm5ld3MuY2EvYWlyLWNhbmFkYS1tdXN0LWluZm9ybS1wdWJsaWMtdGhhdC1zb21lLWNhbmFkaWFucy1hcmUtZXhjbHVkZWQtZnJvbS1jbGFzcy1hY3Rpb24tcXVlYmVjLWp1ZGdlLTEuNjk1ODQ5NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Tech Support</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>2024-07-10 14:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiOGh0dHBzOi8vbWVudGFsaGVhbHRoY29tbWlzc2lvbi5jYS9jYXRhbHlzdC90ZWNoLXN1cHBvcnQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Canada warns of AI-driven Russian 'bot farm' spreading disinformation online</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>2024-07-10 14:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2NhbmFkYS1ydXNzaWFuLWJvdC1mYXJtLTEuNzI1OTY2NdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU5NjY1?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Gilgeous-Alexander, Murray to lead NBA-experienced Canadian Olympic team in Paris</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>2024-07-10 14:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvb2x5bXBpY3Mvc3VtbWVyL2Jhc2tldGJhbGwvY2FuYWRhLW9seW1waWMtbWVucy1iYXNrZXRiYWxsLXJvc3Rlci1wYXJpcy0xLjcyNTkzMDHSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1OTMwMQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Two Quebecers to represent Team Canada basketball at the Paris Olympics</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>2024-07-10 14:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibWh0dHBzOi8vbW9udHJlYWwuY3R2bmV3cy5jYS90d28tcXVlYmVjZXJzLXRvLXJlcHJlc2VudC10ZWFtLWNhbmFkYS1iYXNrZXRiYWxsLWF0LXRoZS1wYXJpcy1vbHltcGljcy0xLjY5NTg1NzPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Canada to announce plan to reach NATO target, spend 2% of GDP on defence: sources</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>2024-07-10 15:19:55.895030</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY2FuYWRhLXRvLWFubm91bmNlLXBsYW4tdG8tcmVhY2gtbmF0by10YXJnZXQtc3BlbmQtMi1vZi1nZHAtb24tZGVmZW5jZS1zb3VyY2VzLTEuNjk1ODY3ONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Canada confirms plan to replace submarine fleet at NATO summit</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>2024-07-10 15:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL3N1Ym1hcmluZS1ibGFpci10cnVkZWF1LW5hdG8tMS43MjU5NzE40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTk3MTg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Average asking rent in Canada up 7% from a year ago, even as price growth slows</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>2024-07-10 15:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiPmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2J1c2luZXNzL3JlbnRhbHMtcmVwb3J0LWp1bmUtMS43MjU5MjEy0gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTkyMTI?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Marsch noncommittal on status of Davies for Canada’s third-place match at Copa America</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>2024-07-10 15:19:55.945152</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9zb2NjZXIvYXJ0aWNsZS9tYXJzaC1ub25jb21taXR0YWwtb24tc3RhdHVzLW9mLWRhdmllcy1mb3ItY2FuYWRhcy10aGlyZC1wbGFjZS1tYXRjaC1hdC1jb3BhLWFtZXJpY2Ev0gF8aHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL3NvY2Nlci9tYXJzaC1ub25jb21taXR0YWwtb24tc3RhdHVzLW9mLWRhdmllcy1mb3ItY2FuYWRhcy10aGlyZC1wbGFjZS1tYXRjaC1hdC1jb3BhLWFtZXJpY2Evc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Canada to announce plan to reach NATO target, spending 2% of GDP on defence</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>2024-07-10 15:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LmN0dm5ld3MuY2EvcG9saXRpY3MvY2FuYWRhLXRvLWFubm91bmNlLXBsYW4tdG8tcmVhY2gtbmF0by10YXJnZXQtc3BlbmRpbmctMi1vZi1nZHAtb24tZGVmZW5jZS0xLjY5NTg2NzjSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Hundreds of migrant farm workers unionize in B.C.</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>2024-07-10 15:19:55.966502</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL211c2hyb29tLWZhcm0tdW5pb24tMS43MjU4OTkz0gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTg5OTM?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Canada commits to buying 12 new conventionally-powered, under-the-ice submarines</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vYnJlYWtpbmdkZWZlbnNlLmNvbS8yMDI0LzA3L2NhbmFkYS1jb21taXRzLXRvLWJ1eWluZy0xMi1uZXctY29udmVudGlvbmFsbHktcG93ZXJlZC11bmRlci10aGUtaWNlLXN1Ym1hcmluZXMv0gF6aHR0cHM6Ly9icmVha2luZ2RlZmVuc2UuY29tLzIwMjQvMDcvY2FuYWRhLWNvbW1pdHMtdG8tYnV5aW5nLTEyLW5ldy1jb252ZW50aW9uYWxseS1wb3dlcmVkLXVuZGVyLXRoZS1pY2Utc3VibWFyaW5lcy8_YW1wPTE?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Canada pledges Ukraine aid, plan to buy submarines as NATO spending questions dog PM</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.910857</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vbmF0aW9uYWxwb3N0LmNvbS9uZXdzL2NhbmFkYS9jYW5hZGEtdWtyYWluZS1haWQtc3VibWFyaW5lcy1uYXRv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Canada to unveil NATO spending plan, details ‘first step’ on new submarines</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTWh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE1MTk0L2NhbmFkYS1zdWJtYXJpbmVzLXB1cmNoYXNlLW5hdG8tbWlsaXRhcnkv0gFRaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTUxOTQvY2FuYWRhLXN1Ym1hcmluZXMtcHVyY2hhc2UtbmF0by1taWxpdGFyeS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Niagara no longer under tornado watch, rainfall warnings for area continue</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9oYW1pbHRvbi90b3JuYWRvLXdhdGNoLW5pYWdhcmEtMS43MjU5MzA30gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTkzMDc?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Canada promises $500M in military aid to Ukraine as part of NATO package</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiogFodHRwczovL3d3dy50aGVzdGFyLmNvbS9wb2xpdGljcy9mZWRlcmFsL2NhbmFkYS1wcm9taXNlcy01MDBtLWluLW1pbGl0YXJ5LWFpZC10by11a3JhaW5lLWFzLXBhcnQtb2YtbmF0by1wYWNrYWdlL2FydGljbGVfM2NhOGQyZTItM2VjYy0xMWVmLWIxMDAtNmZmZTYzYTM3N2IwLmh0bWzSAaYBaHR0cHM6Ly93d3cudGhlc3Rhci5jb20vcG9saXRpY3MvZmVkZXJhbC9jYW5hZGEtcHJvbWlzZXMtNTAwbS1pbi1taWxpdGFyeS1haWQtdG8tdWtyYWluZS1hcy1wYXJ0LW9mLW5hdG8tcGFja2FnZS9hcnRpY2xlXzNjYThkMmUyLTNlY2MtMTFlZi1iMTAwLTZmZmU2M2EzNzdiMC5hbXAuaHRtbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Has Canada’s hog industry turned the corner?</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.944289</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3LmZjYy1mYWMuY2EvZW4va25vd2xlZGdlL2Vjb25vbWljcy9jYW5hZGEtaG9nLXNlY3Rvci1wcmVzc3VyZWQtcHJvZml0YWJpbGl0eS0yMDI00gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Hudson's Bay closes several stores across Canada during heat wave</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2h1ZHNvbnMtYmF5LWhlYXR3YXZlLTEuNzI1OTcyMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU5NzIx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Deal reached to 'peacefully end' encampment at University of Windsor</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS93aW5kc29yL3Byby1wYWxlc3Rpbmlhbi1lbmNhbXBtZW50LWRlYWwtMS43MjU5NTU50gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTk1NTk?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Interpol data confirms Canada is ‘ground zero’ for car thefts: experts</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE1MTE2L2NhbmFkYS1zdG9sZW4tdmVoaWNsZXMtYXV0by10aGVmdC1pbnRlcnBvbC_SAVNodHRwczovL2dsb2JhbG5ld3MuY2EvbmV3cy8xMDYxNTExNi9jYW5hZGEtc3RvbGVuLXZlaGljbGVzLWF1dG8tdGhlZnQtaW50ZXJwb2wvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Strathcona, Canada Growth Fund partner on $2-billion carbon capture project for oil sands</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>2024-07-10 16:19:55.961451</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vYnVzaW5lc3MvYXJ0aWNsZS1zdHJhdGhjb25hLWNhbmFkYS1ncm93dGgtZnVuZC1vaWwtc2FuZHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Team Canada’s Paris 2024 men’s basketball team unveiled</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vb2x5bXBpYy5jYS9wcmVzcy90ZWFtLWNhbmFkYXMtcGFyaXMtMjAyNC1tZW5zLWJhc2tldGJhbGwtdGVhbS11bnZlaWxlZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>How to watch Copa America 2024 in Canada: Live streams, TV channels, full schedule &amp; more</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifmh0dHBzOi8vd3d3LnNwb3J0aW5nbmV3cy5jb20vY2Evc29jY2VyL25ld3MvaG93LXdhdGNoLWNvcGEtYW1lcmljYS0yMDI0LWNhbmFkYS1saXZlLXN0cmVhbS10di1jaGFubmVsL2FjMDM1ZWNjMTBmNzUwNzA5Mzg3M2E5MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Edmonton Oilers goalie Stuart Skinner named to projected Team Canada tournament squad but not everyone loving it</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:45.448172</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vZWRtb250b25qb3VybmFsLmNvbS9zcG9ydHMvaG9ja2V5L25obC9jdWx0LW9mLWhvY2tleS9zdHVhcnQtc2tpbm5lci10ZWFtLWNhbmFkYS1nb2FsaWUtZm91ci1uYXRpb25zLXRvdXJuYW1lbnTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Canada coach Marsch sees many positives in Copa campaign but says more work needed</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvc29jY2VyL2NhbmFkYS1jb3BhLWFtZXJpY2EtZXZhbHVhdGlvbi1qZXNzZS1tYXJzY2gtMS43MjU5OTg00gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNTk5ODQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Surging optimism as Canada continues to shock the soccer world at Copa America</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmN0dm5ld3MuY2Evc3BvcnRzL3N1cmdpbmctb3B0aW1pc20tYXMtY2FuYWRhLWNvbnRpbnVlcy10by1zaG9jay10aGUtc29jY2VyLXdvcmxkLWF0LWNvcGEtYW1lcmljYS0xLjY5NTg5MzPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Opinion | Canada Is a NATO Scofflaw</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vd3d3Lndzai5jb20vYXJ0aWNsZXMvY2FuYWRhLW5hdG8tZGVmZW5zZS1zcGVuZGluZy1qdXN0aW4tdHJ1ZGVhdS03YWUyYzc2NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Canada makes submarine procurement announcement after days of defence-spending criticism from NATO allies</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMif2h0dHBzOi8vd3d3LnRoZWdsb2JlYW5kbWFpbC5jb20vd29ybGQvdXMtcG9saXRpY3MvYXJ0aWNsZS1jYW5hZGEtbWFrZXMtZGVmZW5jZS1hbm5vdW5jZW1lbnRzLWFmdGVyLWRheXMtb2YtY3JpdGljaXNtLWZyb20tbmF0by_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Atlantic Canada next in line for a soaking, flood risk from Beryl remnants</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy50aGV3ZWF0aGVybmV0d29yay5jb20vZW4vbmV3cy93ZWF0aGVyL2ZvcmVjYXN0cy9hdGxhbnRpYy1jYW5hZGEtbmV4dC1pbi1saW5lLWZvci1hLXNvYWtpbmctZmxvb2Qtcmlzay1mcm9tLWJlcnlsLXJlbW5hbnRz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>'I'm just so proud of them': Former Winnipegger in stands cheering on Canada at Copa America 2024 semifinals</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3dpbm5pcGVnLmN0dm5ld3MuY2EvaS1tLWp1c3Qtc28tcHJvdWQtb2YtdGhlbS1mb3JtZXItd2lubmlwZWdnZXItaW4tc3RhbmRzLWNoZWVyaW5nLW9uLWNhbmFkYS1hdC1jb3BhLWFtZXJpY2EtMjAyNC1zZW1pZmluYWxzLTEuNjk1ODkwMNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Conrad Black, who battled Chrétien over British peerage, removed from U.K. House of Lords</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>2024-07-10 17:19:55.961451</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL2NvbnJhZC1ibGFjay1yZW1vdmVkLWhvdXNlLW9mLWxvcmRzLTEuNzI1OTk0ONIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU5OTQ4?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Ford digs in on booze sales expansion plan as LCBO strike drags on</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>2024-07-10 18:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS90b3JvbnRvL2xjYm8tc3RyaWtlLWZvcmQtYmV0aGxlbmZhbHZ5LTEuNzI1OTEyMdIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjU5MTIx?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Eels on a plane: Slippery specimens escape aircraft at Vancouver airport</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>2024-07-10 18:19:45.448172</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE1OTk5L2VlbHMtcGxhbmUtYWlyLWNhbmFkYS1lc2NhcGUtdmlkZW8v0gFLaHR0cHM6Ly9nbG9iYWxuZXdzLmNhL25ld3MvMTA2MTU5OTkvZWVscy1wbGFuZS1haXItY2FuYWRhLWVzY2FwZS12aWRlby9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Source Atlantic being sold to Lawson Canada</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>2024-07-10 18:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LmNvdW50cnk5NC5jYS8yMDI0LzA3LzEwL3NvdXJjZS1hdGxhbnRpYy1iZWluZy1zb2xkLXRvLWxhd3Nvbi1jYW5hZGEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Costco to increase annual membership fee to $65 this September</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>2024-07-10 18:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZ2h0dHBzOi8vd3d3LmN0dm5ld3MuY2EvYnVzaW5lc3MvY29zdGNvLXRvLWluY3JlYXNlLWFubnVhbC1tZW1iZXJzaGlwLWZlZS10by02NS10aGlzLXNlcHRlbWJlci0xLjY5NTkwOTfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Federal government to offer NATO a 'timeline' for boosting defence spending</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>2024-07-10 18:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL3BvbGl0aWNzL25hdG8tY2FuYWRhLXR3by1wZXJjZW50LWdkcC0xLjcyNjAwNzTSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI2MDA3NA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Newfoundland fish harvesters crash news conference to demand reinstating of cod moratorium</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>2024-07-10 19:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9uZXdmb3VuZGxhbmQtbGFicmFkb3IvY29kLW1vcmF0b3JpdW0tcHJvdGVzdGVycy0xLjcyNTk3MzXSASBodHRwczovL3d3dy5jYmMuY2EvYW1wLzEuNzI1OTczNQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Alberta will see more frequent extreme weather: Environment Canada</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>2024-07-10 19:19:45.448172</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS92aWRlby8xMDYxNjI4NC9hbGJlcnRhLXdpbGwtc2VlLW1vcmUtZnJlcXVlbnQtZXh0cmVtZS13ZWF0aGVyLWVudmlyb25tZW50LWNhbmFkYdIBa2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS92aWRlby8xMDYxNjI4NC9hbGJlcnRhLXdpbGwtc2VlLW1vcmUtZnJlcXVlbnQtZXh0cmVtZS13ZWF0aGVyLWVudmlyb25tZW50LWNhbmFkYS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Eels writhe on Vancouver airport tarmac after escaping from box</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>2024-07-10 19:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2VlbHMtdmFuY291dmVyLWFpcnBvcnQtdGFybWFjLTEuNzI2MDEzM9IBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjYwMTMz?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Marsch: Copa can 'change trajectory' of Canada</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>2024-07-10 19:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vd3d3LmVzcG4uY29tL3NvY2Nlci9zdG9yeS9fL2lkLzQwNTM1MTcwL2NvcGEtYW1lcmljYS1jYW5hZGEtamVzc2UtbWFyc2NoLXR1cm5pbmctcG9pbnQtc29jY2Vy0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Canada's soccer success fuels youth participation</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWGh0dHBzOi8vc2Fza2F0b29uLmN0dm5ld3MuY2EvY2FuYWRhLXMtc29jY2VyLXN1Y2Nlc3MtZnVlbHMteW91dGgtcGFydGljaXBhdGlvbi0xLjY5NTkyNTTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Team Canada rises above racist comment, wins world ball hockey championship</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE1MzgwL2NhbmFkYS1iYWxsLWhvY2tleS1yYWNpc20td29ybGQtY2hhbXBpb25zL9IBUmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE1MzgwL2NhbmFkYS1iYWxsLWhvY2tleS1yYWNpc20td29ybGQtY2hhbXBpb25zL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Workers at Shell's Canada unit ratify new deal</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3LnJldXRlcnMuY29tL21hcmtldHMvY29tbW9kaXRpZXMvd29ya2Vycy1zaGVsbHMtc2NvdGZvcmQtZmFjaWxpdHktY2FuYWRhLXN0cmlrZS1uZXctd2FnZS1kZWFsLTIwMjQtMDctMTEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Canada criticized for NATO spending</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vYXRsYW50aWMuY3R2bmV3cy5jYS9tb3JlL2NhbmFkYS1jcml0aWNpemVkLWZvci1uYXRvLXNwZW5kaW5nLTEuNjk1OTI4NtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Ontario Issues 1,666 Canada Immigration Invitations To International Graduates</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiaWh0dHBzOi8vd3d3LmltbWlncmF0aW9uLmNhL29udGFyaW8taXNzdWVzLTE2NjYtY2FuYWRhLWltbWlncmF0aW9uLWludml0YXRpb25zLXRvLWludGVybmF0aW9uYWwtZ3JhZHVhdGVzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>The encampment is gone. Protesters say McGill went about it the wrong way</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9tb250cmVhbC9tY2dpbGwtZW5jYW1wbWVudC1kaXNtYW50bGVkLTEuNzI2MDAwONIBIGh0dHBzOi8vd3d3LmNiYy5jYS9hbXAvMS43MjYwMDA4?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>How the historic Canadian men's Olympic roster came together</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMicWh0dHBzOi8vd3d3LnRzbi5jYS9vbHltcGljcy9qb3NoLWxld2VuYmVyZy1ob3ctdGhlLWhpc3RvcmljLWNhbmFkaWFuLW1lbi1zLW9seW1waWMtcm9zdGVyLWNhbWUtdG9nZXRoZXItMS4yMTQ2OTM20gFwaHR0cHM6Ly93d3cudHNuLmNhL2pvc2gtbGV3ZW5iZXJnLWhvdy10aGUtaGlzdG9yaWMtY2FuYWRpYW4tbWVuLXMtb2x5bXBpYy1yb3N0ZXItY2FtZS10b2dldGhlci0xLjIxNDY5MzY_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Over 300 properties on alert as dozens of new B.C. wildfires burn</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>2024-07-10 20:19:55.961451</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LmNiYy5jYS9uZXdzL2NhbmFkYS9icml0aXNoLWNvbHVtYmlhL2JjLXdpbGRmaXJlLWp1bHktMTAtMjAyNC1kYXdzb24tY3JlZWstMS43MjYwMDY40gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNjAwNjg?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Happy Belated Canada Day! Barrhaven Is A True Reflection Of Our Nation</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>2024-07-10 21:19:45.391596</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMicWh0dHBzOi8vYmFycmhhdmVuaW5kZXBlbmRlbnQuY2EvMjAyNC8wNy8xMC9oYXBweS1iZWxhdGVkLWNhbmFkYS1kYXktYmFycmhhdmVuLWlzLWEtdHJ1ZS1yZWZsZWN0aW9uLW9mLW91ci1uYXRpb24v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>EDITORIAL: How should Canada play its role on the world’s stage</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>2024-07-10 21:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LmtlbG93bmFjYXBuZXdzLmNvbS9vcGluaW9uL2VkaXRvcmlhbC1ob3ctc2hvdWxkLWNhbmFkYS1wbGF5LWl0cy1yb2xlLW9uLXRoZS13b3JsZHMtc3RhZ2UtNzQzMjY0NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>NATO summit: Canada to buy up to 12 conventional submarines for Arctic defence</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>2024-07-10 21:19:45.422934</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vZ2xvYmFsbmV3cy5jYS92aWRlby8xMDYxNjQyNi9uYXRvLXN1bW1pdC1jYW5hZGEtdG8tYnV5LXVwLXRvLTEyLWNvbnZlbnRpb25hbC1zdWJtYXJpbmVzLWZvci1hcmN0aWMtZGVmZW5jZdIBd2h0dHBzOi8vZ2xvYmFsbmV3cy5jYS92aWRlby8xMDYxNjQyNi9uYXRvLXN1bW1pdC1jYW5hZGEtdG8tYnV5LXVwLXRvLTEyLWNvbnZlbnRpb25hbC1zdWJtYXJpbmVzLWZvci1hcmN0aWMtZGVmZW5jZS9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>Costco memberships are going up in Canada</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>2024-07-10 21:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vd3d3Lmluc2F1Z2EuY29tL2Nvc3Rjby1tZW1iZXJzaGlwcy1hcmUtZ29pbmctdXAtaW4tY2FuYWRhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>Colombia advances to Copa America final; Uruguay to meet Canada for third</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>2024-07-10 21:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvY29sb21iaWEtYWR2YW5jZXMtdG8tY29wYS1hbWVyaWNhLWZpbmFsLXVydWd1YXktdG8tbWVldC1jYW5hZGEtaW4tdGhpcmQtcGxhY2UtZ2FtZS0xLjIxNDY5NTHSAXdodHRwczovL3d3dy50c24uY2EvY29sb21iaWEtYWR2YW5jZXMtdG8tY29wYS1hbWVyaWNhLWZpbmFsLXVydWd1YXktdG8tbWVldC1jYW5hZGEtaW4tdGhpcmQtcGxhY2UtZ2FtZS0xLjIxNDY5NTE_dHNuLWFtcA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>‘Increases’: Costco announces changes to membership fees in Canada and people online have mixed reactions</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>2024-07-10 21:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMivgFodHRwczovL3d3dy5pbnNpZGVoYWx0b24uY29tL2J1c2luZXNzL2luY3JlYXNlcy1jb3N0Y28tYW5ub3VuY2VzLWNoYW5nZXMtdG8tbWVtYmVyc2hpcC1mZWVzLWluLWNhbmFkYS1hbmQtcGVvcGxlLW9ubGluZS1oYXZlLW1peGVkLXJlYWN0aW9ucy9hcnRpY2xlXzJkY2Q5ZjJlLTkyYTktNTUwOS1iYzM0LTBiNDM1NWRhNzg3Yi5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Forge defeats slumping Toronto FC in opening leg of Canadian Championship semifinal</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>2024-07-10 22:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMieGh0dHBzOi8vZ2xvYmFsbmV3cy5jYS9uZXdzLzEwNjE2NTE0L2ZvcmdlLWRlZmVhdHMtc2x1bXBpbmctdG9yb250by1mYy1pbi1vcGVuaW5nLWxlZy1vZi1jYW5hZGlhbi1jaGFtcGlvbnNoaXAtc2VtaWZpbmFsL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>Canada pledges nearly $370 million in military aid for Ukraine.</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>2024-07-10 22:19:55.961451</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8va3lpdmluZGVwZW5kZW50LmNvbS9jYW5hZGEtcGxlZGdlcy1uZWFybHktMzcwLW1pbGxpb24taW4tbWlsaXRhcnktYWlkLWZvci11a3JhaW5lL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>NATO confirms F-16s for Ukraine, Canada announces plans for new sub fleet</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>2024-07-10 22:19:55.966502</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDQ4ODnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Bold Experiment or Safety Risk? Canada Is Divided on How to Stop Drug Deaths.</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>2024-07-10 23:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vd3d3Lm55dGltZXMuY29tLzIwMjQvMDcvMTEvd29ybGQvY2FuYWRhL2NhbmFkYS1vcGlvaWQtY3Jpc2lzLWRlY3JpbWluYWxpemF0aW9uLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Steph Curry, Anthony Davis lead Team USA in exhibition game vs. Canada / News</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vYmFza2V0bmV3cy5jb20vbmV3cy0yMDkwMTUtc3RlcGgtY3VycnktYW50aG9ueS1kYXZpcy1sZWFkLXRlYW0tdXNhLWluLWV4aGliaXRpb24tZ2FtZS12cy1jYW5hZGEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>Vancouver fans proud of Canada despite loss to Argentina in historic soccer game</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:45.422934</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmNiYy5jYS9wbGF5ZXIvcGxheS92aWRlby85LjY0NDQ0ODHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>How does Canada stack up with Uruguay?</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:45.422934</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vd3d3LnRzbi5jYS92aWRlby9ob3ctZG9lcy1jYW5hZGEtc3RhY2stdXAtd2l0aC11cnVndWF5fjI5NTYwMTDSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>U.S. tops Canada in Olympic men's basketball exhibition</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.895030</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3LmNiYy5jYS9zcG9ydHMvb2x5bXBpY3Mvc3VtbWVyL2Jhc2tldGJhbGwvY2FuYWRhLXVzYS1vbHltcGljLW1lbnMtYmFza2V0YmFsbC1leGhpYml0aW9uLXJlY2FwLWp1bHktMTAtMS43MjYwMDU00gEgaHR0cHM6Ly93d3cuY2JjLmNhL2FtcC8xLjcyNjAwNTQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Whitecaps edge Pacific FC in Canadian Championship semifinal</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LnRzbi5jYS9zb2NjZXIvd2hpdGVjYXBzLWVkZ2UtcGFjaWZpYy1pbi1vcGVuaW5nLWxlZy1vZi1jYW5hZGlhbi1jaGFtcGlvbnNoaXAtc2VtaWZpbmFsLTEuMjE0Njk5MtIBbWh0dHBzOi8vd3d3LnRzbi5jYS93aGl0ZWNhcHMtZWRnZS1wYWNpZmljLWluLW9wZW5pbmctbGVnLW9mLWNhbmFkaWFuLWNoYW1waW9uc2hpcC1zZW1pZmluYWwtMS4yMTQ2OTkyP3Rzbi1hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>USA Basketball tops Canada 86-72 in exhibition opener on the road to Paris Olympics</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vYXBuZXdzLmNvbS9hcnRpY2xlL2NhbmFkYS11c2EtYmFza2V0YmFsbC1wYXJpcy1vbHltcGljcy05MWRhN2RlZGMxYzQ2ODUzNDEwZDgzNmI3MWIxNTBjN9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>Team USA defeats medal contender Canada in first Olympic basketball tune-up</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LnVzYXRvZGF5LmNvbS9zdG9yeS9zcG9ydHMvb2x5bXBpY3MvMjAyNC8wNy8xMS91c2EtY2FuYWRhLWJhc2tldGJhbGwtZXhoaWJpdGlvbi1wYXJpcy1vbHltcGljcy83NDM2MTkwODAwNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>USA defeat Canada in summer premiere</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LmZpYmEuYmFza2V0YmFsbC9lbi9ldmVudHMvbWVucy1vbHltcGljLWJhc2tldGJhbGwtdG91cm5hbWVudC1wYXJpcy0yMDI0L25ld3MvdXNhLWJlYXQtY2FuYWRhLWluLXN1bW1lci1wcmVtaWVyZdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>Canada vs. United States Highlights | USA Basketball Showcase</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiNGh0dHBzOi8vd3d3LmZveHNwb3J0cy5jb20vd2F0Y2gvZm1jLXg2Nno5ZWhjM3Z0N3phcXHSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>Canada takes step to acquire up to 12 submarines to guard Arctic</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3LmV1cmFjdGl2LmNvbS9zZWN0aW9uL2RlZmVuY2UtYW5kLXNlY3VyaXR5L25ld3MvY2FuYWRhLXRha2VzLXN0ZXAtdG8tYWNxdWlyZS11cC10by0xMi1zdWJtYXJpbmVzLXRvLWd1YXJkLWFyY3RpYy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>Canada loses to U.S. in first Olympic tune-up game</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9vbHltcGljcy9hcnRpY2xlL2NhbmFkYS1sb3Nlcy10by11LXMtaW4tZmlyc3Qtb2x5bXBpYy10dW5lLXVwLWdhbWUv0gFbaHR0cHM6Ly93d3cuc3BvcnRzbmV0LmNhL29seW1waWNzL2NhbmFkYS1sb3Nlcy10by11LXMtaW4tZmlyc3Qtb2x5bXBpYy10dW5lLXVwLWdhbWUvc24tYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>Team USA shakes off slow start to beat Canada in pre-Olympics exhibition opener</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vc3BvcnRzLnlhaG9vLmNvbS90ZWFtLXVzYS1zaGFrZXMtb2ZmLXNsb3ctc3RhcnQtdG8tYmVhdC1jYW5hZGEtaW4tcHJlLW9seW1waWNzLWV4aGliaXRpb24tb3BlbmVyLTA0MzIxODQ3Ny5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>Steph Curry, LeBron James, Anthony Davis Impress Fans in Team USA Win vs. SGA, Canada</t>
+        </is>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>2024-07-11 00:19:55.966502</t>
+        </is>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifmh0dHBzOi8vYmxlYWNoZXJyZXBvcnQuY29tL2FydGljbGVzLzEwMTI3OTI4LXN0ZXBoLWN1cnJ5LWxlYnJvbi1qYW1lcy1hbnRob255LWRhdmlzLWltcHJlc3MtZmFucy1pbi10ZWFtLXVzYS13aW4tdnMtc2dhLWNhbmFkYdIBjgFodHRwczovL3N5bmRpY2F0aW9uLmJsZWFjaGVycmVwb3J0LmNvbS9hbXAvMTAxMjc5Mjgtc3RlcGgtY3VycnktbGVicm9uLWphbWVzLWFudGhvbnktZGF2aXMtaW1wcmVzcy1mYW5zLWluLXRlYW0tdXNhLXdpbi12cy1zZ2EtY2FuYWRhLmFtcC5odG1s?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>Canada soccer coach Jesse Marsch says he has no interest in vacant U.S. position</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>2024-07-11 01:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vY2Euc3BvcnRzLnlhaG9vLmNvbS9uZXdzL2NhbmFkYS1zb2NjZXItY29hY2gtamVzc2UtbWFyc2NoLTEzNTAxMDg2Ni5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>USA vs Canada score updates: Time, TV channel, streaming for USA Basketball Showcase</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>2024-07-11 01:19:55.928216</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihwFodHRwczovL3d3dy5va2xhaG9tYW4uY29tL3N0b3J5L3Nwb3J0cy9vbHltcGljcy8yMDI0LzA3LzEwL3VzLWNhbmFkYS1saXZlLXVwZGF0ZXMtc2NvcmUtaGlnaGxpZ2h0cy11c2EtYmFza2V0YmFsbC1zaG93Y2FzZS83NDM2MDY2NDAwNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>USA Open Showcase with 86-72 Win over Canada</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>2024-07-11 01:19:55.945371</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LnVzYWIuY29tL25ld3MvMjAyNC8wNy91c2Etb3Blbi1zaG93Y2FzZS13aXRoLTg2LTcyLXdpbi1vdmVyLWNhbmFkYdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>Team USA showcases defense, tops Canada in Olympic tuneup</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>2024-07-11 02:19:45.407336</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vYWJjbmV3cy5nby5jb20vU3BvcnRzL3RlYW0tdXNhLXNob3djYXNlcy1kZWZlbnNlLXRvcHMtY2FuYWRhLW9seW1waWMtdHVuZXVwL3N0b3J5P2lkPTExMTgzNjEzMdIBamh0dHBzOi8vYWJjbmV3cy5nby5jb20vYW1wL1Nwb3J0cy90ZWFtLXVzYS1zaG93Y2FzZXMtZGVmZW5zZS10b3BzLWNhbmFkYS1vbHltcGljLXR1bmV1cC9zdG9yeT9pZD0xMTE4MzYxMzE?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>CTV National News: Extreme weather in Canada</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>2024-07-11 02:19:45.422934</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vYmFycmllLmN0dm5ld3MuY2EvdmlkZW8vYzI5NTYzMzYtY3R2LW5hdGlvbmFsLW5ld3MtLWV4dHJlbWUtd2VhdGhlci1pbi1jYW5hZGE_YmluSWQ9MS4xMjcyNDI50gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>CTV National News: Canada's NATO commitments</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>2024-07-11 02:19:45.438555</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vYXRsYW50aWMuY3R2bmV3cy5jYS92aWRlby9jMjk1NjMzNS1jdHYtbmF0aW9uYWwtbmV3cy0tY2FuYWRhLXMtbmF0by1jb21taXRtZW50cz9wbGF5bGlzdElkPTEuNjgyOTUxONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>Oppressive heat poses health risk in Atlantic Canada, could topple records</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>2024-07-11 02:19:45.448172</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vb3BwcmVzc2l2ZS1oZWF0LXBvc2VzLWhlYWx0aC1yaXNrLTAwMzUyMTI4MC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>Canada trying to find rhythm after loss to U.S. in first Olympic tune-up</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>2024-07-11 02:19:55.911666</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9vbHltcGljcy9hcnRpY2xlL2NhbmFkYS10cnlpbmctdG8tZmluZC1yaHl0aG0tYWZ0ZXItbG9zcy10by11LXMtaW4tZmlyc3Qtb2x5bXBpYy10dW5lLXVwL9IBcWh0dHBzOi8vd3d3LnNwb3J0c25ldC5jYS9vbHltcGljcy9jYW5hZGEtdHJ5aW5nLXRvLWZpbmQtcmh5dGhtLWFmdGVyLWxvc3MtdG8tdS1zLWluLWZpcnN0LW9seW1waWMtdHVuZS11cC9zbi1hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>

</xml_diff>